<commit_message>
Changed FLC001->010 and added requirements for Drag due to Pitchrate and Leading Edge Flap Deflection.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF5B41-5C21-4980-870F-3B3EAA53BE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB713E4F-A64E-5E43-9D59-F3F36607233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="513">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -1562,12 +1562,6 @@
     <t>The program shall use the drag coefficient from angle of flight</t>
   </si>
   <si>
-    <t>SAYS-PRR-003</t>
-  </si>
-  <si>
-    <t>The program shall use a pre-determined table given in the XML File.</t>
-  </si>
-  <si>
     <t>The program shall place the tank(s) and their information in a tab labeled "Tanks".</t>
   </si>
   <si>
@@ -1578,13 +1572,34 @@
   </si>
   <si>
     <t>The program shall include a button labeled "Detail Tank" that will allow users to modify a listed tank.</t>
+  </si>
+  <si>
+    <t>SYS-PLE-001</t>
+  </si>
+  <si>
+    <t>The program shall calculate drag due to pitchrate and leading edge flap deflection.</t>
+  </si>
+  <si>
+    <t>SYS-PLE-002-001</t>
+  </si>
+  <si>
+    <t>SYS-PLE-002-002</t>
+  </si>
+  <si>
+    <t>The program shall calculate drag using wing area, air pressure, pitchrate, a conversion factor, leading edge flap position, and coefficient</t>
+  </si>
+  <si>
+    <t>The program will find the coefficient used to calculate drag as a look-ip table based on the angle of attack.</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1619,8 +1634,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1660,6 +1681,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1823,7 +1850,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1920,6 +1947,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
@@ -2295,22 +2323,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
-  <dimension ref="A2:F235"/>
+  <dimension ref="A2:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="79" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D218" sqref="D218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="180.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="180.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2327,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -2342,7 +2370,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -2357,7 +2385,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2400,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2387,7 +2415,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2402,7 +2430,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2417,7 +2445,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -2432,7 +2460,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2447,7 +2475,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -2462,7 +2490,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2477,7 +2505,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -2494,7 +2522,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2537,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -2524,7 +2552,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -2539,7 +2567,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -2554,7 +2582,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -2569,7 +2597,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -2584,7 +2612,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2599,7 +2627,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2614,7 +2642,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -2629,7 +2657,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2644,7 +2672,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -2654,14 +2682,14 @@
       <c r="D24" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="55" t="s">
-        <v>15</v>
+      <c r="E24" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -2671,14 +2699,14 @@
       <c r="D25" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="56" t="s">
-        <v>15</v>
+      <c r="E25" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2688,12 +2716,12 @@
       <c r="D26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="27" t="s">
-        <v>15</v>
+      <c r="E26" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2703,14 +2731,14 @@
       <c r="D27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="27" t="s">
-        <v>15</v>
+      <c r="E27" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -2720,12 +2748,12 @@
       <c r="D28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="27" t="s">
-        <v>15</v>
+      <c r="E28" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -2735,14 +2763,14 @@
       <c r="D29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="27" t="s">
-        <v>15</v>
+      <c r="E29" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -2752,12 +2780,12 @@
       <c r="D30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="28" t="s">
-        <v>15</v>
+      <c r="E30" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -2767,14 +2795,14 @@
       <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="27" t="s">
-        <v>15</v>
+      <c r="E31" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -2784,12 +2812,12 @@
       <c r="D32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="28" t="s">
-        <v>15</v>
+      <c r="E32" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -2799,14 +2827,14 @@
       <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="27" t="s">
-        <v>15</v>
+      <c r="E33" s="60" t="s">
+        <v>512</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -2821,7 +2849,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2841,7 +2869,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -2856,7 +2884,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -2873,7 +2901,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -2888,7 +2916,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -2905,7 +2933,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -2920,7 +2948,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -2937,7 +2965,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -2952,7 +2980,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -2969,7 +2997,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -2984,7 +3012,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3001,7 +3029,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3016,7 +3044,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3033,7 +3061,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3048,7 +3076,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3063,7 +3091,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3080,7 +3108,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3095,7 +3123,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3110,7 +3138,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3125,7 +3153,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3140,7 +3168,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3155,7 +3183,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3172,7 +3200,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3187,7 +3215,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3202,7 +3230,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3217,7 +3245,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -3232,7 +3260,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -3247,7 +3275,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -3264,7 +3292,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -3279,7 +3307,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -3294,7 +3322,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -3309,7 +3337,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -3324,7 +3352,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -3339,7 +3367,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -3356,7 +3384,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -3371,7 +3399,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -3386,7 +3414,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -3401,7 +3429,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -3416,7 +3444,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -3431,7 +3459,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -3448,7 +3476,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -3463,7 +3491,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -3478,7 +3506,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -3493,7 +3521,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -3508,7 +3536,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -3523,7 +3551,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -3540,7 +3568,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -3555,7 +3583,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -3570,7 +3598,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -3585,7 +3613,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -3600,7 +3628,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -3615,7 +3643,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -3632,7 +3660,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -3647,7 +3675,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -3662,7 +3690,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -3677,7 +3705,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -3692,7 +3720,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -3707,7 +3735,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -3724,7 +3752,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B93" s="3" t="s">
         <v>211</v>
       </c>
@@ -3739,7 +3767,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B94" s="3" t="s">
         <v>213</v>
       </c>
@@ -3754,7 +3782,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B95" s="3" t="s">
         <v>215</v>
       </c>
@@ -3769,7 +3797,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B96" s="3" t="s">
         <v>217</v>
       </c>
@@ -3784,7 +3812,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B97" s="3" t="s">
         <v>219</v>
       </c>
@@ -3799,7 +3827,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B98" s="3" t="s">
         <v>221</v>
       </c>
@@ -3814,7 +3842,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B99" s="3" t="s">
         <v>223</v>
       </c>
@@ -3829,7 +3857,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="3" t="s">
         <v>225</v>
       </c>
@@ -3844,7 +3872,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="3" t="s">
         <v>227</v>
       </c>
@@ -3859,7 +3887,7 @@
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B102" s="3" t="s">
         <v>229</v>
       </c>
@@ -3874,7 +3902,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -3889,7 +3917,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B104" s="20" t="s">
         <v>233</v>
       </c>
@@ -3904,7 +3932,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B105" s="20" t="s">
         <v>235</v>
       </c>
@@ -3919,7 +3947,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B106" s="20" t="s">
         <v>237</v>
       </c>
@@ -3934,7 +3962,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="20" t="s">
         <v>239</v>
       </c>
@@ -3949,7 +3977,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="20" t="s">
         <v>241</v>
       </c>
@@ -3964,7 +3992,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="20" t="s">
         <v>243</v>
       </c>
@@ -3979,7 +4007,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="20" t="s">
         <v>245</v>
       </c>
@@ -3994,7 +4022,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="20" t="s">
         <v>247</v>
       </c>
@@ -4009,7 +4037,7 @@
       </c>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="20" t="s">
         <v>247</v>
       </c>
@@ -4024,7 +4052,7 @@
       </c>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="7" t="s">
         <v>251</v>
       </c>
@@ -4042,7 +4070,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="7" t="s">
         <v>253</v>
       </c>
@@ -4060,7 +4088,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="7" t="s">
         <v>255</v>
       </c>
@@ -4078,7 +4106,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="7" t="s">
         <v>257</v>
       </c>
@@ -4096,7 +4124,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="7" t="s">
         <v>259</v>
       </c>
@@ -4113,7 +4141,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="7" t="s">
         <v>262</v>
       </c>
@@ -4130,7 +4158,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
         <v>265</v>
       </c>
@@ -4146,7 +4174,7 @@
       </c>
       <c r="F119" s="7"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B120" s="7" t="s">
         <v>266</v>
       </c>
@@ -4163,7 +4191,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="7" t="s">
         <v>269</v>
       </c>
@@ -4181,7 +4209,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B122" s="7" t="s">
         <v>271</v>
       </c>
@@ -4198,7 +4226,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="7" t="s">
         <v>274</v>
       </c>
@@ -4215,7 +4243,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="3" t="s">
         <v>277</v>
       </c>
@@ -4232,7 +4260,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="3" t="s">
         <v>280</v>
       </c>
@@ -4247,7 +4275,7 @@
       </c>
       <c r="F125" s="7"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
         <v>282</v>
       </c>
@@ -4262,7 +4290,7 @@
       </c>
       <c r="F126" s="7"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
         <v>284</v>
       </c>
@@ -4277,7 +4305,7 @@
       </c>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
         <v>286</v>
       </c>
@@ -4294,7 +4322,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
         <v>289</v>
       </c>
@@ -4311,7 +4339,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
         <v>292</v>
       </c>
@@ -4326,7 +4354,7 @@
       </c>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B131" s="3" t="s">
         <v>294</v>
       </c>
@@ -4343,7 +4371,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>296</v>
       </c>
@@ -4360,7 +4388,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
         <v>299</v>
       </c>
@@ -4377,7 +4405,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B134" s="3" t="s">
         <v>302</v>
       </c>
@@ -4392,7 +4420,7 @@
       </c>
       <c r="F134" s="7"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="3" t="s">
         <v>304</v>
       </c>
@@ -4407,7 +4435,7 @@
       </c>
       <c r="F135" s="7"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B136" s="3" t="s">
         <v>306</v>
       </c>
@@ -4422,7 +4450,7 @@
       </c>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B137" s="3" t="s">
         <v>308</v>
       </c>
@@ -4437,7 +4465,7 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B138" s="3" t="s">
         <v>310</v>
       </c>
@@ -4452,7 +4480,7 @@
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B139" s="3" t="s">
         <v>312</v>
       </c>
@@ -4467,7 +4495,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B140" s="3" t="s">
         <v>314</v>
       </c>
@@ -4482,7 +4510,7 @@
       </c>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B141" s="3" t="s">
         <v>316</v>
       </c>
@@ -4497,7 +4525,7 @@
       </c>
       <c r="F141" s="7"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="3" t="s">
         <v>318</v>
       </c>
@@ -4512,7 +4540,7 @@
       </c>
       <c r="F142" s="7"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B143" s="3" t="s">
         <v>320</v>
       </c>
@@ -4527,7 +4555,7 @@
       </c>
       <c r="F143" s="7"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" s="3" t="s">
         <v>322</v>
       </c>
@@ -4542,7 +4570,7 @@
       </c>
       <c r="F144" s="7"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="20" t="s">
         <v>324</v>
       </c>
@@ -4557,7 +4585,7 @@
       </c>
       <c r="F145" s="7"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B146" s="20" t="s">
         <v>326</v>
       </c>
@@ -4572,7 +4600,7 @@
       </c>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B147" s="20" t="s">
         <v>328</v>
       </c>
@@ -4587,7 +4615,7 @@
       </c>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B148" s="20" t="s">
         <v>330</v>
       </c>
@@ -4602,7 +4630,7 @@
       </c>
       <c r="F148" s="7"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B149" s="20" t="s">
         <v>332</v>
       </c>
@@ -4617,7 +4645,7 @@
       </c>
       <c r="F149" s="7"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B150" s="20" t="s">
         <v>334</v>
       </c>
@@ -4632,7 +4660,7 @@
       </c>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B151" s="20" t="s">
         <v>336</v>
       </c>
@@ -4647,7 +4675,7 @@
       </c>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B152" s="20" t="s">
         <v>338</v>
       </c>
@@ -4662,7 +4690,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B153" s="20" t="s">
         <v>340</v>
       </c>
@@ -4677,7 +4705,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B154" s="20" t="s">
         <v>342</v>
       </c>
@@ -4692,7 +4720,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B155" s="20" t="s">
         <v>344</v>
       </c>
@@ -4707,7 +4735,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B156" s="20" t="s">
         <v>346</v>
       </c>
@@ -4722,7 +4750,7 @@
       </c>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B157" s="9" t="s">
         <v>348</v>
       </c>
@@ -4740,7 +4768,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B158" s="9" t="s">
         <v>350</v>
       </c>
@@ -4756,7 +4784,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B159" s="9" t="s">
         <v>351</v>
       </c>
@@ -4774,7 +4802,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B160" s="9" t="s">
         <v>353</v>
       </c>
@@ -4790,7 +4818,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B161" s="9" t="s">
         <v>354</v>
       </c>
@@ -4808,7 +4836,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B162" s="9" t="s">
         <v>356</v>
       </c>
@@ -4826,7 +4854,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B163" s="9" t="s">
         <v>358</v>
       </c>
@@ -4841,7 +4869,7 @@
       </c>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B164" s="9" t="s">
         <v>360</v>
       </c>
@@ -4859,7 +4887,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B165" s="9" t="s">
         <v>362</v>
       </c>
@@ -4877,7 +4905,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B166" s="9" t="s">
         <v>364</v>
       </c>
@@ -4895,7 +4923,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B167" s="9" t="s">
         <v>366</v>
       </c>
@@ -4913,7 +4941,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B168" s="9" t="s">
         <v>368</v>
       </c>
@@ -4928,7 +4956,7 @@
       </c>
       <c r="F168" s="7"/>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B169" s="10" t="s">
         <v>370</v>
       </c>
@@ -4936,7 +4964,7 @@
         <v>6</v>
       </c>
       <c r="D169" s="59" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E169" s="28" t="s">
         <v>15</v>
@@ -4945,7 +4973,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B170" s="10" t="s">
         <v>372</v>
       </c>
@@ -4953,7 +4981,7 @@
         <v>6</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E170" s="28" t="s">
         <v>15</v>
@@ -4962,7 +4990,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B171" s="10" t="s">
         <v>374</v>
       </c>
@@ -4970,7 +4998,7 @@
         <v>6</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E171" s="28" t="s">
         <v>15</v>
@@ -4979,7 +5007,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B172" s="10" t="s">
         <v>376</v>
       </c>
@@ -4987,7 +5015,7 @@
         <v>6</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E172" s="28" t="s">
         <v>15</v>
@@ -4996,7 +5024,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B173" s="21" t="s">
         <v>378</v>
       </c>
@@ -5011,7 +5039,7 @@
       </c>
       <c r="F173" s="7"/>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B174" s="21" t="s">
         <v>380</v>
       </c>
@@ -5026,7 +5054,7 @@
       </c>
       <c r="F174" s="7"/>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B175" s="21" t="s">
         <v>382</v>
       </c>
@@ -5041,7 +5069,7 @@
       </c>
       <c r="F175" s="7"/>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B176" s="21" t="s">
         <v>384</v>
       </c>
@@ -5056,7 +5084,7 @@
       </c>
       <c r="F176" s="7"/>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B177" s="21" t="s">
         <v>386</v>
       </c>
@@ -5071,7 +5099,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B178" s="21" t="s">
         <v>388</v>
       </c>
@@ -5086,7 +5114,7 @@
       </c>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B179" s="3" t="s">
         <v>390</v>
       </c>
@@ -5101,7 +5129,7 @@
       </c>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B180" s="3" t="s">
         <v>392</v>
       </c>
@@ -5116,7 +5144,7 @@
       </c>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B181" s="3" t="s">
         <v>394</v>
       </c>
@@ -5131,7 +5159,7 @@
       </c>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B182" s="3" t="s">
         <v>396</v>
       </c>
@@ -5146,7 +5174,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B183" s="21" t="s">
         <v>398</v>
       </c>
@@ -5161,7 +5189,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B184" s="3" t="s">
         <v>400</v>
       </c>
@@ -5176,7 +5204,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B185" s="3" t="s">
         <v>402</v>
       </c>
@@ -5191,7 +5219,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B186" s="21" t="s">
         <v>404</v>
       </c>
@@ -5206,7 +5234,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B187" s="3" t="s">
         <v>406</v>
       </c>
@@ -5221,7 +5249,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B188" s="3" t="s">
         <v>408</v>
       </c>
@@ -5238,7 +5266,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B189" s="3" t="s">
         <v>410</v>
       </c>
@@ -5253,7 +5281,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B190" s="3" t="s">
         <v>412</v>
       </c>
@@ -5268,7 +5296,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B191" s="3" t="s">
         <v>414</v>
       </c>
@@ -5283,7 +5311,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B192" s="3" t="s">
         <v>416</v>
       </c>
@@ -5298,7 +5326,7 @@
       </c>
       <c r="F192" s="7"/>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B193" s="3" t="s">
         <v>418</v>
       </c>
@@ -5313,7 +5341,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B194" s="3" t="s">
         <v>420</v>
       </c>
@@ -5328,7 +5356,7 @@
       </c>
       <c r="F194" s="7"/>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B195" s="3" t="s">
         <v>422</v>
       </c>
@@ -5343,7 +5371,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B196" s="3" t="s">
         <v>424</v>
       </c>
@@ -5358,7 +5386,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B197" s="3" t="s">
         <v>426</v>
       </c>
@@ -5373,7 +5401,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B198" s="3" t="s">
         <v>428</v>
       </c>
@@ -5388,7 +5416,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B199" s="3" t="s">
         <v>430</v>
       </c>
@@ -5403,7 +5431,7 @@
       </c>
       <c r="F199" s="7"/>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B200" s="3" t="s">
         <v>432</v>
       </c>
@@ -5418,7 +5446,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B201" s="3" t="s">
         <v>434</v>
       </c>
@@ -5433,7 +5461,7 @@
       </c>
       <c r="F201" s="7"/>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B202" s="21" t="s">
         <v>436</v>
       </c>
@@ -5448,7 +5476,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B203" s="21" t="s">
         <v>438</v>
       </c>
@@ -5463,7 +5491,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B204" s="21" t="s">
         <v>440</v>
       </c>
@@ -5478,7 +5506,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B205" s="12" t="s">
         <v>442</v>
       </c>
@@ -5493,7 +5521,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B206" s="12" t="s">
         <v>444</v>
       </c>
@@ -5508,7 +5536,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B207" s="12" t="s">
         <v>446</v>
       </c>
@@ -5523,7 +5551,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B208" s="12" t="s">
         <v>448</v>
       </c>
@@ -5538,7 +5566,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B209" s="21" t="s">
         <v>450</v>
       </c>
@@ -5553,7 +5581,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B210" s="21" t="s">
         <v>452</v>
       </c>
@@ -5568,7 +5596,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B211" s="21" t="s">
         <v>454</v>
       </c>
@@ -5583,7 +5611,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B212" s="21" t="s">
         <v>456</v>
       </c>
@@ -5598,7 +5626,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B213" s="21" t="s">
         <v>458</v>
       </c>
@@ -5613,7 +5641,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B214" s="21" t="s">
         <v>460</v>
       </c>
@@ -5628,7 +5656,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B215" s="21" t="s">
         <v>462</v>
       </c>
@@ -5643,7 +5671,7 @@
       </c>
       <c r="F215" s="7"/>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B216" s="21" t="s">
         <v>464</v>
       </c>
@@ -5658,7 +5686,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B217" s="21" t="s">
         <v>466</v>
       </c>
@@ -5673,7 +5701,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B218" s="12" t="s">
         <v>468</v>
       </c>
@@ -5688,7 +5716,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B219" s="12" t="s">
         <v>470</v>
       </c>
@@ -5703,7 +5731,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B220" s="12" t="s">
         <v>472</v>
       </c>
@@ -5718,7 +5746,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B221" s="12" t="s">
         <v>474</v>
       </c>
@@ -5733,7 +5761,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B222" s="12" t="s">
         <v>476</v>
       </c>
@@ -5748,7 +5776,7 @@
       </c>
       <c r="F222" s="7"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B223" s="12" t="s">
         <v>478</v>
       </c>
@@ -5763,7 +5791,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B224" s="12" t="s">
         <v>480</v>
       </c>
@@ -5778,7 +5806,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B225" s="12" t="s">
         <v>482</v>
       </c>
@@ -5793,7 +5821,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B226" s="12" t="s">
         <v>484</v>
       </c>
@@ -5808,7 +5836,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B227" s="12" t="s">
         <v>486</v>
       </c>
@@ -5823,7 +5851,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B228" s="12" t="s">
         <v>488</v>
       </c>
@@ -5838,7 +5866,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B229" s="12" t="s">
         <v>490</v>
       </c>
@@ -5853,7 +5881,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B230" s="12" t="s">
         <v>492</v>
       </c>
@@ -5868,7 +5896,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B231" s="12" t="s">
         <v>494</v>
       </c>
@@ -5883,7 +5911,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B232" s="12" t="s">
         <v>496</v>
       </c>
@@ -5898,7 +5926,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B233" s="12" t="s">
         <v>498</v>
       </c>
@@ -5913,7 +5941,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B234" s="12" t="s">
         <v>500</v>
       </c>
@@ -5928,20 +5956,57 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="12" t="s">
-        <v>502</v>
-      </c>
-      <c r="C235" s="58" t="s">
-        <v>23</v>
+        <v>506</v>
+      </c>
+      <c r="C235" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D235" s="12" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="E235" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F235" s="7"/>
+    </row>
+    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B236" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="C236" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D236" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="E236" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F236" s="7"/>
+    </row>
+    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B237" s="12" t="s">
+        <v>509</v>
+      </c>
+      <c r="C237" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D237" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="E237" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F237" s="7"/>
+    </row>
+    <row r="238" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B238" s="12"/>
+      <c r="C238" s="58"/>
+      <c r="D238" s="12"/>
+      <c r="E238" s="37"/>
+      <c r="F238" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F217">
@@ -5950,18 +6015,18 @@
     <sortCondition descending="1" sortBy="cellColor" ref="C3:C217" dxfId="1"/>
     <sortCondition descending="1" sortBy="cellColor" ref="C3:C217" dxfId="0"/>
   </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6186,17 +6251,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6221,11 +6289,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix Missing References in Requirements
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/jsbsimedit2/requirements_specification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB713E4F-A64E-5E43-9D59-F3F36607233A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF230C0-E6DF-4943-9A32-F4DE0F4C174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="529">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -1593,13 +1593,61 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for the mass of the aircraft.</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for the units of mass variable.</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for the location of the center of mass of the aircraft.</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for the units of location variable.</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for the pointmass variables related to the aircraft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The program shall include a button element to add an additional point mass. </t>
+  </si>
+  <si>
+    <t>The program shall contain all PRO variables, buttons, and text in a tab labeled "Propulsion".</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for all engines and the "engine file" name for each.</t>
+  </si>
+  <si>
+    <t>The program shall list all engines in a tab labeled "Available Engines".</t>
+  </si>
+  <si>
+    <t>The program shall recieve xml input for all thrusters and the "thruster file" name for each.</t>
+  </si>
+  <si>
+    <t>The program shall list all thrusters in a tab labeled "Available Thrusters".</t>
+  </si>
+  <si>
+    <t>The program shall include a scroll bar to see all elements in the "Available Engines" tab.</t>
+  </si>
+  <si>
+    <t>The program shall place the engine(s) and their thruster(s) in a tab labeled "Subscribed Engine(s)(*)".</t>
+  </si>
+  <si>
+    <t>The program shall include a button labeled "New Pair" that will allow users to pair and engine with a thruster.</t>
+  </si>
+  <si>
+    <t>The program shall include a button labeled "Delete Pair" that will allow users to delete a listed pair.</t>
+  </si>
+  <si>
+    <t>The program shall include a button labeled "Detail Pair" that will allow users to modify a listed pair</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1640,8 +1688,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1690,8 +1744,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAF2D0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1844,13 +1904,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF156082"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1948,6 +2034,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
@@ -2325,20 +2427,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="79" workbookViewId="0">
-      <selection activeCell="D218" sqref="D218"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="180.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="180.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2355,7 +2457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -2370,7 +2472,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -2385,7 +2487,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -2400,7 +2502,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2415,7 +2517,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2430,7 +2532,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2445,7 +2547,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -2460,7 +2562,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2475,7 +2577,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -2490,7 +2592,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -2505,7 +2607,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -2522,7 +2624,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -2537,7 +2639,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2654,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -2567,7 +2669,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -2582,7 +2684,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -2597,7 +2699,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -2612,7 +2714,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2627,7 +2729,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -2642,7 +2744,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -2657,7 +2759,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2672,7 +2774,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -2689,7 +2791,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -2706,7 +2808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -2721,7 +2823,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -2738,7 +2840,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -2753,7 +2855,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -2770,7 +2872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -2785,7 +2887,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -2802,7 +2904,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -2817,7 +2919,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -2834,7 +2936,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -2849,7 +2951,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2869,7 +2971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -2884,7 +2986,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -2901,7 +3003,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -2916,7 +3018,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -2933,7 +3035,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -2948,7 +3050,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -2965,7 +3067,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -2980,7 +3082,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -2997,7 +3099,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -3012,7 +3114,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3029,7 +3131,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3044,7 +3146,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3061,7 +3163,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3076,7 +3178,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3091,7 +3193,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3108,7 +3210,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3123,7 +3225,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3138,7 +3240,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3153,7 +3255,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3168,7 +3270,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3183,7 +3285,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3200,7 +3302,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3215,7 +3317,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3230,7 +3332,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3245,7 +3347,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -3260,7 +3362,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -3275,7 +3377,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -3292,7 +3394,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -3307,7 +3409,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -3322,7 +3424,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -3337,7 +3439,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -3352,7 +3454,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -3367,7 +3469,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -3384,7 +3486,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -3399,7 +3501,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -3414,7 +3516,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -3429,7 +3531,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -3444,7 +3546,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -3459,7 +3561,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -3476,7 +3578,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -3491,7 +3593,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -3506,7 +3608,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -3521,7 +3623,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -3536,7 +3638,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -3551,7 +3653,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -3568,7 +3670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -3583,7 +3685,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -3598,7 +3700,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -3613,7 +3715,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -3628,7 +3730,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -3643,7 +3745,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -3660,7 +3762,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -3675,7 +3777,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -3690,7 +3792,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -3705,7 +3807,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -3720,7 +3822,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -3735,7 +3837,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -3752,7 +3854,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
         <v>211</v>
       </c>
@@ -3767,7 +3869,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
         <v>213</v>
       </c>
@@ -3782,7 +3884,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
         <v>215</v>
       </c>
@@ -3797,7 +3899,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
         <v>217</v>
       </c>
@@ -3812,7 +3914,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
         <v>219</v>
       </c>
@@ -3827,7 +3929,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
         <v>221</v>
       </c>
@@ -3842,7 +3944,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
         <v>223</v>
       </c>
@@ -3857,7 +3959,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
         <v>225</v>
       </c>
@@ -3872,7 +3974,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
         <v>227</v>
       </c>
@@ -3887,7 +3989,7 @@
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
         <v>229</v>
       </c>
@@ -3902,7 +4004,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -3917,7 +4019,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="20" t="s">
         <v>233</v>
       </c>
@@ -3932,7 +4034,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="20" t="s">
         <v>235</v>
       </c>
@@ -3947,7 +4049,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="20" t="s">
         <v>237</v>
       </c>
@@ -3962,7 +4064,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="20" t="s">
         <v>239</v>
       </c>
@@ -3977,7 +4079,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="20" t="s">
         <v>241</v>
       </c>
@@ -3992,7 +4094,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="20" t="s">
         <v>243</v>
       </c>
@@ -4007,7 +4109,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="20" t="s">
         <v>245</v>
       </c>
@@ -4022,7 +4124,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="20" t="s">
         <v>247</v>
       </c>
@@ -4037,7 +4139,7 @@
       </c>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="20" t="s">
         <v>247</v>
       </c>
@@ -4052,16 +4154,15 @@
       </c>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D113" s="62" t="s">
+        <v>513</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>15</v>
@@ -4070,16 +4171,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="7" t="s">
         <v>253</v>
       </c>
       <c r="C114" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D114" s="63" t="s">
+        <v>514</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>15</v>
@@ -4088,16 +4188,15 @@
         <v>254</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="7" t="s">
         <v>255</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D115" s="63" t="s">
+        <v>515</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>15</v>
@@ -4106,16 +4205,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="7" t="s">
         <v>257</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D116" s="63" t="s">
+        <v>516</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>15</v>
@@ -4124,7 +4222,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="7" t="s">
         <v>259</v>
       </c>
@@ -4141,7 +4239,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B118" s="7" t="s">
         <v>262</v>
       </c>
@@ -4158,23 +4256,22 @@
         <v>264</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="7" t="s">
         <v>265</v>
       </c>
       <c r="C119" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D119" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D119" s="63" t="s">
+        <v>517</v>
       </c>
       <c r="E119" s="26" t="s">
         <v>15</v>
       </c>
       <c r="F119" s="7"/>
     </row>
-    <row r="120" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B120" s="7" t="s">
         <v>266</v>
       </c>
@@ -4191,16 +4288,15 @@
         <v>268</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B121" s="7" t="s">
         <v>269</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D121" s="8" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D121" s="63" t="s">
+        <v>518</v>
       </c>
       <c r="E121" s="26" t="s">
         <v>15</v>
@@ -4209,7 +4305,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="7" t="s">
         <v>271</v>
       </c>
@@ -4226,7 +4322,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B123" s="7" t="s">
         <v>274</v>
       </c>
@@ -4243,14 +4339,14 @@
         <v>276</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
         <v>277</v>
       </c>
       <c r="C124" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="61" t="s">
         <v>278</v>
       </c>
       <c r="E124" s="28" t="s">
@@ -4260,7 +4356,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
         <v>280</v>
       </c>
@@ -4275,7 +4371,7 @@
       </c>
       <c r="F125" s="7"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
         <v>282</v>
       </c>
@@ -4290,7 +4386,7 @@
       </c>
       <c r="F126" s="7"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
         <v>284</v>
       </c>
@@ -4305,7 +4401,7 @@
       </c>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
         <v>286</v>
       </c>
@@ -4322,7 +4418,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
         <v>289</v>
       </c>
@@ -4339,7 +4435,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
         <v>292</v>
       </c>
@@ -4354,7 +4450,7 @@
       </c>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
         <v>294</v>
       </c>
@@ -4371,7 +4467,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
         <v>296</v>
       </c>
@@ -4388,7 +4484,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
         <v>299</v>
       </c>
@@ -4405,7 +4501,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
         <v>302</v>
       </c>
@@ -4420,7 +4516,7 @@
       </c>
       <c r="F134" s="7"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
         <v>304</v>
       </c>
@@ -4435,7 +4531,7 @@
       </c>
       <c r="F135" s="7"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
         <v>306</v>
       </c>
@@ -4450,7 +4546,7 @@
       </c>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
         <v>308</v>
       </c>
@@ -4465,7 +4561,7 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
         <v>310</v>
       </c>
@@ -4480,7 +4576,7 @@
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
         <v>312</v>
       </c>
@@ -4495,7 +4591,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
         <v>314</v>
       </c>
@@ -4510,7 +4606,7 @@
       </c>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
         <v>316</v>
       </c>
@@ -4525,7 +4621,7 @@
       </c>
       <c r="F141" s="7"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
         <v>318</v>
       </c>
@@ -4540,7 +4636,7 @@
       </c>
       <c r="F142" s="7"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
         <v>320</v>
       </c>
@@ -4555,7 +4651,7 @@
       </c>
       <c r="F143" s="7"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
         <v>322</v>
       </c>
@@ -4570,7 +4666,7 @@
       </c>
       <c r="F144" s="7"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B145" s="20" t="s">
         <v>324</v>
       </c>
@@ -4585,7 +4681,7 @@
       </c>
       <c r="F145" s="7"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B146" s="20" t="s">
         <v>326</v>
       </c>
@@ -4600,7 +4696,7 @@
       </c>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B147" s="20" t="s">
         <v>328</v>
       </c>
@@ -4615,7 +4711,7 @@
       </c>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B148" s="20" t="s">
         <v>330</v>
       </c>
@@ -4630,7 +4726,7 @@
       </c>
       <c r="F148" s="7"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B149" s="20" t="s">
         <v>332</v>
       </c>
@@ -4645,7 +4741,7 @@
       </c>
       <c r="F149" s="7"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B150" s="20" t="s">
         <v>334</v>
       </c>
@@ -4660,7 +4756,7 @@
       </c>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B151" s="20" t="s">
         <v>336</v>
       </c>
@@ -4675,7 +4771,7 @@
       </c>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B152" s="20" t="s">
         <v>338</v>
       </c>
@@ -4690,7 +4786,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B153" s="20" t="s">
         <v>340</v>
       </c>
@@ -4705,7 +4801,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B154" s="20" t="s">
         <v>342</v>
       </c>
@@ -4720,7 +4816,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B155" s="20" t="s">
         <v>344</v>
       </c>
@@ -4735,7 +4831,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="20" t="s">
         <v>346</v>
       </c>
@@ -4750,16 +4846,15 @@
       </c>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="9" t="s">
         <v>348</v>
       </c>
       <c r="C157" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D157" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D157" s="64" t="s">
+        <v>519</v>
       </c>
       <c r="E157" s="54" t="s">
         <v>15</v>
@@ -4768,32 +4863,30 @@
         <v>349</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="9" t="s">
         <v>350</v>
       </c>
       <c r="C158" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D158" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D158" s="65" t="s">
+        <v>520</v>
       </c>
       <c r="E158" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B159" s="9" t="s">
         <v>351</v>
       </c>
       <c r="C159" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D159" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D159" s="66" t="s">
+        <v>521</v>
       </c>
       <c r="E159" s="54" t="s">
         <v>15</v>
@@ -4802,32 +4895,30 @@
         <v>352</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="9" t="s">
         <v>353</v>
       </c>
       <c r="C160" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D160" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D160" s="65" t="s">
+        <v>522</v>
       </c>
       <c r="E160" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="9" t="s">
         <v>354</v>
       </c>
       <c r="C161" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D161" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D161" s="66" t="s">
+        <v>523</v>
       </c>
       <c r="E161" s="54" t="s">
         <v>15</v>
@@ -4836,16 +4927,15 @@
         <v>355</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="9" t="s">
         <v>356</v>
       </c>
       <c r="C162" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D162" s="9" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D162" s="66" t="s">
+        <v>524</v>
       </c>
       <c r="E162" s="54" t="s">
         <v>15</v>
@@ -4854,7 +4944,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="163" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="9" t="s">
         <v>358</v>
       </c>
@@ -4869,16 +4959,15 @@
       </c>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="9" t="s">
         <v>360</v>
       </c>
       <c r="C164" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D164" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D164" s="66" t="s">
+        <v>525</v>
       </c>
       <c r="E164" s="54" t="s">
         <v>15</v>
@@ -4887,16 +4976,15 @@
         <v>361</v>
       </c>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="9" t="s">
         <v>362</v>
       </c>
       <c r="C165" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D165" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D165" s="66" t="s">
+        <v>526</v>
       </c>
       <c r="E165" s="54" t="s">
         <v>15</v>
@@ -4905,16 +4993,15 @@
         <v>363</v>
       </c>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="9" t="s">
         <v>364</v>
       </c>
       <c r="C166" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D166" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D166" s="66" t="s">
+        <v>527</v>
       </c>
       <c r="E166" s="54" t="s">
         <v>15</v>
@@ -4923,16 +5010,15 @@
         <v>365</v>
       </c>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="9" t="s">
         <v>366</v>
       </c>
       <c r="C167" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D167" s="6" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D167" s="66" t="s">
+        <v>528</v>
       </c>
       <c r="E167" s="54" t="s">
         <v>15</v>
@@ -4941,7 +5027,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="168" spans="2:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="9" t="s">
         <v>368</v>
       </c>
@@ -4956,7 +5042,7 @@
       </c>
       <c r="F168" s="7"/>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B169" s="10" t="s">
         <v>370</v>
       </c>
@@ -4973,7 +5059,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B170" s="10" t="s">
         <v>372</v>
       </c>
@@ -4990,7 +5076,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B171" s="10" t="s">
         <v>374</v>
       </c>
@@ -5007,7 +5093,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B172" s="10" t="s">
         <v>376</v>
       </c>
@@ -5024,7 +5110,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B173" s="21" t="s">
         <v>378</v>
       </c>
@@ -5039,7 +5125,7 @@
       </c>
       <c r="F173" s="7"/>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B174" s="21" t="s">
         <v>380</v>
       </c>
@@ -5054,7 +5140,7 @@
       </c>
       <c r="F174" s="7"/>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B175" s="21" t="s">
         <v>382</v>
       </c>
@@ -5069,7 +5155,7 @@
       </c>
       <c r="F175" s="7"/>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B176" s="21" t="s">
         <v>384</v>
       </c>
@@ -5084,7 +5170,7 @@
       </c>
       <c r="F176" s="7"/>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B177" s="21" t="s">
         <v>386</v>
       </c>
@@ -5099,7 +5185,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B178" s="21" t="s">
         <v>388</v>
       </c>
@@ -5114,7 +5200,7 @@
       </c>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B179" s="3" t="s">
         <v>390</v>
       </c>
@@ -5129,7 +5215,7 @@
       </c>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B180" s="3" t="s">
         <v>392</v>
       </c>
@@ -5144,7 +5230,7 @@
       </c>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B181" s="3" t="s">
         <v>394</v>
       </c>
@@ -5159,7 +5245,7 @@
       </c>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B182" s="3" t="s">
         <v>396</v>
       </c>
@@ -5174,7 +5260,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B183" s="21" t="s">
         <v>398</v>
       </c>
@@ -5189,7 +5275,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B184" s="3" t="s">
         <v>400</v>
       </c>
@@ -5204,7 +5290,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B185" s="3" t="s">
         <v>402</v>
       </c>
@@ -5219,7 +5305,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B186" s="21" t="s">
         <v>404</v>
       </c>
@@ -5234,7 +5320,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B187" s="3" t="s">
         <v>406</v>
       </c>
@@ -5249,7 +5335,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B188" s="3" t="s">
         <v>408</v>
       </c>
@@ -5266,7 +5352,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B189" s="3" t="s">
         <v>410</v>
       </c>
@@ -5281,7 +5367,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B190" s="3" t="s">
         <v>412</v>
       </c>
@@ -5296,7 +5382,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B191" s="3" t="s">
         <v>414</v>
       </c>
@@ -5311,7 +5397,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B192" s="3" t="s">
         <v>416</v>
       </c>
@@ -5326,7 +5412,7 @@
       </c>
       <c r="F192" s="7"/>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B193" s="3" t="s">
         <v>418</v>
       </c>
@@ -5341,7 +5427,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B194" s="3" t="s">
         <v>420</v>
       </c>
@@ -5356,7 +5442,7 @@
       </c>
       <c r="F194" s="7"/>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B195" s="3" t="s">
         <v>422</v>
       </c>
@@ -5371,7 +5457,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B196" s="3" t="s">
         <v>424</v>
       </c>
@@ -5386,7 +5472,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B197" s="3" t="s">
         <v>426</v>
       </c>
@@ -5401,7 +5487,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B198" s="3" t="s">
         <v>428</v>
       </c>
@@ -5416,7 +5502,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B199" s="3" t="s">
         <v>430</v>
       </c>
@@ -5431,7 +5517,7 @@
       </c>
       <c r="F199" s="7"/>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B200" s="3" t="s">
         <v>432</v>
       </c>
@@ -5446,7 +5532,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B201" s="3" t="s">
         <v>434</v>
       </c>
@@ -5461,7 +5547,7 @@
       </c>
       <c r="F201" s="7"/>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B202" s="21" t="s">
         <v>436</v>
       </c>
@@ -5476,7 +5562,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B203" s="21" t="s">
         <v>438</v>
       </c>
@@ -5491,7 +5577,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B204" s="21" t="s">
         <v>440</v>
       </c>
@@ -5506,7 +5592,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B205" s="12" t="s">
         <v>442</v>
       </c>
@@ -5521,7 +5607,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B206" s="12" t="s">
         <v>444</v>
       </c>
@@ -5536,7 +5622,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B207" s="12" t="s">
         <v>446</v>
       </c>
@@ -5551,7 +5637,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B208" s="12" t="s">
         <v>448</v>
       </c>
@@ -5566,7 +5652,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B209" s="21" t="s">
         <v>450</v>
       </c>
@@ -5581,7 +5667,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B210" s="21" t="s">
         <v>452</v>
       </c>
@@ -5596,7 +5682,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B211" s="21" t="s">
         <v>454</v>
       </c>
@@ -5611,7 +5697,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B212" s="21" t="s">
         <v>456</v>
       </c>
@@ -5626,7 +5712,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B213" s="21" t="s">
         <v>458</v>
       </c>
@@ -5641,7 +5727,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B214" s="21" t="s">
         <v>460</v>
       </c>
@@ -5656,7 +5742,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B215" s="21" t="s">
         <v>462</v>
       </c>
@@ -5671,7 +5757,7 @@
       </c>
       <c r="F215" s="7"/>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B216" s="21" t="s">
         <v>464</v>
       </c>
@@ -5686,7 +5772,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B217" s="21" t="s">
         <v>466</v>
       </c>
@@ -5701,7 +5787,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B218" s="12" t="s">
         <v>468</v>
       </c>
@@ -5716,7 +5802,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B219" s="12" t="s">
         <v>470</v>
       </c>
@@ -5731,7 +5817,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B220" s="12" t="s">
         <v>472</v>
       </c>
@@ -5746,7 +5832,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B221" s="12" t="s">
         <v>474</v>
       </c>
@@ -5761,7 +5847,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="12" t="s">
         <v>476</v>
       </c>
@@ -5776,7 +5862,7 @@
       </c>
       <c r="F222" s="7"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B223" s="12" t="s">
         <v>478</v>
       </c>
@@ -5791,7 +5877,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="12" t="s">
         <v>480</v>
       </c>
@@ -5806,7 +5892,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B225" s="12" t="s">
         <v>482</v>
       </c>
@@ -5821,7 +5907,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B226" s="12" t="s">
         <v>484</v>
       </c>
@@ -5836,7 +5922,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B227" s="12" t="s">
         <v>486</v>
       </c>
@@ -5851,7 +5937,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B228" s="12" t="s">
         <v>488</v>
       </c>
@@ -5866,7 +5952,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B229" s="12" t="s">
         <v>490</v>
       </c>
@@ -5881,7 +5967,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B230" s="12" t="s">
         <v>492</v>
       </c>
@@ -5896,7 +5982,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B231" s="12" t="s">
         <v>494</v>
       </c>
@@ -5911,7 +5997,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B232" s="12" t="s">
         <v>496</v>
       </c>
@@ -5926,7 +6012,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B233" s="12" t="s">
         <v>498</v>
       </c>
@@ -5941,7 +6027,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B234" s="12" t="s">
         <v>500</v>
       </c>
@@ -5956,7 +6042,7 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B235" s="12" t="s">
         <v>506</v>
       </c>
@@ -5971,7 +6057,7 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B236" s="12" t="s">
         <v>508</v>
       </c>
@@ -5986,7 +6072,7 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B237" s="12" t="s">
         <v>509</v>
       </c>
@@ -6001,7 +6087,7 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B238" s="12"/>
       <c r="C238" s="58"/>
       <c r="D238" s="12"/>
@@ -6022,14 +6108,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -6250,6 +6328,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6260,16 +6346,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6288,6 +6364,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix and Add to Menu Requirements
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF230C0-E6DF-4943-9A32-F4DE0F4C174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0F1076-1C17-49DD-98A9-C7EDDD57C60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>tc={047D126E-D947-419E-ABB9-ADAD162C5DD2}</author>
   </authors>
   <commentList>
-    <comment ref="D189" authorId="0" shapeId="0" xr:uid="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
+    <comment ref="D193" authorId="0" shapeId="0" xr:uid="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="538">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -890,12 +890,6 @@
     <t>SYS-MEN-001</t>
   </si>
   <si>
-    <t>The program shall display a window called "JSBSim Commander" containing the options to open the xml editor or to exit.</t>
-  </si>
-  <si>
-    <t>UIID-004/006</t>
-  </si>
-  <si>
     <t>SYS-MEN-002</t>
   </si>
   <si>
@@ -917,9 +911,6 @@
     <t>SYS-MEN-005</t>
   </si>
   <si>
-    <t>If the user clicks on the open button, the program shall open a new window called "Aircraft Commander".</t>
-  </si>
-  <si>
     <t>UIID-016</t>
   </si>
   <si>
@@ -1641,6 +1632,42 @@
   </si>
   <si>
     <t>The program shall include a button labeled "Detail Pair" that will allow users to modify a listed pair</t>
+  </si>
+  <si>
+    <t>If the user clicks on the open button, the program shall load the xml data into the appropriate tabs as dictated by the schema.</t>
+  </si>
+  <si>
+    <t>The program shall display a window called "Aircraft Commander" containing file I/O options, an exit option, and several tabs.</t>
+  </si>
+  <si>
+    <t>SYS-MEN-011</t>
+  </si>
+  <si>
+    <t>Upon loading a file, the program shall display feedback if the load was successful.</t>
+  </si>
+  <si>
+    <t>SYS-MEN-012</t>
+  </si>
+  <si>
+    <t>Upon loading a file, the program shall display an error message if the load was unsuccessful.</t>
+  </si>
+  <si>
+    <t>SYS-MEN-013</t>
+  </si>
+  <si>
+    <t>SYS-MEN-014</t>
+  </si>
+  <si>
+    <t>Upon saving a file, the program shall display feedback if the save was successful.</t>
+  </si>
+  <si>
+    <t>Upon saving a file, the program shall display an error message if the save was unsuccessful.</t>
+  </si>
+  <si>
+    <t>UIID-008/016</t>
+  </si>
+  <si>
+    <t>UIID-008</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1963,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2050,13 +2077,65 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2417,7 +2496,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D189" dT="2025-10-22T19:44:42.55" personId="{0B44E5FE-6282-4086-A5CD-8A4B3BD81016}" id="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
+  <threadedComment ref="D193" dT="2025-10-22T19:44:42.55" personId="{0B44E5FE-6282-4086-A5CD-8A4B3BD81016}" id="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
     <text>Link to UI Elements(also in github)- https://mavsuta-my.sharepoint.com/:x:/g/personal/eeh6400_mavs_uta_edu/EdM1amBmGwpIlWEx4x01hZsB9_bqH9pYalj-9kd7PPfp2A</text>
   </threadedComment>
 </ThreadedComments>
@@ -2425,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
-  <dimension ref="A2:F238"/>
+  <dimension ref="A2:F242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="79" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2785,7 +2864,7 @@
         <v>53</v>
       </c>
       <c r="E24" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>54</v>
@@ -2802,7 +2881,7 @@
         <v>56</v>
       </c>
       <c r="E25" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>57</v>
@@ -2819,7 +2898,7 @@
         <v>59</v>
       </c>
       <c r="E26" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F26" s="7"/>
     </row>
@@ -2834,7 +2913,7 @@
         <v>61</v>
       </c>
       <c r="E27" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>62</v>
@@ -2851,7 +2930,7 @@
         <v>64</v>
       </c>
       <c r="E28" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F28" s="7"/>
     </row>
@@ -2866,7 +2945,7 @@
         <v>66</v>
       </c>
       <c r="E29" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>67</v>
@@ -2883,7 +2962,7 @@
         <v>69</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F30" s="7"/>
     </row>
@@ -2898,7 +2977,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>72</v>
@@ -2915,7 +2994,7 @@
         <v>74</v>
       </c>
       <c r="E32" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F32" s="7"/>
     </row>
@@ -2930,7 +3009,7 @@
         <v>76</v>
       </c>
       <c r="E33" s="60" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>77</v>
@@ -4162,7 +4241,7 @@
         <v>6</v>
       </c>
       <c r="D113" s="62" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>15</v>
@@ -4179,7 +4258,7 @@
         <v>6</v>
       </c>
       <c r="D114" s="63" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>15</v>
@@ -4196,7 +4275,7 @@
         <v>6</v>
       </c>
       <c r="D115" s="63" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>15</v>
@@ -4213,7 +4292,7 @@
         <v>6</v>
       </c>
       <c r="D116" s="63" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>15</v>
@@ -4264,7 +4343,7 @@
         <v>6</v>
       </c>
       <c r="D119" s="63" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E119" s="26" t="s">
         <v>15</v>
@@ -4296,7 +4375,7 @@
         <v>6</v>
       </c>
       <c r="D121" s="63" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E121" s="26" t="s">
         <v>15</v>
@@ -4347,24 +4426,24 @@
         <v>6</v>
       </c>
       <c r="D124" s="61" t="s">
-        <v>278</v>
+        <v>527</v>
       </c>
       <c r="E124" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F124" s="7" t="s">
-        <v>279</v>
+      <c r="F124" s="68" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C125" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E125" s="28" t="s">
         <v>15</v>
@@ -4373,13 +4452,13 @@
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E126" s="28" t="s">
         <v>15</v>
@@ -4388,13 +4467,13 @@
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E127" s="28" t="s">
         <v>15</v>
@@ -4403,47 +4482,47 @@
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>287</v>
+      <c r="D128" s="11" t="s">
+        <v>526</v>
       </c>
       <c r="E128" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F128" s="7" t="s">
-        <v>288</v>
+      <c r="F128" s="68" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C129" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E129" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C130" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>293</v>
+      <c r="D130" s="11" t="s">
+        <v>290</v>
       </c>
       <c r="E130" s="28" t="s">
         <v>15</v>
@@ -4452,379 +4531,379 @@
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C131" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E131" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F131" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B132" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C132" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E132" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C133" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D133" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E133" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C134" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D134" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="E134" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F134" s="7"/>
+    </row>
+    <row r="135" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C135" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="E135" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F135" s="7"/>
+    </row>
+    <row r="136" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B136" s="61" t="s">
+        <v>532</v>
+      </c>
+      <c r="C136" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="E136" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F136" s="7"/>
+    </row>
+    <row r="137" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B137" s="61" t="s">
+        <v>533</v>
+      </c>
+      <c r="C137" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="E137" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F137" s="7"/>
+    </row>
+    <row r="138" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B138" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C138" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E133" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F133" s="7" t="s">
+      <c r="E138" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F138" s="7"/>
+    </row>
+    <row r="139" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="3" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B134" s="3" t="s">
+      <c r="C139" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C134" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D134" s="2" t="s">
+      <c r="E139" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F139" s="7"/>
+    </row>
+    <row r="140" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B140" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E134" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F134" s="7"/>
-    </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B135" s="3" t="s">
+      <c r="C140" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C135" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D135" s="2" t="s">
+      <c r="E140" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F140" s="7"/>
+    </row>
+    <row r="141" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B141" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="E135" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F135" s="7"/>
-    </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B136" s="3" t="s">
+      <c r="C141" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C136" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D136" s="2" t="s">
+      <c r="E141" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F141" s="7"/>
+    </row>
+    <row r="142" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B142" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E136" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F136" s="7"/>
-    </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B137" s="3" t="s">
+      <c r="C142" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C137" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D137" s="2" t="s">
+      <c r="E142" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F142" s="7"/>
+    </row>
+    <row r="143" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B143" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E137" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F137" s="7"/>
-    </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B138" s="3" t="s">
+      <c r="C143" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D143" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C138" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" s="2" t="s">
+      <c r="E143" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F143" s="7"/>
+    </row>
+    <row r="144" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="E138" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F138" s="7"/>
-    </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B139" s="3" t="s">
+      <c r="C144" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D144" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C139" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D139" s="2" t="s">
+      <c r="E144" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F144" s="7"/>
+    </row>
+    <row r="145" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E139" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F139" s="7"/>
-    </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B140" s="3" t="s">
+      <c r="C145" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C140" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D140" s="2" t="s">
+      <c r="E145" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F145" s="7"/>
+    </row>
+    <row r="146" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B146" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E140" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F140" s="7"/>
-    </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B141" s="3" t="s">
+      <c r="C146" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C141" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D141" s="2" t="s">
+      <c r="E146" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" s="7"/>
+    </row>
+    <row r="147" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E141" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F141" s="7"/>
-    </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B142" s="3" t="s">
+      <c r="C147" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D147" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C142" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D142" s="2" t="s">
+      <c r="E147" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F147" s="7"/>
+    </row>
+    <row r="148" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="E142" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F142" s="7"/>
-    </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B143" s="3" t="s">
+      <c r="C148" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D148" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C143" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D143" s="2" t="s">
+      <c r="E148" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F148" s="7"/>
+    </row>
+    <row r="149" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="E143" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F143" s="7"/>
-    </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B144" s="3" t="s">
+      <c r="C149" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="C144" s="48" t="s">
-        <v>249</v>
-      </c>
-      <c r="D144" s="2" t="s">
+      <c r="E149" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F149" s="7"/>
+    </row>
+    <row r="150" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="E144" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F144" s="7"/>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B145" s="20" t="s">
+      <c r="C150" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="C145" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D145" s="24" t="s">
+      <c r="E150" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F150" s="7"/>
+    </row>
+    <row r="151" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="E145" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F145" s="7"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B146" s="20" t="s">
+      <c r="C151" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="C146" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D146" s="11" t="s">
+      <c r="E151" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F151" s="7"/>
+    </row>
+    <row r="152" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="E146" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F146" s="7"/>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B147" s="20" t="s">
+      <c r="C152" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="C147" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D147" s="11" t="s">
+      <c r="E152" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F152" s="7"/>
+    </row>
+    <row r="153" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="E147" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F147" s="7"/>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B148" s="20" t="s">
+      <c r="C153" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D153" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="C148" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D148" s="11" t="s">
+      <c r="E153" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" s="7"/>
+    </row>
+    <row r="154" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="E148" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F148" s="7"/>
-    </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B149" s="20" t="s">
+      <c r="C154" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="C149" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D149" s="11" t="s">
+      <c r="E154" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F154" s="7"/>
+    </row>
+    <row r="155" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="E149" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F149" s="7"/>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B150" s="20" t="s">
+      <c r="C155" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" s="20" t="s">
         <v>334</v>
-      </c>
-      <c r="C150" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D150" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="E150" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F150" s="7"/>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B151" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="C151" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D151" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="E151" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F151" s="7"/>
-    </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B152" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="C152" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D152" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="E152" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F152" s="7"/>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B153" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="C153" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D153" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="E153" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F153" s="7"/>
-    </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B154" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="C154" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D154" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="E154" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F154" s="7"/>
-    </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B155" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="C155" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="D155" s="11" t="s">
-        <v>345</v>
       </c>
       <c r="E155" s="30" t="s">
         <v>15</v>
@@ -4833,77 +4912,75 @@
     </row>
     <row r="156" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C156" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D156" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="E156" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F156" s="7"/>
+    </row>
+    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C157" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D157" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E157" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F157" s="7"/>
+    </row>
+    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="C158" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D158" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E158" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F158" s="7"/>
+    </row>
+    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="C159" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E159" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F159" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="C156" s="45" t="s">
+    </row>
+    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C160" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="D156" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="E156" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F156" s="7"/>
-    </row>
-    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B157" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="C157" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D157" s="64" t="s">
-        <v>519</v>
-      </c>
-      <c r="E157" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F157" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B158" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="C158" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D158" s="65" t="s">
-        <v>520</v>
-      </c>
-      <c r="E158" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F158" s="7"/>
-    </row>
-    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="C159" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D159" s="66" t="s">
-        <v>521</v>
-      </c>
-      <c r="E159" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F159" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B160" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="C160" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D160" s="65" t="s">
-        <v>522</v>
+      <c r="D160" s="11" t="s">
+        <v>344</v>
       </c>
       <c r="E160" s="54" t="s">
         <v>15</v>
@@ -4912,1130 +4989,1132 @@
     </row>
     <row r="161" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="9" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C161" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D161" s="66" t="s">
-        <v>523</v>
+      <c r="D161" s="64" t="s">
+        <v>516</v>
       </c>
       <c r="E161" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F161" s="7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="162" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="C162" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D162" s="66" t="s">
-        <v>524</v>
+        <v>347</v>
+      </c>
+      <c r="C162" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D162" s="65" t="s">
+        <v>517</v>
       </c>
       <c r="E162" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="F162" s="7" t="s">
-        <v>357</v>
-      </c>
+      <c r="F162" s="7"/>
     </row>
     <row r="163" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="C163" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D163" s="51" t="s">
-        <v>359</v>
-      </c>
-      <c r="E163" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F163" s="7"/>
+        <v>348</v>
+      </c>
+      <c r="C163" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" s="66" t="s">
+        <v>518</v>
+      </c>
+      <c r="E163" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F163" s="7" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="164" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C164" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D164" s="66" t="s">
-        <v>525</v>
+        <v>350</v>
+      </c>
+      <c r="C164" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" s="65" t="s">
+        <v>519</v>
       </c>
       <c r="E164" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F164" s="7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="165" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="C165" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C165" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D165" s="66" t="s">
-        <v>526</v>
-      </c>
-      <c r="E165" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F165" s="7" t="s">
-        <v>363</v>
-      </c>
+        <v>520</v>
+      </c>
+      <c r="E165" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F165" s="7"/>
     </row>
     <row r="166" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="C166" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="C166" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D166" s="66" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="E166" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F166" s="7" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="167" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="C167" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D167" s="66" t="s">
-        <v>528</v>
+        <v>355</v>
+      </c>
+      <c r="C167" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D167" s="51" t="s">
+        <v>356</v>
       </c>
       <c r="E167" s="54" t="s">
         <v>15</v>
       </c>
       <c r="F167" s="7" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="168" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C168" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" s="66" t="s">
+        <v>522</v>
+      </c>
+      <c r="E168" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F168" s="7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B169" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="C169" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" s="66" t="s">
+        <v>523</v>
+      </c>
+      <c r="E169" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B170" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="C170" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" s="66" t="s">
+        <v>524</v>
+      </c>
+      <c r="E170" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F170" s="7"/>
+    </row>
+    <row r="171" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="C171" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" s="66" t="s">
+        <v>525</v>
+      </c>
+      <c r="E171" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F171" s="7" t="s">
         <v>368</v>
       </c>
-      <c r="C168" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D168" s="51" t="s">
+    </row>
+    <row r="172" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="C172" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D172" s="51" t="s">
+        <v>366</v>
+      </c>
+      <c r="E172" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F172" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B173" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="C173" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" s="59" t="s">
+        <v>499</v>
+      </c>
+      <c r="E173" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F173" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="E168" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F168" s="7"/>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B169" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="C169" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D169" s="59" t="s">
+      <c r="C174" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="E174" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C175" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D175" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="E175" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F175" s="7"/>
+    </row>
+    <row r="176" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B176" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="C176" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D176" s="6" t="s">
         <v>502</v>
       </c>
-      <c r="E169" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F169" s="7" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B170" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="C170" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D170" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="E170" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F170" s="7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B171" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="C171" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D171" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="E171" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F171" s="7" t="s">
+      <c r="E176" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F176" s="7"/>
+    </row>
+    <row r="177" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B177" s="21" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B172" s="10" t="s">
+      <c r="C177" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D177" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="C172" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="E172" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F172" s="7" t="s">
+      <c r="E177" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F177" s="7"/>
+    </row>
+    <row r="178" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B178" s="21" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B173" s="21" t="s">
+      <c r="C178" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D178" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="C173" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D173" s="2" t="s">
+      <c r="E178" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F178" s="7"/>
+    </row>
+    <row r="179" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B179" s="21" t="s">
         <v>379</v>
       </c>
-      <c r="E173" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F173" s="7"/>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B174" s="21" t="s">
+      <c r="C179" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D179" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C174" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D174" s="25" t="s">
+      <c r="E179" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F179" s="7"/>
+    </row>
+    <row r="180" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B180" s="21" t="s">
         <v>381</v>
       </c>
-      <c r="E174" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F174" s="7"/>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B175" s="21" t="s">
+      <c r="C180" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C175" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D175" s="2" t="s">
+      <c r="E180" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" s="7"/>
+    </row>
+    <row r="181" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B181" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="E175" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F175" s="7"/>
-    </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B176" s="21" t="s">
+      <c r="C181" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C176" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D176" s="2" t="s">
+      <c r="E181" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" s="7"/>
+    </row>
+    <row r="182" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B182" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E176" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F176" s="7"/>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B177" s="21" t="s">
+      <c r="C182" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C177" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D177" s="2" t="s">
+      <c r="E182" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F182" s="7"/>
+    </row>
+    <row r="183" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B183" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E177" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F177" s="7"/>
-    </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B178" s="21" t="s">
+      <c r="C183" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C178" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D178" s="2" t="s">
+      <c r="E183" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" s="7"/>
+    </row>
+    <row r="184" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B184" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="E178" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F178" s="7"/>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B179" s="3" t="s">
+      <c r="C184" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D184" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C179" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D179" s="2" t="s">
+      <c r="E184" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F184" s="7"/>
+    </row>
+    <row r="185" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B185" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="E179" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F179" s="7"/>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B180" s="3" t="s">
+      <c r="C185" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C180" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D180" s="2" t="s">
+      <c r="E185" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F185" s="7"/>
+    </row>
+    <row r="186" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B186" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E180" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F180" s="7"/>
-    </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B181" s="3" t="s">
+      <c r="C186" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D186" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C181" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D181" s="3" t="s">
+      <c r="E186" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" s="7"/>
+    </row>
+    <row r="187" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B187" s="21" t="s">
         <v>395</v>
       </c>
-      <c r="E181" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F181" s="7"/>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B182" s="3" t="s">
+      <c r="C187" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D187" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C182" s="18" t="s">
+      <c r="E187" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F187" s="7"/>
+    </row>
+    <row r="188" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B188" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C188" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D182" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E182" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F182" s="7"/>
-    </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B183" s="21" t="s">
+      <c r="D188" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C183" s="49" t="s">
+      <c r="E188" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F188" s="7"/>
+    </row>
+    <row r="189" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B189" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C189" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D183" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E183" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F183" s="7"/>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B184" s="3" t="s">
+      <c r="D189" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C184" s="18" t="s">
+      <c r="E189" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F189" s="7"/>
+    </row>
+    <row r="190" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B190" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="C190" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E190" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="191" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B191" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C191" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E191" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F191" s="7"/>
+    </row>
+    <row r="192" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B192" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C192" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E192" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F192" s="7"/>
+    </row>
+    <row r="193" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B193" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C193" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E193" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F193" s="7"/>
+    </row>
+    <row r="194" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B194" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C194" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E194" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F194" s="7"/>
+    </row>
+    <row r="195" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B195" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C195" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E195" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F195" s="7"/>
+    </row>
+    <row r="196" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B196" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C196" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E196" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F196" s="7"/>
+    </row>
+    <row r="197" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B197" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C197" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E197" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F197" s="7"/>
+    </row>
+    <row r="198" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B198" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C198" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E198" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F198" s="7"/>
+    </row>
+    <row r="199" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B199" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C199" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E199" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F199" s="7"/>
+    </row>
+    <row r="200" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B200" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C200" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E200" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F200" s="7"/>
+    </row>
+    <row r="201" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B201" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C201" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E201" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F201" s="7"/>
+    </row>
+    <row r="202" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B202" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C202" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E202" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" s="7"/>
+    </row>
+    <row r="203" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B203" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C203" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E203" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F203" s="7"/>
+    </row>
+    <row r="204" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B204" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C204" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E204" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F204" s="7"/>
+    </row>
+    <row r="205" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B205" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C205" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E205" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F205" s="7"/>
+    </row>
+    <row r="206" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B206" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C206" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="E206" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F206" s="7"/>
+    </row>
+    <row r="207" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B207" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="C207" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D207" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="E207" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F207" s="7"/>
+    </row>
+    <row r="208" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B208" s="21" t="s">
+        <v>437</v>
+      </c>
+      <c r="C208" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D208" s="21" t="s">
+        <v>438</v>
+      </c>
+      <c r="E208" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F208" s="7"/>
+    </row>
+    <row r="209" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B209" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="C209" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D209" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="E209" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F209" s="7"/>
+    </row>
+    <row r="210" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B210" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="C210" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D210" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="E210" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F210" s="7"/>
+    </row>
+    <row r="211" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B211" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="C211" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D211" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="E211" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F211" s="7"/>
+    </row>
+    <row r="212" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B212" s="12" t="s">
+        <v>445</v>
+      </c>
+      <c r="C212" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D212" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="E212" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F212" s="7"/>
+    </row>
+    <row r="213" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B213" s="21" t="s">
+        <v>447</v>
+      </c>
+      <c r="C213" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D213" s="21" t="s">
+        <v>448</v>
+      </c>
+      <c r="E213" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F213" s="7"/>
+    </row>
+    <row r="214" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B214" s="21" t="s">
+        <v>449</v>
+      </c>
+      <c r="C214" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D214" s="21" t="s">
+        <v>450</v>
+      </c>
+      <c r="E214" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F214" s="7"/>
+    </row>
+    <row r="215" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B215" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="C215" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D215" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="E215" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F215" s="7"/>
+    </row>
+    <row r="216" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B216" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="C216" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D216" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="E216" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F216" s="7"/>
+    </row>
+    <row r="217" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B217" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="C217" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D184" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E184" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F184" s="7"/>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B185" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="C185" s="18" t="s">
+      <c r="D217" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="E217" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F217" s="7"/>
+    </row>
+    <row r="218" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B218" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="C218" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D185" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E185" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F185" s="7"/>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B186" s="21" t="s">
-        <v>404</v>
-      </c>
-      <c r="C186" s="43" t="s">
+      <c r="D218" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="E218" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F218" s="7"/>
+    </row>
+    <row r="219" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B219" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="C219" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D219" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="E219" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F219" s="7"/>
+    </row>
+    <row r="220" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B220" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="C220" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="D186" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E186" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F186" s="7"/>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B187" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="C187" s="48" t="s">
+      <c r="D220" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="E220" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F220" s="7"/>
+    </row>
+    <row r="221" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B221" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="C221" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="D187" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E187" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F187" s="7"/>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B188" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C188" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D188" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E188" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B189" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="C189" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D189" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="E189" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F189" s="7"/>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B190" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="C190" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="E190" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F190" s="7"/>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B191" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="C191" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D191" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E191" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F191" s="7"/>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B192" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="C192" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D192" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E192" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F192" s="7"/>
-    </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B193" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C193" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E193" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F193" s="7"/>
-    </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B194" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="C194" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="E194" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F194" s="7"/>
-    </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B195" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="C195" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E195" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F195" s="7"/>
-    </row>
-    <row r="196" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B196" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="C196" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="E196" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F196" s="7"/>
-    </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B197" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="C197" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E197" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F197" s="7"/>
-    </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B198" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="C198" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="E198" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F198" s="7"/>
-    </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B199" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="C199" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="E199" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F199" s="7"/>
-    </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B200" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="C200" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="E200" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F200" s="7"/>
-    </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B201" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="C201" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="E201" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F201" s="7"/>
-    </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B202" s="21" t="s">
-        <v>436</v>
-      </c>
-      <c r="C202" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D202" s="21" t="s">
-        <v>437</v>
-      </c>
-      <c r="E202" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F202" s="7"/>
-    </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B203" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="C203" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D203" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="E203" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F203" s="7"/>
-    </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B204" s="21" t="s">
-        <v>440</v>
-      </c>
-      <c r="C204" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D204" s="21" t="s">
-        <v>441</v>
-      </c>
-      <c r="E204" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F204" s="7"/>
-    </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B205" s="12" t="s">
-        <v>442</v>
-      </c>
-      <c r="C205" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D205" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="E205" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F205" s="7"/>
-    </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B206" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="C206" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D206" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="E206" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F206" s="7"/>
-    </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B207" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="C207" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D207" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="E207" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F207" s="7"/>
-    </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B208" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="C208" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="D208" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="E208" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F208" s="7"/>
-    </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B209" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="C209" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D209" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="E209" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F209" s="7"/>
-    </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B210" s="21" t="s">
-        <v>452</v>
-      </c>
-      <c r="C210" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D210" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="E210" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F210" s="7"/>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B211" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="C211" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D211" s="21" t="s">
-        <v>455</v>
-      </c>
-      <c r="E211" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F211" s="7"/>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B212" s="21" t="s">
-        <v>456</v>
-      </c>
-      <c r="C212" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D212" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="E212" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F212" s="7"/>
-    </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B213" s="21" t="s">
-        <v>458</v>
-      </c>
-      <c r="C213" s="33" t="s">
+      <c r="D221" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="E221" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F221" s="7"/>
+    </row>
+    <row r="222" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B222" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="C222" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D222" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="E222" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F222" s="7"/>
+    </row>
+    <row r="223" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B223" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C223" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="E223" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F223" s="7"/>
+    </row>
+    <row r="224" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B224" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="C224" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D224" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="E224" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F224" s="7"/>
+    </row>
+    <row r="225" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B225" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="C225" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D225" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="E225" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F225" s="7"/>
+    </row>
+    <row r="226" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B226" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="C226" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D226" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="E226" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F226" s="7"/>
+    </row>
+    <row r="227" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B227" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C227" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D227" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="E227" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F227" s="7"/>
+    </row>
+    <row r="228" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B228" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="C228" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D228" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="E228" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F228" s="7"/>
+    </row>
+    <row r="229" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B229" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="C229" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D229" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="E229" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F229" s="7"/>
+    </row>
+    <row r="230" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B230" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="C230" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D230" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="E230" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F230" s="7"/>
+    </row>
+    <row r="231" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B231" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="C231" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D213" s="21" t="s">
-        <v>459</v>
-      </c>
-      <c r="E213" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F213" s="7"/>
-    </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B214" s="21" t="s">
-        <v>460</v>
-      </c>
-      <c r="C214" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D214" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="E214" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F214" s="7"/>
-    </row>
-    <row r="215" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B215" s="21" t="s">
-        <v>462</v>
-      </c>
-      <c r="C215" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D215" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="E215" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F215" s="7"/>
-    </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B216" s="21" t="s">
-        <v>464</v>
-      </c>
-      <c r="C216" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="D216" s="21" t="s">
-        <v>465</v>
-      </c>
-      <c r="E216" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F216" s="7"/>
-    </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B217" s="21" t="s">
-        <v>466</v>
-      </c>
-      <c r="C217" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="D217" s="21" t="s">
-        <v>467</v>
-      </c>
-      <c r="E217" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F217" s="7"/>
-    </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B218" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="C218" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D218" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="E218" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F218" s="7"/>
-    </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B219" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="C219" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D219" s="12" t="s">
-        <v>471</v>
-      </c>
-      <c r="E219" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F219" s="7"/>
-    </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B220" s="12" t="s">
-        <v>472</v>
-      </c>
-      <c r="C220" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D220" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="E220" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F220" s="7"/>
-    </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B221" s="12" t="s">
-        <v>474</v>
-      </c>
-      <c r="C221" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D221" s="12" t="s">
-        <v>475</v>
-      </c>
-      <c r="E221" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F221" s="7"/>
-    </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B222" s="12" t="s">
-        <v>476</v>
-      </c>
-      <c r="C222" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D222" s="12" t="s">
-        <v>477</v>
-      </c>
-      <c r="E222" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F222" s="7"/>
-    </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B223" s="12" t="s">
-        <v>478</v>
-      </c>
-      <c r="C223" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D223" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="E223" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F223" s="7"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B224" s="12" t="s">
-        <v>480</v>
-      </c>
-      <c r="C224" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D224" s="12" t="s">
-        <v>481</v>
-      </c>
-      <c r="E224" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F224" s="7"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B225" s="12" t="s">
-        <v>482</v>
-      </c>
-      <c r="C225" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D225" s="12" t="s">
-        <v>483</v>
-      </c>
-      <c r="E225" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F225" s="7"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B226" s="12" t="s">
+      <c r="D231" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="C226" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D226" s="12" t="s">
+      <c r="E231" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F231" s="7"/>
+    </row>
+    <row r="232" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B232" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="E226" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F226" s="7"/>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B227" s="12" t="s">
+      <c r="C232" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D232" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="C227" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="D227" s="12" t="s">
+      <c r="E232" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F232" s="7"/>
+    </row>
+    <row r="233" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B233" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="E227" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F227" s="7"/>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B228" s="12" t="s">
+      <c r="C233" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D233" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="C228" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D228" s="12" t="s">
+      <c r="E233" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F233" s="7"/>
+    </row>
+    <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B234" s="12" t="s">
         <v>489</v>
       </c>
-      <c r="E228" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F228" s="7"/>
-    </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B229" s="12" t="s">
+      <c r="C234" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D234" s="12" t="s">
         <v>490</v>
-      </c>
-      <c r="C229" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D229" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="E229" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F229" s="7"/>
-    </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B230" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="C230" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D230" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="E230" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F230" s="7"/>
-    </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B231" s="12" t="s">
-        <v>494</v>
-      </c>
-      <c r="C231" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D231" s="12" t="s">
-        <v>495</v>
-      </c>
-      <c r="E231" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F231" s="7"/>
-    </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B232" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="C232" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D232" s="12" t="s">
-        <v>497</v>
-      </c>
-      <c r="E232" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F232" s="7"/>
-    </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B233" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="C233" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D233" s="12" t="s">
-        <v>499</v>
-      </c>
-      <c r="E233" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F233" s="7"/>
-    </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B234" s="12" t="s">
-        <v>500</v>
-      </c>
-      <c r="C234" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D234" s="12" t="s">
-        <v>501</v>
       </c>
       <c r="E234" s="37" t="s">
         <v>15</v>
@@ -6044,13 +6123,13 @@
     </row>
     <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B235" s="12" t="s">
-        <v>506</v>
+        <v>491</v>
       </c>
       <c r="C235" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D235" s="12" t="s">
-        <v>507</v>
+        <v>492</v>
       </c>
       <c r="E235" s="37" t="s">
         <v>15</v>
@@ -6059,13 +6138,13 @@
     </row>
     <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B236" s="12" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="C236" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D236" s="12" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="E236" s="37" t="s">
         <v>15</v>
@@ -6074,32 +6153,84 @@
     </row>
     <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B237" s="12" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="C237" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D237" s="12" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="E237" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B238" s="12"/>
-      <c r="C238" s="58"/>
-      <c r="D238" s="12"/>
-      <c r="E238" s="37"/>
+    <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B238" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="C238" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D238" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="E238" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F238" s="7"/>
     </row>
+    <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B239" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="C239" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D239" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="E239" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F239" s="7"/>
+    </row>
+    <row r="240" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B240" s="12" t="s">
+        <v>505</v>
+      </c>
+      <c r="C240" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D240" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="E240" s="37"/>
+      <c r="F240" s="7"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B241" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="C241" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D241" s="12" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B242" s="12"/>
+      <c r="C242" s="58"/>
+      <c r="D242" s="12"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F217">
-    <sortCondition ref="B3:B217"/>
-    <sortCondition sortBy="cellColor" ref="C3:C217" dxfId="2"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C217" dxfId="1"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C217" dxfId="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F219">
+    <sortCondition ref="B3:B219"/>
+    <sortCondition sortBy="cellColor" ref="C3:C219" dxfId="8"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C219" dxfId="7"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C219" dxfId="6"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6329,20 +6460,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6365,6 +6496,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6372,12 +6511,4 @@
     <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Definitions and Missing Reqs
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0643F5-5AED-499C-A663-B3243D75E4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2145E7-B036-49F2-A5F6-38F8C1FC887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="2772" windowWidth="20964" windowHeight="8880" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="616">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -1511,48 +1512,6 @@
     <t>The program shall have drag values at defined alpha points.</t>
   </si>
   <si>
-    <t>SAYS-PRR-001</t>
-  </si>
-  <si>
-    <t>The program shall calculate the drag coefficient due to pitch rate.</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-001</t>
-  </si>
-  <si>
-    <t>The program shall calculate the drag coefficient using 5 terms</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-002</t>
-  </si>
-  <si>
-    <t>The program shall use dynamic air pressure</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-003</t>
-  </si>
-  <si>
-    <t>The program shall use wing area</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-004</t>
-  </si>
-  <si>
-    <t>The program shall use pitch rate</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-005</t>
-  </si>
-  <si>
-    <t>The program shall use and apply a velocity conversion factor.</t>
-  </si>
-  <si>
-    <t>SAYS-PRR-002-006</t>
-  </si>
-  <si>
-    <t>The program shall use the drag coefficient from angle of flight</t>
-  </si>
-  <si>
     <t>The program shall place the tank(s) and their information in a tab labeled "Tanks".</t>
   </si>
   <si>
@@ -1565,24 +1524,6 @@
     <t>The program shall include a button labeled "Detail Tank" that will allow users to modify a listed tank.</t>
   </si>
   <si>
-    <t>SYS-PLE-001</t>
-  </si>
-  <si>
-    <t>The program shall calculate drag due to pitchrate and leading edge flap deflection.</t>
-  </si>
-  <si>
-    <t>SYS-PLE-002-001</t>
-  </si>
-  <si>
-    <t>SYS-PLE-002-002</t>
-  </si>
-  <si>
-    <t>The program shall calculate drag using wing area, air pressure, pitchrate, a conversion factor, leading edge flap position, and coefficient</t>
-  </si>
-  <si>
-    <t>The program will find the coefficient used to calculate drag as a look-ip table based on the angle of attack.</t>
-  </si>
-  <si>
     <t>Complete</t>
   </si>
   <si>
@@ -1695,13 +1636,280 @@
   </si>
   <si>
     <t>UIID-068/069/070/071</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-006</t>
+  </si>
+  <si>
+    <t>The program shall ensure that aerodynamic side-force components due to sideslip (CYb), Mach variation (CYb_M), aileron deflection (CYDa), rudder deflection (CYdr), roll rate (CYp), and yaw rate (CYr) are correctly instantiated as aerodynamic function objects under &lt;axis name="SIDE"&gt;. Each function shall compute the total side force contribution in accordance with the XML configuration structure</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-007</t>
+  </si>
+  <si>
+    <t>The program shall perform a validation check during initialization to confirm that removal of the &lt;axis unit&gt; attribute does not result in a unit mismatch in force computation or display modules. If a mismatch is detected, the program shall issue a configuration warning message and continue using the globally defined aerodynamic unit system</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-008</t>
+  </si>
+  <si>
+    <t>The program shall verify through integration testing that fcs/aileron-pos-rad input affects the computed side-force coefficient (CYDa) equivalently to the legacy configuration’s fcs/left-aileron-pos-rad, ensuring full backward compatibility</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-009</t>
+  </si>
+  <si>
+    <t>The program shall perform automated XML schema validation on the SIDE-axis definition to ensure that all functions, properties, and values comply with the aerodynamic model schema after modificationThe program shall perform automated XML schema validation on the SIDE-axis definition to ensure that all functions, properties, and values comply with the aerodynamic model schema after modification</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-010</t>
+  </si>
+  <si>
+    <t>The program shall include regression test cases comparing the computed side-force (Y) across a range of sideslip angles (−10° ≤ β ≤ +10°) between the legacy and updated XML configurations, with deviation ≤ 0.1%</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-011</t>
+  </si>
+  <si>
+    <t>The program shall log all aerodynamic coefficient loading messages related to the SIDE-axis to a configuration audit file to support verification traceabilityThe program shall log all aerodynamic coefficient loading messages related to the SIDE-axis to a configuration audit file to support verification traceability</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-012</t>
+  </si>
+  <si>
+    <t>The program shall log all aerodynamic coefficient loading messages related to the SIDE-axis to a configuration audit file to support verification traceability</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Expanded</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-001</t>
+  </si>
+  <si>
+    <t>The program shall remove the attribute unit="LBS" from the &lt;axis name="LIFT"&gt; element and ensure that lift force units are determined from global aerodynamic configuration parameters rather than per-axis attributes. Validation shall confirm computed lift values match legacy outputs within ±0.1%.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-002</t>
+  </si>
+  <si>
+    <t>The program shall update &lt;function name="aero/coefficient/CLDlef"&gt; to replace &lt;property&gt;fcs/lef-pos-norm&lt;/property&gt; with &lt;property&gt;fcs/lef-pos-rad&lt;/property&gt;. The lift-due-to-leading-edge-flap calculation shall use control surface deflection in radians, maintaining equivalent lift behavior to the normalized input model.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-005</t>
+  </si>
+  <si>
+    <t>The program shall ensure that &lt;function name="aero/coefficient/CLq_Dsb"&gt; includes the corrected description “Lift_due_to_pitch_rate_and_speedbrake_deflection” to accurately reflect the combined aerodynamic effect of pitch rate and speedbrake deflection.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-006</t>
+  </si>
+  <si>
+    <t>The program shall include &lt;property&gt;aero/function/kCLge&lt;/property&gt; within &lt;function name="aero/coefficient/CLq"&gt; to apply ground-effect scaling to lift generated by pitch rate. Validation shall confirm that lift reduction in ground effect matches expected aerodynamic performance.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-007</t>
+  </si>
+  <si>
+    <t>The program shall standardize all numeric constants and table values within the LIFT-axis XML (e.g., CLDh, CLDlef, CLDflaps, CLDsb, CLq, CLq_Dsb) to four-decimal precision without altering data values.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-008</t>
+  </si>
+  <si>
+    <t>The program shall retain &lt;value&gt;0.3500&lt;/value&gt; under &lt;function name="aero/coefficient/CLDflaps"&gt; and confirm that the lift increment due to trailing-edge flaps remains equivalent to the legacy value 0.35.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-009</t>
+  </si>
+  <si>
+    <t>The program shall verify that the &lt;table&gt; under &lt;function name="aero/coefficient/CLDh"&gt; maintains its two-dimensional interpolation structure, with aero/alpha-rad as the row and fcs/elevator-pos-rad as the column lookup variables, ensuring unchanged interpolation logic.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-010</t>
+  </si>
+  <si>
+    <t>The program shall ensure the aerodynamic functions CLDh, CLDlef, CLDflaps, CLDsb, CLq, and CLq_Dsb are instantiated correctly under the &lt;axis name="LIFT"&gt; hierarchy and that each product chain correctly computes lift components due to control-surface deflections, pitch rate, and Mach effects.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-011</t>
+  </si>
+  <si>
+    <t>The program shall validate via regression testing that lift coefficients produced from the updated XML across representative conditions (−10° ≤ α ≤ +45°, full control deflection range) remain within ±0.1% deviation from the legacy configuration.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-012</t>
+  </si>
+  <si>
+    <t>The program documentation shall be updated to reflect the transition from normalized control inputs (*_pos-norm) to radian-based inputs (*_pos-rad), including examples in aerodynamic modeling references.</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-013</t>
+  </si>
+  <si>
+    <t>The configuration management system shall record this update to the LIFT-axis XML as a controlled baseline change (Version 2.0), referencing SYS-LIFT-001 through SYS-LIFT-012 in the change log.</t>
+  </si>
+  <si>
+    <t>SYS-DTM-XXX</t>
+  </si>
+  <si>
+    <t>Mach Drag Coefficient</t>
+  </si>
+  <si>
+    <t>SYS-EXT-XXX</t>
+  </si>
+  <si>
+    <t>External Reactions</t>
+  </si>
+  <si>
+    <t>SYS-FLA-XXX</t>
+  </si>
+  <si>
+    <t>Flaps</t>
+  </si>
+  <si>
+    <t>SYS-FLC-XXX</t>
+  </si>
+  <si>
+    <t>Flight Control</t>
+  </si>
+  <si>
+    <t>SYS-GLC-XXX</t>
+  </si>
+  <si>
+    <t>Ground Effect Lift Coefficient</t>
+  </si>
+  <si>
+    <t>SYS-HDE-XXX</t>
+  </si>
+  <si>
+    <t>Horizontal Drag Coefficient</t>
+  </si>
+  <si>
+    <t>SYS-LFD-004</t>
+  </si>
+  <si>
+    <t>SYS-LFD-XXX</t>
+  </si>
+  <si>
+    <t>Leading Edge Flap Drag</t>
+  </si>
+  <si>
+    <t>SYS-MAB-XXX</t>
+  </si>
+  <si>
+    <t>Mass Balance</t>
+  </si>
+  <si>
+    <t>SYS-MEN-XXX</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>SYS-METR-XXX</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>SYS-PITCH-XXX</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>SYS-PRO-XXX</t>
+  </si>
+  <si>
+    <t>Propulsion</t>
+  </si>
+  <si>
+    <t>SYS-ROLL-XXX</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>SYS-SPE-XXX</t>
+  </si>
+  <si>
+    <t>Speedbrake</t>
+  </si>
+  <si>
+    <t>SYS-TFD-XXX</t>
+  </si>
+  <si>
+    <t>Trailing Edge Flap Drag</t>
+  </si>
+  <si>
+    <t>SYS-YAW-XXX</t>
+  </si>
+  <si>
+    <t>Yaw</t>
+  </si>
+  <si>
+    <t>SYS-GDR-XXX</t>
+  </si>
+  <si>
+    <t>Ground Reaction</t>
+  </si>
+  <si>
+    <t>SYS-SDE-XXX</t>
+  </si>
+  <si>
+    <t>Speedbrake Drag Coefficient</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-001</t>
+  </si>
+  <si>
+    <t>The program shall remove the attribute unit="LBS" from the &lt;axis name="SIDE"&gt; element and ensure that force units are resolved through the global aerodynamic configuration or derived from reference parameters (e.g., metrics/Sw-sqft and aero/qbar-psf). The implementation shall validate that all downstream calculations involving side force remain numerically consistent with previous outputs (tolerance ±0.1%)</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-002</t>
+  </si>
+  <si>
+    <t>The program shall modify the &lt;function name="aero/coefficient/CYDa"&gt; definition to replace &lt;property&gt;fcs/left-aileron-pos-rad&lt;/property&gt; with &lt;property&gt;fcs/aileron-pos-rad&lt;/property&gt;. The updated implementation shall map the unified aileron input channel to both left and right control surface effects to ensure symmetric aerodynamic response. Regression testing shall verify identical roll-yaw coupling behavior compared to the previous configuration</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-003</t>
+  </si>
+  <si>
+    <t>The program shall standardize the numerical precision of all constants and lookup table data within the SIDE-axis XML definition to four decimal places. This ensures consistency with system-wide aerodynamic data formatting standards and prevents floating-point truncation errors during coefficient interpolation</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-004</t>
+  </si>
+  <si>
+    <t>The program shall maintain the coefficient &lt;value&gt;-1.1460&lt;/value&gt; in &lt;function name="aero/coefficient/CYb"&gt;. The implementation shall verify that the resulting aerodynamic side force due to sideslip (β) remains equivalent to the prior version, using identical input conditions and solver configurations</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-005</t>
+  </si>
+  <si>
+    <t>The program shall preserve the aerodynamic coefficient datasets for &lt;function name="aero/coefficient/CYb_M"&gt;, &lt;function name="aero/coefficient/CYp"&gt;, and &lt;function name="aero/coefficient/CYr"&gt; as defined in the legacy XML, with only formatting updates applied. The interpolation algorithm shall remain unchanged to maintain consistent side force behavior across Mach and alpha ranges</t>
+  </si>
+  <si>
+    <t>SYS-SIDE-XXX</t>
+  </si>
+  <si>
+    <t>Aerodynamic SIDE</t>
+  </si>
+  <si>
+    <t>SYS-LIFT-XXX</t>
+  </si>
+  <si>
+    <t>Aerodynamic LEFT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,8 +1956,16 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1804,8 +2020,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1984,13 +2206,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2108,9 +2341,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
@@ -2483,17 +2724,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
-  <dimension ref="A2:F242"/>
+  <dimension ref="A2:F254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="79" workbookViewId="0">
-      <selection activeCell="F242" sqref="F242"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="79" workbookViewId="0">
+      <selection activeCell="D258" sqref="D258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="180.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" customWidth="1"/>
     <col min="6" max="6" width="29.109375" customWidth="1"/>
   </cols>
@@ -2843,7 +3084,7 @@
         <v>53</v>
       </c>
       <c r="E24" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>54</v>
@@ -2860,7 +3101,7 @@
         <v>56</v>
       </c>
       <c r="E25" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>57</v>
@@ -2877,7 +3118,7 @@
         <v>59</v>
       </c>
       <c r="E26" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F26" s="7"/>
     </row>
@@ -2892,7 +3133,7 @@
         <v>61</v>
       </c>
       <c r="E27" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>62</v>
@@ -2909,7 +3150,7 @@
         <v>64</v>
       </c>
       <c r="E28" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F28" s="7"/>
     </row>
@@ -2924,7 +3165,7 @@
         <v>66</v>
       </c>
       <c r="E29" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>67</v>
@@ -2941,7 +3182,7 @@
         <v>69</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F30" s="7"/>
     </row>
@@ -2956,7 +3197,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>72</v>
@@ -2973,7 +3214,7 @@
         <v>74</v>
       </c>
       <c r="E32" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F32" s="7"/>
     </row>
@@ -2988,7 +3229,7 @@
         <v>76</v>
       </c>
       <c r="E33" s="60" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>77</v>
@@ -4186,7 +4427,7 @@
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="20" t="s">
-        <v>247</v>
+        <v>577</v>
       </c>
       <c r="C111" s="35" t="s">
         <v>6</v>
@@ -4222,7 +4463,7 @@
         <v>6</v>
       </c>
       <c r="D113" s="62" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
       <c r="E113" s="26" t="s">
         <v>15</v>
@@ -4239,7 +4480,7 @@
         <v>6</v>
       </c>
       <c r="D114" s="63" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="E114" s="26" t="s">
         <v>15</v>
@@ -4256,7 +4497,7 @@
         <v>6</v>
       </c>
       <c r="D115" s="63" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="E115" s="26" t="s">
         <v>15</v>
@@ -4273,7 +4514,7 @@
         <v>6</v>
       </c>
       <c r="D116" s="63" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="E116" s="26" t="s">
         <v>15</v>
@@ -4324,7 +4565,7 @@
         <v>6</v>
       </c>
       <c r="D119" s="63" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
       <c r="E119" s="26" t="s">
         <v>15</v>
@@ -4356,7 +4597,7 @@
         <v>6</v>
       </c>
       <c r="D121" s="63" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="E121" s="26" t="s">
         <v>15</v>
@@ -4407,13 +4648,13 @@
         <v>6</v>
       </c>
       <c r="D124" s="61" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="E124" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F124" s="68" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.3">
@@ -4469,13 +4710,13 @@
         <v>6</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
       <c r="E128" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F128" s="68" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
@@ -4563,13 +4804,13 @@
     </row>
     <row r="134" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="3" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="C134" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="E134" s="29" t="s">
         <v>15</v>
@@ -4578,13 +4819,13 @@
     </row>
     <row r="135" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="3" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="C135" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="E135" s="29" t="s">
         <v>15</v>
@@ -4593,13 +4834,13 @@
     </row>
     <row r="136" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="61" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
       <c r="C136" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
       <c r="E136" s="27" t="s">
         <v>15</v>
@@ -4608,13 +4849,13 @@
     </row>
     <row r="137" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="61" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="C137" s="67" t="s">
         <v>23</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="E137" s="27" t="s">
         <v>15</v>
@@ -4635,7 +4876,7 @@
         <v>15</v>
       </c>
       <c r="F138" s="68" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
     </row>
     <row r="139" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4652,7 +4893,7 @@
         <v>15</v>
       </c>
       <c r="F139" s="68" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
     </row>
     <row r="140" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4669,7 +4910,7 @@
         <v>15</v>
       </c>
       <c r="F140" s="68" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
     </row>
     <row r="141" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4686,7 +4927,7 @@
         <v>15</v>
       </c>
       <c r="F141" s="68" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
     </row>
     <row r="142" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4703,7 +4944,7 @@
         <v>15</v>
       </c>
       <c r="F142" s="68" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
     </row>
     <row r="143" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4720,7 +4961,7 @@
         <v>15</v>
       </c>
       <c r="F143" s="68" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
     </row>
     <row r="144" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4752,7 +4993,7 @@
         <v>15</v>
       </c>
       <c r="F145" s="68" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
     </row>
     <row r="146" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4769,7 +5010,7 @@
         <v>15</v>
       </c>
       <c r="F146" s="68" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
     </row>
     <row r="147" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4786,7 +5027,7 @@
         <v>15</v>
       </c>
       <c r="F147" s="68" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4996,7 +5237,7 @@
         <v>6</v>
       </c>
       <c r="D161" s="64" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
       <c r="E161" s="54" t="s">
         <v>15</v>
@@ -5013,7 +5254,7 @@
         <v>6</v>
       </c>
       <c r="D162" s="65" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="E162" s="54" t="s">
         <v>15</v>
@@ -5028,7 +5269,7 @@
         <v>6</v>
       </c>
       <c r="D163" s="66" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
       <c r="E163" s="54" t="s">
         <v>15</v>
@@ -5045,7 +5286,7 @@
         <v>6</v>
       </c>
       <c r="D164" s="65" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="E164" s="54" t="s">
         <v>15</v>
@@ -5062,7 +5303,7 @@
         <v>6</v>
       </c>
       <c r="D165" s="66" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="E165" s="26" t="s">
         <v>15</v>
@@ -5077,7 +5318,7 @@
         <v>6</v>
       </c>
       <c r="D166" s="66" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="E166" s="54" t="s">
         <v>15</v>
@@ -5111,7 +5352,7 @@
         <v>6</v>
       </c>
       <c r="D168" s="66" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
       <c r="E168" s="54" t="s">
         <v>15</v>
@@ -5128,7 +5369,7 @@
         <v>6</v>
       </c>
       <c r="D169" s="66" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="E169" s="54" t="s">
         <v>15</v>
@@ -5145,7 +5386,7 @@
         <v>6</v>
       </c>
       <c r="D170" s="66" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
       <c r="E170" s="26" t="s">
         <v>15</v>
@@ -5160,7 +5401,7 @@
         <v>6</v>
       </c>
       <c r="D171" s="66" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="E171" s="28" t="s">
         <v>15</v>
@@ -5194,7 +5435,7 @@
         <v>6</v>
       </c>
       <c r="D173" s="59" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="E173" s="28" t="s">
         <v>15</v>
@@ -5211,7 +5452,7 @@
         <v>6</v>
       </c>
       <c r="D174" s="6" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="E174" s="28" t="s">
         <v>15</v>
@@ -5228,7 +5469,7 @@
         <v>6</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="E175" s="28" t="s">
         <v>15</v>
@@ -5243,7 +5484,7 @@
         <v>6</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="E176" s="28" t="s">
         <v>15</v>
@@ -6082,163 +6323,337 @@
       <c r="F231" s="7"/>
     </row>
     <row r="232" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B232" s="12" t="s">
-        <v>485</v>
+      <c r="B232" s="69" t="s">
+        <v>602</v>
       </c>
       <c r="C232" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D232" s="12" t="s">
-        <v>486</v>
-      </c>
-      <c r="E232" s="37" t="s">
+      <c r="D232" s="69" t="s">
+        <v>603</v>
+      </c>
+      <c r="E232" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F232" s="7"/>
     </row>
     <row r="233" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B233" s="12" t="s">
-        <v>487</v>
+      <c r="B233" s="69" t="s">
+        <v>604</v>
       </c>
       <c r="C233" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D233" s="12" t="s">
-        <v>488</v>
-      </c>
-      <c r="E233" s="37" t="s">
+      <c r="D233" s="69" t="s">
+        <v>605</v>
+      </c>
+      <c r="E233" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F233" s="7"/>
     </row>
     <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B234" s="12" t="s">
-        <v>489</v>
-      </c>
-      <c r="C234" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D234" s="12" t="s">
-        <v>490</v>
-      </c>
-      <c r="E234" s="37" t="s">
+      <c r="B234" s="69" t="s">
+        <v>606</v>
+      </c>
+      <c r="C234" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D234" s="69" t="s">
+        <v>607</v>
+      </c>
+      <c r="E234" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F234" s="7"/>
     </row>
     <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B235" s="12" t="s">
-        <v>491</v>
-      </c>
-      <c r="C235" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D235" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="E235" s="37" t="s">
+      <c r="B235" s="69" t="s">
+        <v>608</v>
+      </c>
+      <c r="C235" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D235" s="69" t="s">
+        <v>609</v>
+      </c>
+      <c r="E235" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F235" s="7"/>
     </row>
     <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B236" s="12" t="s">
-        <v>493</v>
-      </c>
-      <c r="C236" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D236" s="12" t="s">
-        <v>494</v>
-      </c>
-      <c r="E236" s="37" t="s">
+      <c r="B236" s="69" t="s">
+        <v>610</v>
+      </c>
+      <c r="C236" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D236" s="69" t="s">
+        <v>611</v>
+      </c>
+      <c r="E236" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F236" s="7"/>
     </row>
     <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B237" s="12" t="s">
-        <v>495</v>
-      </c>
-      <c r="C237" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D237" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="E237" s="37" t="s">
+      <c r="B237" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="C237" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D237" s="69" t="s">
+        <v>528</v>
+      </c>
+      <c r="E237" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F237" s="7"/>
     </row>
     <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B238" s="12" t="s">
-        <v>497</v>
+      <c r="B238" s="69" t="s">
+        <v>529</v>
       </c>
       <c r="C238" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D238" s="12" t="s">
-        <v>498</v>
-      </c>
-      <c r="E238" s="37" t="s">
+      <c r="D238" s="69" t="s">
+        <v>530</v>
+      </c>
+      <c r="E238" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F238" s="7"/>
     </row>
     <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B239" s="12" t="s">
-        <v>503</v>
+      <c r="B239" s="69" t="s">
+        <v>531</v>
       </c>
       <c r="C239" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D239" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="E239" s="37" t="s">
+      <c r="D239" s="69" t="s">
+        <v>532</v>
+      </c>
+      <c r="E239" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F239" s="7"/>
     </row>
     <row r="240" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B240" s="12" t="s">
-        <v>505</v>
+      <c r="B240" s="69" t="s">
+        <v>533</v>
       </c>
       <c r="C240" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D240" s="12" t="s">
-        <v>507</v>
-      </c>
-      <c r="E240" s="37" t="s">
+      <c r="D240" s="69" t="s">
+        <v>534</v>
+      </c>
+      <c r="E240" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F240" s="7"/>
     </row>
     <row r="241" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B241" s="12" t="s">
-        <v>506</v>
-      </c>
-      <c r="C241" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D241" s="12" t="s">
-        <v>508</v>
-      </c>
-      <c r="E241" s="37" t="s">
+      <c r="B241" s="69" t="s">
+        <v>535</v>
+      </c>
+      <c r="C241" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D241" s="69" t="s">
+        <v>536</v>
+      </c>
+      <c r="E241" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F241" s="7"/>
     </row>
     <row r="242" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B242" s="12"/>
-      <c r="C242" s="58"/>
-      <c r="D242" s="12"/>
-      <c r="E242" s="37" t="s">
+      <c r="B242" s="69" t="s">
+        <v>537</v>
+      </c>
+      <c r="C242" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D242" s="69" t="s">
+        <v>538</v>
+      </c>
+      <c r="E242" s="69" t="s">
         <v>15</v>
       </c>
       <c r="F242" s="7"/>
+    </row>
+    <row r="243" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B243" s="69" t="s">
+        <v>539</v>
+      </c>
+      <c r="C243" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D243" s="69" t="s">
+        <v>540</v>
+      </c>
+      <c r="E243" s="69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="244" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B244" s="72" t="s">
+        <v>543</v>
+      </c>
+      <c r="C244" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D244" s="72" t="s">
+        <v>544</v>
+      </c>
+      <c r="E244" s="72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="245" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B245" s="72" t="s">
+        <v>545</v>
+      </c>
+      <c r="C245" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D245" s="73" t="s">
+        <v>546</v>
+      </c>
+      <c r="E245" s="72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="246" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B246" s="72" t="s">
+        <v>547</v>
+      </c>
+      <c r="C246" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D246" s="73" t="s">
+        <v>548</v>
+      </c>
+      <c r="E246" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B247" s="72" t="s">
+        <v>549</v>
+      </c>
+      <c r="C247" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D247" s="73" t="s">
+        <v>550</v>
+      </c>
+      <c r="E247" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B248" s="72" t="s">
+        <v>551</v>
+      </c>
+      <c r="C248" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D248" s="73" t="s">
+        <v>552</v>
+      </c>
+      <c r="E248" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="249" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B249" s="72" t="s">
+        <v>553</v>
+      </c>
+      <c r="C249" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D249" s="73" t="s">
+        <v>554</v>
+      </c>
+      <c r="E249" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="250" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B250" s="72" t="s">
+        <v>555</v>
+      </c>
+      <c r="C250" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D250" s="73" t="s">
+        <v>556</v>
+      </c>
+      <c r="E250" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="251" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B251" s="72" t="s">
+        <v>557</v>
+      </c>
+      <c r="C251" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D251" s="73" t="s">
+        <v>558</v>
+      </c>
+      <c r="E251" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="252" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B252" s="72" t="s">
+        <v>559</v>
+      </c>
+      <c r="C252" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D252" s="73" t="s">
+        <v>560</v>
+      </c>
+      <c r="E252" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="253" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B253" s="72" t="s">
+        <v>561</v>
+      </c>
+      <c r="C253" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D253" s="73" t="s">
+        <v>562</v>
+      </c>
+      <c r="E253" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="254" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B254" s="72" t="s">
+        <v>563</v>
+      </c>
+      <c r="C254" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D254" s="73" t="s">
+        <v>564</v>
+      </c>
+      <c r="E254" s="37" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F219">
@@ -6250,6 +6665,201 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D04BD7-46BC-42FA-8579-8BAD2EA11B93}">
+  <dimension ref="B2:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B2" s="71" t="s">
+        <v>541</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="74" t="s">
+        <v>565</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="74" t="s">
+        <v>567</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="74" t="s">
+        <v>569</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="74" t="s">
+        <v>571</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="74" t="s">
+        <v>573</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="74" t="s">
+        <v>575</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="74" t="s">
+        <v>578</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="74" t="s">
+        <v>580</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="74" t="s">
+        <v>582</v>
+      </c>
+      <c r="C11" s="74" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="74" t="s">
+        <v>584</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="74" t="s">
+        <v>586</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="74" t="s">
+        <v>588</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="74" t="s">
+        <v>590</v>
+      </c>
+      <c r="C15" s="74" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="74" t="s">
+        <v>592</v>
+      </c>
+      <c r="C16" s="74" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="74" t="s">
+        <v>594</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="74" t="s">
+        <v>596</v>
+      </c>
+      <c r="C18" s="74" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="74" t="s">
+        <v>598</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="74" t="s">
+        <v>600</v>
+      </c>
+      <c r="C20" s="74" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="74" t="s">
+        <v>612</v>
+      </c>
+      <c r="C21" s="74" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="74" t="s">
+        <v>614</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed Sorting of New Requirements
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2145E7-B036-49F2-A5F6-38F8C1FC887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6635E75-0D1D-48BD-A29F-C6BB8445DD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="2772" windowWidth="20964" windowHeight="8880" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -2724,10 +2724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
-  <dimension ref="A2:F254"/>
+  <dimension ref="A2:F258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="79" workbookViewId="0">
-      <selection activeCell="D258" sqref="D258"/>
+    <sheetView tabSelected="1" topLeftCell="A246" zoomScale="79" workbookViewId="0">
+      <selection activeCell="F253" sqref="F253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6332,7 +6332,7 @@
       <c r="D232" s="69" t="s">
         <v>603</v>
       </c>
-      <c r="E232" s="69" t="s">
+      <c r="E232" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F232" s="7"/>
@@ -6347,132 +6347,132 @@
       <c r="D233" s="69" t="s">
         <v>605</v>
       </c>
-      <c r="E233" s="69" t="s">
+      <c r="E233" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F233" s="7"/>
     </row>
     <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B234" s="69" t="s">
-        <v>606</v>
-      </c>
-      <c r="C234" s="58" t="s">
-        <v>23</v>
+        <v>529</v>
+      </c>
+      <c r="C234" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D234" s="69" t="s">
-        <v>607</v>
-      </c>
-      <c r="E234" s="69" t="s">
+        <v>530</v>
+      </c>
+      <c r="E234" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F234" s="7"/>
     </row>
     <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B235" s="69" t="s">
-        <v>608</v>
-      </c>
-      <c r="C235" s="58" t="s">
-        <v>23</v>
+        <v>531</v>
+      </c>
+      <c r="C235" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D235" s="69" t="s">
-        <v>609</v>
-      </c>
-      <c r="E235" s="69" t="s">
+        <v>532</v>
+      </c>
+      <c r="E235" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F235" s="7"/>
     </row>
     <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B236" s="69" t="s">
-        <v>610</v>
-      </c>
-      <c r="C236" s="32" t="s">
-        <v>249</v>
+        <v>533</v>
+      </c>
+      <c r="C236" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D236" s="69" t="s">
-        <v>611</v>
-      </c>
-      <c r="E236" s="69" t="s">
+        <v>534</v>
+      </c>
+      <c r="E236" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F236" s="7"/>
     </row>
     <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B237" s="69" t="s">
-        <v>527</v>
+        <v>606</v>
       </c>
       <c r="C237" s="58" t="s">
         <v>23</v>
       </c>
       <c r="D237" s="69" t="s">
-        <v>528</v>
-      </c>
-      <c r="E237" s="69" t="s">
+        <v>607</v>
+      </c>
+      <c r="E237" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F237" s="7"/>
     </row>
     <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B238" s="69" t="s">
-        <v>529</v>
-      </c>
-      <c r="C238" s="50" t="s">
-        <v>6</v>
+        <v>608</v>
+      </c>
+      <c r="C238" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D238" s="69" t="s">
-        <v>530</v>
-      </c>
-      <c r="E238" s="69" t="s">
+        <v>609</v>
+      </c>
+      <c r="E238" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F238" s="7"/>
     </row>
     <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B239" s="69" t="s">
-        <v>531</v>
-      </c>
-      <c r="C239" s="50" t="s">
-        <v>6</v>
+        <v>527</v>
+      </c>
+      <c r="C239" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D239" s="69" t="s">
-        <v>532</v>
-      </c>
-      <c r="E239" s="69" t="s">
+        <v>528</v>
+      </c>
+      <c r="E239" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F239" s="7"/>
     </row>
     <row r="240" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B240" s="69" t="s">
-        <v>533</v>
-      </c>
-      <c r="C240" s="50" t="s">
-        <v>6</v>
+        <v>535</v>
+      </c>
+      <c r="C240" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D240" s="69" t="s">
-        <v>534</v>
-      </c>
-      <c r="E240" s="69" t="s">
+        <v>536</v>
+      </c>
+      <c r="E240" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F240" s="7"/>
     </row>
     <row r="241" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B241" s="69" t="s">
-        <v>535</v>
-      </c>
-      <c r="C241" s="58" t="s">
-        <v>23</v>
+        <v>610</v>
+      </c>
+      <c r="C241" s="32" t="s">
+        <v>249</v>
       </c>
       <c r="D241" s="69" t="s">
-        <v>536</v>
-      </c>
-      <c r="E241" s="69" t="s">
+        <v>611</v>
+      </c>
+      <c r="E241" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B242" s="69" t="s">
         <v>537</v>
       </c>
@@ -6482,12 +6482,12 @@
       <c r="D242" s="69" t="s">
         <v>538</v>
       </c>
-      <c r="E242" s="69" t="s">
+      <c r="E242" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B243" s="69" t="s">
         <v>539</v>
       </c>
@@ -6497,9 +6497,10 @@
       <c r="D243" s="69" t="s">
         <v>540</v>
       </c>
-      <c r="E243" s="69" t="s">
-        <v>15</v>
-      </c>
+      <c r="E243" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F243" s="7"/>
     </row>
     <row r="244" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B244" s="72" t="s">
@@ -6511,9 +6512,10 @@
       <c r="D244" s="72" t="s">
         <v>544</v>
       </c>
-      <c r="E244" s="72" t="s">
-        <v>15</v>
-      </c>
+      <c r="E244" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F244" s="7"/>
     </row>
     <row r="245" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B245" s="72" t="s">
@@ -6525,93 +6527,100 @@
       <c r="D245" s="73" t="s">
         <v>546</v>
       </c>
-      <c r="E245" s="72" t="s">
-        <v>15</v>
-      </c>
+      <c r="E245" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F245" s="7"/>
     </row>
     <row r="246" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B246" s="72" t="s">
-        <v>547</v>
-      </c>
-      <c r="C246" s="58" t="s">
-        <v>23</v>
+        <v>549</v>
+      </c>
+      <c r="C246" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D246" s="73" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E246" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F246" s="7"/>
     </row>
     <row r="247" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B247" s="72" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="C247" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D247" s="73" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="E247" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F247" s="7"/>
     </row>
     <row r="248" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B248" s="72" t="s">
-        <v>551</v>
-      </c>
-      <c r="C248" s="58" t="s">
-        <v>23</v>
+        <v>557</v>
+      </c>
+      <c r="C248" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D248" s="73" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="E248" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F248" s="7"/>
     </row>
     <row r="249" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B249" s="72" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="C249" s="58" t="s">
         <v>23</v>
       </c>
       <c r="D249" s="73" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="E249" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F249" s="7"/>
     </row>
     <row r="250" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B250" s="72" t="s">
-        <v>555</v>
-      </c>
-      <c r="C250" s="50" t="s">
-        <v>6</v>
+        <v>551</v>
+      </c>
+      <c r="C250" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D250" s="73" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="E250" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F250" s="7"/>
     </row>
     <row r="251" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B251" s="72" t="s">
-        <v>557</v>
-      </c>
-      <c r="C251" s="50" t="s">
-        <v>6</v>
+        <v>553</v>
+      </c>
+      <c r="C251" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D251" s="73" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E251" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F251" s="7"/>
     </row>
     <row r="252" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B252" s="72" t="s">
@@ -6626,6 +6635,7 @@
       <c r="E252" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F252" s="7"/>
     </row>
     <row r="253" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B253" s="72" t="s">
@@ -6640,8 +6650,9 @@
       <c r="E253" s="37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="254" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F253" s="7"/>
+    </row>
+    <row r="254" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B254" s="72" t="s">
         <v>563</v>
       </c>
@@ -6654,6 +6665,35 @@
       <c r="E254" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="F254" s="7"/>
+    </row>
+    <row r="255" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B255" s="72"/>
+      <c r="C255" s="50"/>
+      <c r="D255" s="73"/>
+      <c r="E255" s="37"/>
+      <c r="F255" s="7"/>
+    </row>
+    <row r="256" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B256" s="72"/>
+      <c r="C256" s="50"/>
+      <c r="D256" s="73"/>
+      <c r="E256" s="37"/>
+      <c r="F256" s="7"/>
+    </row>
+    <row r="257" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B257" s="69"/>
+      <c r="C257" s="50"/>
+      <c r="D257" s="69"/>
+      <c r="E257" s="37"/>
+      <c r="F257" s="7"/>
+    </row>
+    <row r="258" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B258" s="69"/>
+      <c r="C258" s="50"/>
+      <c r="D258" s="69"/>
+      <c r="E258" s="37"/>
+      <c r="F258" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F219">
@@ -6864,6 +6904,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -7084,14 +7132,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7102,6 +7142,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7120,16 +7170,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added requirements to implment planet selection and customization.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/axg7033_mavs_uta_edu/Documents/Submissions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0653B381-3DC5-E842-9AE8-B74783204B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DC90D2-2100-6140-9491-16A6A2144117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27200" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="664">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -2005,6 +2005,48 @@
   </si>
   <si>
     <t>The program shall have a table with the "aero/cofficient/Cnb_M" values represented by independent variable "velocities/mach within the "aero/cofficient/Cnb_M" function.</t>
+  </si>
+  <si>
+    <t>SYS-PLT-001</t>
+  </si>
+  <si>
+    <t>The program shall have a defined template for planets.</t>
+  </si>
+  <si>
+    <t>SYS-PLT-002</t>
+  </si>
+  <si>
+    <t>The program shall allow for planets to be referenced externally</t>
+  </si>
+  <si>
+    <t>SYS-PLT-004</t>
+  </si>
+  <si>
+    <t>SYS-PLT-005</t>
+  </si>
+  <si>
+    <t>The program shall have a 'property' and 'function' element included in the planet definition.</t>
+  </si>
+  <si>
+    <t>SYS-PLT-003-002</t>
+  </si>
+  <si>
+    <t>SYS-PLT-003-001</t>
+  </si>
+  <si>
+    <t>The program shall present those elements only once.</t>
+  </si>
+  <si>
+    <t>SYS-PLT-006</t>
+  </si>
+  <si>
+    <t>The program shall have the planet defintion that includes the following: semimajor axis, semiminor axis, equalatioral axis, equalatorial radius, polar radius, rotation rate, gravity, and J2.</t>
+  </si>
+  <si>
+    <t>The program shall allow for planets to be named by the user.</t>
+  </si>
+  <si>
+    <t>The program must have the J2 element as a POSITIVE number.</t>
   </si>
 </sst>
 </file>
@@ -2842,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B250" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D273" sqref="D273"/>
+    <sheetView tabSelected="1" topLeftCell="A264" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D274" sqref="D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7024,51 +7066,93 @@
       <c r="F270" s="69"/>
     </row>
     <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="72"/>
-      <c r="C271" s="69"/>
-      <c r="D271" s="69"/>
+      <c r="B271" s="72" t="s">
+        <v>650</v>
+      </c>
+      <c r="C271" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D271" s="69" t="s">
+        <v>651</v>
+      </c>
       <c r="E271" s="37"/>
       <c r="F271" s="69"/>
     </row>
     <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="72"/>
-      <c r="C272" s="69"/>
-      <c r="D272" s="69"/>
+      <c r="B272" s="72" t="s">
+        <v>652</v>
+      </c>
+      <c r="C272" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D272" s="69" t="s">
+        <v>653</v>
+      </c>
       <c r="E272" s="37"/>
       <c r="F272" s="69"/>
     </row>
     <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="72"/>
-      <c r="C273" s="69"/>
-      <c r="D273" s="69"/>
+      <c r="B273" s="72" t="s">
+        <v>658</v>
+      </c>
+      <c r="C273" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D273" s="69" t="s">
+        <v>656</v>
+      </c>
       <c r="E273" s="37"/>
       <c r="F273" s="69"/>
     </row>
     <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="72"/>
-      <c r="C274" s="69"/>
-      <c r="D274" s="69"/>
+      <c r="B274" s="72" t="s">
+        <v>657</v>
+      </c>
+      <c r="C274" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D274" s="69" t="s">
+        <v>659</v>
+      </c>
       <c r="E274" s="37"/>
       <c r="F274" s="69"/>
     </row>
     <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="72"/>
-      <c r="C275" s="69"/>
-      <c r="D275" s="69"/>
+      <c r="B275" s="72" t="s">
+        <v>654</v>
+      </c>
+      <c r="C275" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D275" s="69" t="s">
+        <v>661</v>
+      </c>
       <c r="E275" s="37"/>
       <c r="F275" s="69"/>
     </row>
     <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="72"/>
-      <c r="C276" s="69"/>
-      <c r="D276" s="69"/>
+      <c r="B276" s="72" t="s">
+        <v>655</v>
+      </c>
+      <c r="C276" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D276" s="69" t="s">
+        <v>662</v>
+      </c>
       <c r="E276" s="37"/>
       <c r="F276" s="69"/>
     </row>
     <row r="277" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B277" s="72"/>
-      <c r="C277" s="69"/>
-      <c r="D277" s="69"/>
+      <c r="B277" s="72" t="s">
+        <v>660</v>
+      </c>
+      <c r="C277" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D277" s="69" t="s">
+        <v>663</v>
+      </c>
       <c r="E277" s="37"/>
       <c r="F277" s="69"/>
     </row>
@@ -7488,12 +7572,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7718,17 +7801,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7753,18 +7846,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added requirements for input config.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DC90D2-2100-6140-9491-16A6A2144117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4561F5BE-CD07-7945-B2BD-F8D7C1F2AA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="676">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -2047,6 +2047,42 @@
   </si>
   <si>
     <t>The program must have the J2 element as a POSITIVE number.</t>
+  </si>
+  <si>
+    <t>SYS-INP-001</t>
+  </si>
+  <si>
+    <t>The program shall read the input elements and configure the input source automatically.</t>
+  </si>
+  <si>
+    <t>SYS-INP-002</t>
+  </si>
+  <si>
+    <t>The program shall allow input sources from SOCKET, QTJSBSIM, or NONE interfaces.</t>
+  </si>
+  <si>
+    <t>SYS-INP-003</t>
+  </si>
+  <si>
+    <t>The program shall allow the data rate for the input source to manage timing of data collection.</t>
+  </si>
+  <si>
+    <t>SYS-INP-004-001</t>
+  </si>
+  <si>
+    <t>The program shall specify a network port through a network port number</t>
+  </si>
+  <si>
+    <t>SYS-INP-004-002</t>
+  </si>
+  <si>
+    <t>The network port number MUST be a POSITIVE INTEGER.</t>
+  </si>
+  <si>
+    <t>SYS-INP-005-001</t>
+  </si>
+  <si>
+    <t>The program shall have an "Action" attribute to the input souce.</t>
   </si>
 </sst>
 </file>
@@ -2884,8 +2920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D274" sqref="D274"/>
+    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D283" sqref="D283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7075,7 +7111,9 @@
       <c r="D271" s="69" t="s">
         <v>651</v>
       </c>
-      <c r="E271" s="37"/>
+      <c r="E271" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F271" s="69"/>
     </row>
     <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7088,7 +7126,9 @@
       <c r="D272" s="69" t="s">
         <v>653</v>
       </c>
-      <c r="E272" s="37"/>
+      <c r="E272" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F272" s="69"/>
     </row>
     <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7101,7 +7141,9 @@
       <c r="D273" s="69" t="s">
         <v>656</v>
       </c>
-      <c r="E273" s="37"/>
+      <c r="E273" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F273" s="69"/>
     </row>
     <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7114,7 +7156,9 @@
       <c r="D274" s="69" t="s">
         <v>659</v>
       </c>
-      <c r="E274" s="37"/>
+      <c r="E274" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F274" s="69"/>
     </row>
     <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7127,7 +7171,9 @@
       <c r="D275" s="69" t="s">
         <v>661</v>
       </c>
-      <c r="E275" s="37"/>
+      <c r="E275" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F275" s="69"/>
     </row>
     <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7140,7 +7186,9 @@
       <c r="D276" s="69" t="s">
         <v>662</v>
       </c>
-      <c r="E276" s="37"/>
+      <c r="E276" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F276" s="69"/>
     </row>
     <row r="277" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -7153,49 +7201,99 @@
       <c r="D277" s="69" t="s">
         <v>663</v>
       </c>
-      <c r="E277" s="37"/>
+      <c r="E277" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F277" s="69"/>
     </row>
     <row r="278" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B278" s="69"/>
-      <c r="C278" s="69"/>
-      <c r="D278" s="69"/>
-      <c r="E278" s="37"/>
+      <c r="B278" s="69" t="s">
+        <v>664</v>
+      </c>
+      <c r="C278" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D278" s="69" t="s">
+        <v>665</v>
+      </c>
+      <c r="E278" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F278" s="69"/>
     </row>
     <row r="279" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B279" s="69"/>
-      <c r="C279" s="69"/>
-      <c r="D279" s="69"/>
-      <c r="E279" s="69"/>
+      <c r="B279" s="69" t="s">
+        <v>666</v>
+      </c>
+      <c r="C279" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D279" s="69" t="s">
+        <v>667</v>
+      </c>
+      <c r="E279" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F279" s="69"/>
     </row>
     <row r="280" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B280" s="69"/>
-      <c r="C280" s="69"/>
-      <c r="D280" s="69"/>
-      <c r="E280" s="69"/>
+      <c r="B280" s="69" t="s">
+        <v>668</v>
+      </c>
+      <c r="C280" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D280" s="69" t="s">
+        <v>669</v>
+      </c>
+      <c r="E280" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F280" s="69"/>
     </row>
     <row r="281" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B281" s="69"/>
-      <c r="C281" s="69"/>
-      <c r="D281" s="69"/>
-      <c r="E281" s="69"/>
+      <c r="B281" s="69" t="s">
+        <v>670</v>
+      </c>
+      <c r="C281" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D281" s="69" t="s">
+        <v>671</v>
+      </c>
+      <c r="E281" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F281" s="69"/>
     </row>
     <row r="282" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B282" s="69"/>
-      <c r="C282" s="69"/>
-      <c r="D282" s="69"/>
-      <c r="E282" s="69"/>
+      <c r="B282" s="69" t="s">
+        <v>672</v>
+      </c>
+      <c r="C282" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D282" s="69" t="s">
+        <v>673</v>
+      </c>
+      <c r="E282" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F282" s="69"/>
     </row>
     <row r="283" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B283" s="69"/>
-      <c r="C283" s="69"/>
-      <c r="D283" s="69"/>
-      <c r="E283" s="69"/>
+      <c r="B283" s="69" t="s">
+        <v>674</v>
+      </c>
+      <c r="C283" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D283" s="69" t="s">
+        <v>675</v>
+      </c>
+      <c r="E283" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F283" s="69"/>
     </row>
     <row r="284" spans="2:6" x14ac:dyDescent="0.2">
@@ -7572,11 +7670,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7801,27 +7900,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7846,9 +7935,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added advanced tank configuration requirements.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4561F5BE-CD07-7945-B2BD-F8D7C1F2AA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38931FAA-D752-5941-9D92-E3B1947E3E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="700">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -2083,6 +2083,78 @@
   </si>
   <si>
     <t>The program shall have an "Action" attribute to the input souce.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-001</t>
+  </si>
+  <si>
+    <t>The program shall be able to model fuel tanks using a data model defined as the 'tank' element</t>
+  </si>
+  <si>
+    <t>SYS-TNK-002-001</t>
+  </si>
+  <si>
+    <t>The program shall have an attribute called "type", and the tanks will be assigned a type.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-002-002</t>
+  </si>
+  <si>
+    <t>The program shall have 2 types of tanks: FUEL and OXIDIZER</t>
+  </si>
+  <si>
+    <t>SYS-TNK-002-003</t>
+  </si>
+  <si>
+    <t>The program shall allow specification of propellant types from a list.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-003</t>
+  </si>
+  <si>
+    <t>The program shall have a "location" attribute that specifies the position of the tank.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-004</t>
+  </si>
+  <si>
+    <t>The program shall allow tanks to be assigned a number of priority for fuel consumption</t>
+  </si>
+  <si>
+    <t>SYS-TNK-005</t>
+  </si>
+  <si>
+    <t>The program shall have an attribute called "capacity"  for maximum capacity.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-006</t>
+  </si>
+  <si>
+    <t>The program shall have an attrivute called "contents" for current capacity.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-007</t>
+  </si>
+  <si>
+    <t>The program shall have an attribute called "unusable-volume" to specify the fuel that can't be used.</t>
+  </si>
+  <si>
+    <t>SYS-TNK-008-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The program shall have attributes for the tank to specify it's physical attributes. </t>
+  </si>
+  <si>
+    <t>SYS-TNK-008-002</t>
+  </si>
+  <si>
+    <t>The program shall have attributes such as radius, temperature, density, and inertia factor</t>
+  </si>
+  <si>
+    <t>SYS-TNK-009</t>
+  </si>
+  <si>
+    <t>The program shall have an element called "grain configuration" that has cylindrical, endburning, or function typing.</t>
   </si>
 </sst>
 </file>
@@ -2920,8 +2992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D283" sqref="D283"/>
+    <sheetView tabSelected="1" topLeftCell="D270" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D296" sqref="D296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7297,87 +7369,183 @@
       <c r="F283" s="69"/>
     </row>
     <row r="284" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B284" s="69"/>
-      <c r="C284" s="69"/>
-      <c r="D284" s="69"/>
-      <c r="E284" s="69"/>
+      <c r="B284" s="69" t="s">
+        <v>676</v>
+      </c>
+      <c r="C284" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D284" s="69" t="s">
+        <v>677</v>
+      </c>
+      <c r="E284" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F284" s="69"/>
     </row>
     <row r="285" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B285" s="69"/>
-      <c r="C285" s="69"/>
-      <c r="D285" s="69"/>
-      <c r="E285" s="69"/>
+      <c r="B285" s="69" t="s">
+        <v>678</v>
+      </c>
+      <c r="C285" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D285" s="69" t="s">
+        <v>679</v>
+      </c>
+      <c r="E285" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F285" s="69"/>
     </row>
     <row r="286" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B286" s="69"/>
-      <c r="C286" s="69"/>
-      <c r="D286" s="69"/>
-      <c r="E286" s="69"/>
+      <c r="B286" s="69" t="s">
+        <v>680</v>
+      </c>
+      <c r="C286" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D286" s="69" t="s">
+        <v>681</v>
+      </c>
+      <c r="E286" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F286" s="69"/>
     </row>
     <row r="287" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B287" s="69"/>
-      <c r="C287" s="69"/>
-      <c r="D287" s="69"/>
-      <c r="E287" s="69"/>
+      <c r="B287" s="69" t="s">
+        <v>682</v>
+      </c>
+      <c r="C287" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D287" s="69" t="s">
+        <v>683</v>
+      </c>
+      <c r="E287" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F287" s="69"/>
     </row>
     <row r="288" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B288" s="69"/>
-      <c r="C288" s="69"/>
-      <c r="D288" s="69"/>
-      <c r="E288" s="69"/>
+      <c r="B288" s="69" t="s">
+        <v>684</v>
+      </c>
+      <c r="C288" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D288" s="69" t="s">
+        <v>685</v>
+      </c>
+      <c r="E288" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F288" s="69"/>
     </row>
     <row r="289" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B289" s="69"/>
-      <c r="C289" s="69"/>
-      <c r="D289" s="69"/>
-      <c r="E289" s="69"/>
+      <c r="B289" s="69" t="s">
+        <v>686</v>
+      </c>
+      <c r="C289" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D289" s="69" t="s">
+        <v>687</v>
+      </c>
+      <c r="E289" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F289" s="69"/>
     </row>
     <row r="290" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B290" s="69"/>
-      <c r="C290" s="69"/>
-      <c r="D290" s="69"/>
-      <c r="E290" s="69"/>
+      <c r="B290" s="69" t="s">
+        <v>688</v>
+      </c>
+      <c r="C290" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D290" s="69" t="s">
+        <v>689</v>
+      </c>
+      <c r="E290" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F290" s="69"/>
     </row>
     <row r="291" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B291" s="69"/>
-      <c r="C291" s="69"/>
-      <c r="D291" s="69"/>
-      <c r="E291" s="69"/>
+      <c r="B291" s="69" t="s">
+        <v>690</v>
+      </c>
+      <c r="C291" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D291" s="69" t="s">
+        <v>691</v>
+      </c>
+      <c r="E291" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F291" s="69"/>
     </row>
     <row r="292" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B292" s="69"/>
-      <c r="C292" s="69"/>
-      <c r="D292" s="69"/>
-      <c r="E292" s="69"/>
+      <c r="B292" s="69" t="s">
+        <v>692</v>
+      </c>
+      <c r="C292" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D292" s="69" t="s">
+        <v>693</v>
+      </c>
+      <c r="E292" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F292" s="69"/>
     </row>
     <row r="293" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B293" s="69"/>
-      <c r="C293" s="69"/>
-      <c r="D293" s="69"/>
-      <c r="E293" s="69"/>
+      <c r="B293" s="69" t="s">
+        <v>694</v>
+      </c>
+      <c r="C293" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D293" s="69" t="s">
+        <v>695</v>
+      </c>
+      <c r="E293" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F293" s="69"/>
     </row>
     <row r="294" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B294" s="69"/>
-      <c r="C294" s="69"/>
-      <c r="D294" s="69"/>
-      <c r="E294" s="69"/>
+      <c r="B294" s="69" t="s">
+        <v>696</v>
+      </c>
+      <c r="C294" s="75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D294" s="69" t="s">
+        <v>697</v>
+      </c>
+      <c r="E294" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F294" s="69"/>
     </row>
     <row r="295" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B295" s="69"/>
-      <c r="C295" s="69"/>
-      <c r="D295" s="69"/>
-      <c r="E295" s="69"/>
+      <c r="B295" s="69" t="s">
+        <v>698</v>
+      </c>
+      <c r="C295" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D295" s="69" t="s">
+        <v>699</v>
+      </c>
+      <c r="E295" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F295" s="69"/>
     </row>
     <row r="296" spans="2:6" x14ac:dyDescent="0.2">
@@ -7670,12 +7838,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7900,17 +8067,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7935,18 +8112,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Status of MENU requirements.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valad\Documents\UTA\UTAFall2025\FundementalProgramming\jsbsimedit2\requirements_specification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E573A41-DFAC-4354-80DD-4D9EA1ACA04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FEA936-4540-624D-AFDB-1B733173F474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -2277,12 +2277,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDAF2D0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -2309,6 +2303,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2506,7 +2506,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2605,37 +2605,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
@@ -2644,55 +2644,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3063,20 +3015,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="75" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="255.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3093,7 +3045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -3108,7 +3060,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -3123,7 +3075,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -3138,7 +3090,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3153,7 +3105,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3168,7 +3120,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3183,7 +3135,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -3198,7 +3150,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3213,7 +3165,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -3228,7 +3180,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -3243,7 +3195,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -3260,7 +3212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3275,7 +3227,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3290,7 +3242,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3305,7 +3257,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3320,7 +3272,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -3335,7 +3287,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -3350,7 +3302,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -3365,7 +3317,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -3380,7 +3332,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -3395,7 +3347,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -3410,7 +3362,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3420,14 +3372,14 @@
       <c r="D24" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -3437,14 +3389,14 @@
       <c r="D25" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -3454,12 +3406,12 @@
       <c r="D26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="60" t="s">
+      <c r="E26" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -3469,14 +3421,14 @@
       <c r="D27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -3486,12 +3438,12 @@
       <c r="D28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="60" t="s">
+      <c r="E28" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3501,14 +3453,14 @@
       <c r="D29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="60" t="s">
+      <c r="E29" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -3518,12 +3470,12 @@
       <c r="D30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="60" t="s">
+      <c r="E30" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -3533,14 +3485,14 @@
       <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -3550,12 +3502,12 @@
       <c r="D32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -3565,14 +3517,14 @@
       <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -3587,7 +3539,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -3607,7 +3559,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -3622,7 +3574,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -3639,7 +3591,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -3654,7 +3606,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -3671,7 +3623,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -3686,7 +3638,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -3703,7 +3655,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -3718,7 +3670,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -3735,7 +3687,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -3750,7 +3702,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3767,7 +3719,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3782,7 +3734,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3799,7 +3751,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3814,7 +3766,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3829,7 +3781,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3846,7 +3798,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3861,7 +3813,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3876,7 +3828,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3891,7 +3843,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3906,7 +3858,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3921,7 +3873,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3938,7 +3890,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3953,7 +3905,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3968,7 +3920,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3983,7 +3935,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -3998,7 +3950,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -4013,7 +3965,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -4030,7 +3982,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -4045,7 +3997,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -4060,7 +4012,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -4075,7 +4027,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -4090,7 +4042,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -4105,7 +4057,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -4122,7 +4074,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -4137,7 +4089,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -4152,7 +4104,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -4167,7 +4119,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -4182,7 +4134,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -4197,7 +4149,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -4214,7 +4166,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -4229,7 +4181,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -4244,7 +4196,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -4259,7 +4211,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -4274,7 +4226,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -4289,7 +4241,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -4306,7 +4258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -4321,7 +4273,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -4336,7 +4288,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -4351,7 +4303,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -4366,7 +4318,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -4381,7 +4333,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -4398,7 +4350,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -4413,7 +4365,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -4428,7 +4380,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -4443,7 +4395,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -4458,7 +4410,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -4473,7 +4425,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -4490,7 +4442,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B93" s="3" t="s">
         <v>211</v>
       </c>
@@ -4505,7 +4457,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B94" s="3" t="s">
         <v>213</v>
       </c>
@@ -4520,7 +4472,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B95" s="3" t="s">
         <v>215</v>
       </c>
@@ -4535,7 +4487,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B96" s="3" t="s">
         <v>217</v>
       </c>
@@ -4550,7 +4502,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B97" s="3" t="s">
         <v>219</v>
       </c>
@@ -4565,7 +4517,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B98" s="3" t="s">
         <v>221</v>
       </c>
@@ -4580,7 +4532,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B99" s="3" t="s">
         <v>223</v>
       </c>
@@ -4595,7 +4547,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="3" t="s">
         <v>225</v>
       </c>
@@ -4610,7 +4562,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="3" t="s">
         <v>227</v>
       </c>
@@ -4625,7 +4577,7 @@
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
         <v>229</v>
       </c>
@@ -4640,7 +4592,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -4655,37 +4607,37 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="61" t="s">
+    <row r="104" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="60" t="s">
         <v>700</v>
       </c>
-      <c r="C104" s="77" t="s">
+      <c r="C104" s="76" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="11" t="s">
         <v>701</v>
       </c>
-      <c r="E104" s="78" t="s">
+      <c r="E104" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B105" s="61" t="s">
+    <row r="105" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="60" t="s">
         <v>702</v>
       </c>
-      <c r="C105" s="77" t="s">
+      <c r="C105" s="76" t="s">
         <v>703</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>704</v>
       </c>
-      <c r="E105" s="78" t="s">
+      <c r="E105" s="77" t="s">
         <v>489</v>
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B106" s="20" t="s">
         <v>233</v>
       </c>
@@ -4700,7 +4652,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="20" t="s">
         <v>235</v>
       </c>
@@ -4715,7 +4667,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="20" t="s">
         <v>237</v>
       </c>
@@ -4730,7 +4682,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="20" t="s">
         <v>239</v>
       </c>
@@ -4745,7 +4697,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="20" t="s">
         <v>241</v>
       </c>
@@ -4760,7 +4712,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="20" t="s">
         <v>243</v>
       </c>
@@ -4773,11 +4725,11 @@
       <c r="E111" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="F111" s="68" t="s">
+      <c r="F111" s="67" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="20" t="s">
         <v>245</v>
       </c>
@@ -4792,7 +4744,7 @@
       </c>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="20" t="s">
         <v>577</v>
       </c>
@@ -4807,7 +4759,7 @@
       </c>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B114" s="20" t="s">
         <v>247</v>
       </c>
@@ -4822,14 +4774,14 @@
       </c>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="7" t="s">
         <v>251</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="62" t="s">
+      <c r="D115" s="61" t="s">
         <v>490</v>
       </c>
       <c r="E115" s="26" t="s">
@@ -4839,14 +4791,14 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="7" t="s">
         <v>253</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="63" t="s">
+      <c r="D116" s="62" t="s">
         <v>491</v>
       </c>
       <c r="E116" s="26" t="s">
@@ -4856,14 +4808,14 @@
         <v>254</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B117" s="7" t="s">
         <v>255</v>
       </c>
       <c r="C117" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="63" t="s">
+      <c r="D117" s="62" t="s">
         <v>492</v>
       </c>
       <c r="E117" s="26" t="s">
@@ -4873,14 +4825,14 @@
         <v>256</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="7" t="s">
         <v>257</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D118" s="63" t="s">
+      <c r="D118" s="62" t="s">
         <v>493</v>
       </c>
       <c r="E118" s="26" t="s">
@@ -4890,7 +4842,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="7" t="s">
         <v>259</v>
       </c>
@@ -4907,7 +4859,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B120" s="7" t="s">
         <v>262</v>
       </c>
@@ -4924,14 +4876,14 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B121" s="7" t="s">
         <v>265</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D121" s="63" t="s">
+      <c r="D121" s="62" t="s">
         <v>494</v>
       </c>
       <c r="E121" s="26" t="s">
@@ -4939,7 +4891,7 @@
       </c>
       <c r="F121" s="7"/>
     </row>
-    <row r="122" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B122" s="7" t="s">
         <v>266</v>
       </c>
@@ -4956,14 +4908,14 @@
         <v>268</v>
       </c>
     </row>
-    <row r="123" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="7" t="s">
         <v>269</v>
       </c>
       <c r="C123" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="63" t="s">
+      <c r="D123" s="62" t="s">
         <v>495</v>
       </c>
       <c r="E123" s="26" t="s">
@@ -4973,7 +4925,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
         <v>271</v>
       </c>
@@ -4990,7 +4942,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="7" t="s">
         <v>274</v>
       </c>
@@ -5007,24 +4959,24 @@
         <v>276</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
         <v>277</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D126" s="61" t="s">
+      <c r="D126" s="60" t="s">
         <v>507</v>
       </c>
-      <c r="E126" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F126" s="68" t="s">
+      <c r="E126" s="77" t="s">
+        <v>489</v>
+      </c>
+      <c r="F126" s="67" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
         <v>278</v>
       </c>
@@ -5034,12 +4986,12 @@
       <c r="D127" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="E127" s="28" t="s">
-        <v>15</v>
+      <c r="E127" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
         <v>280</v>
       </c>
@@ -5049,12 +5001,12 @@
       <c r="D128" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E128" s="28" t="s">
-        <v>15</v>
+      <c r="E128" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
         <v>282</v>
       </c>
@@ -5064,12 +5016,12 @@
       <c r="D129" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E129" s="28" t="s">
-        <v>15</v>
+      <c r="E129" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
         <v>284</v>
       </c>
@@ -5079,14 +5031,14 @@
       <c r="D130" s="11" t="s">
         <v>506</v>
       </c>
-      <c r="E130" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F130" s="68" t="s">
+      <c r="E130" s="77" t="s">
+        <v>489</v>
+      </c>
+      <c r="F130" s="67" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
         <v>286</v>
       </c>
@@ -5096,14 +5048,14 @@
       <c r="D131" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E131" s="27" t="s">
-        <v>15</v>
+      <c r="E131" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F131" s="7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
         <v>289</v>
       </c>
@@ -5113,12 +5065,12 @@
       <c r="D132" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="E132" s="28" t="s">
-        <v>15</v>
+      <c r="E132" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F132" s="7"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
         <v>291</v>
       </c>
@@ -5128,14 +5080,14 @@
       <c r="D133" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E133" s="28" t="s">
-        <v>15</v>
+      <c r="E133" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F133" s="7" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="134" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
         <v>293</v>
       </c>
@@ -5145,14 +5097,14 @@
       <c r="D134" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E134" s="27" t="s">
-        <v>15</v>
+      <c r="E134" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F134" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
         <v>296</v>
       </c>
@@ -5162,18 +5114,18 @@
       <c r="D135" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E135" s="27" t="s">
-        <v>15</v>
+      <c r="E135" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F135" s="7" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C136" s="67" t="s">
+      <c r="C136" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D136" s="11" t="s">
@@ -5184,11 +5136,11 @@
       </c>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="C137" s="67" t="s">
+      <c r="C137" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D137" s="11" t="s">
@@ -5199,26 +5151,26 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B138" s="61" t="s">
+    <row r="138" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="60" t="s">
         <v>512</v>
       </c>
-      <c r="C138" s="67" t="s">
+      <c r="C138" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D138" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="E138" s="27" t="s">
-        <v>15</v>
+      <c r="E138" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B139" s="61" t="s">
+    <row r="139" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="60" t="s">
         <v>513</v>
       </c>
-      <c r="C139" s="67" t="s">
+      <c r="C139" s="66" t="s">
         <v>23</v>
       </c>
       <c r="D139" s="11" t="s">
@@ -5229,7 +5181,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
         <v>299</v>
       </c>
@@ -5242,11 +5194,11 @@
       <c r="E140" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F140" s="68" t="s">
+      <c r="F140" s="67" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
         <v>301</v>
       </c>
@@ -5259,11 +5211,11 @@
       <c r="E141" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F141" s="68" t="s">
+      <c r="F141" s="67" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
         <v>303</v>
       </c>
@@ -5276,11 +5228,11 @@
       <c r="E142" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F142" s="68" t="s">
+      <c r="F142" s="67" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
         <v>305</v>
       </c>
@@ -5293,11 +5245,11 @@
       <c r="E143" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F143" s="68" t="s">
+      <c r="F143" s="67" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
         <v>307</v>
       </c>
@@ -5310,11 +5262,11 @@
       <c r="E144" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F144" s="68" t="s">
+      <c r="F144" s="67" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
         <v>309</v>
       </c>
@@ -5327,11 +5279,11 @@
       <c r="E145" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F145" s="68" t="s">
+      <c r="F145" s="67" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
         <v>311</v>
       </c>
@@ -5346,7 +5298,7 @@
       </c>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
         <v>313</v>
       </c>
@@ -5359,11 +5311,11 @@
       <c r="E147" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F147" s="68" t="s">
+      <c r="F147" s="67" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="148" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
         <v>315</v>
       </c>
@@ -5376,11 +5328,11 @@
       <c r="E148" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F148" s="68" t="s">
+      <c r="F148" s="67" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
         <v>317</v>
       </c>
@@ -5393,11 +5345,11 @@
       <c r="E149" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F149" s="68" t="s">
+      <c r="F149" s="67" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
         <v>319</v>
       </c>
@@ -5412,7 +5364,7 @@
       </c>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B151" s="20" t="s">
         <v>321</v>
       </c>
@@ -5425,11 +5377,11 @@
       <c r="E151" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F151" s="68" t="s">
+      <c r="F151" s="67" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B152" s="20" t="s">
         <v>323</v>
       </c>
@@ -5444,7 +5396,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="20" t="s">
         <v>325</v>
       </c>
@@ -5459,7 +5411,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B154" s="20" t="s">
         <v>327</v>
       </c>
@@ -5474,7 +5426,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="20" t="s">
         <v>329</v>
       </c>
@@ -5489,7 +5441,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="20" t="s">
         <v>331</v>
       </c>
@@ -5504,7 +5456,7 @@
       </c>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="20" t="s">
         <v>333</v>
       </c>
@@ -5519,7 +5471,7 @@
       </c>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B158" s="20" t="s">
         <v>335</v>
       </c>
@@ -5534,7 +5486,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B159" s="20" t="s">
         <v>337</v>
       </c>
@@ -5549,7 +5501,7 @@
       </c>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B160" s="20" t="s">
         <v>339</v>
       </c>
@@ -5564,7 +5516,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B161" s="20" t="s">
         <v>341</v>
       </c>
@@ -5581,7 +5533,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B162" s="20" t="s">
         <v>343</v>
       </c>
@@ -5596,14 +5548,14 @@
       </c>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B163" s="9" t="s">
         <v>345</v>
       </c>
       <c r="C163" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D163" s="64" t="s">
+      <c r="D163" s="63" t="s">
         <v>496</v>
       </c>
       <c r="E163" s="54" t="s">
@@ -5613,14 +5565,14 @@
         <v>349</v>
       </c>
     </row>
-    <row r="164" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>347</v>
       </c>
       <c r="C164" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D164" s="65" t="s">
+      <c r="D164" s="64" t="s">
         <v>497</v>
       </c>
       <c r="E164" s="54" t="s">
@@ -5628,14 +5580,14 @@
       </c>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>348</v>
       </c>
       <c r="C165" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D165" s="66" t="s">
+      <c r="D165" s="65" t="s">
         <v>498</v>
       </c>
       <c r="E165" s="54" t="s">
@@ -5645,14 +5597,14 @@
         <v>352</v>
       </c>
     </row>
-    <row r="166" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B166" s="9" t="s">
         <v>350</v>
       </c>
       <c r="C166" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D166" s="65" t="s">
+      <c r="D166" s="64" t="s">
         <v>499</v>
       </c>
       <c r="E166" s="54" t="s">
@@ -5662,14 +5614,14 @@
         <v>354</v>
       </c>
     </row>
-    <row r="167" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="9" t="s">
         <v>351</v>
       </c>
       <c r="C167" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D167" s="66" t="s">
+      <c r="D167" s="65" t="s">
         <v>500</v>
       </c>
       <c r="E167" s="26" t="s">
@@ -5677,14 +5629,14 @@
       </c>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="9" t="s">
         <v>353</v>
       </c>
       <c r="C168" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D168" s="66" t="s">
+      <c r="D168" s="65" t="s">
         <v>501</v>
       </c>
       <c r="E168" s="54" t="s">
@@ -5694,7 +5646,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="169" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="9" t="s">
         <v>355</v>
       </c>
@@ -5711,14 +5663,14 @@
         <v>360</v>
       </c>
     </row>
-    <row r="170" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="9" t="s">
         <v>357</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D170" s="66" t="s">
+      <c r="D170" s="65" t="s">
         <v>502</v>
       </c>
       <c r="E170" s="54" t="s">
@@ -5728,14 +5680,14 @@
         <v>362</v>
       </c>
     </row>
-    <row r="171" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="9" t="s">
         <v>359</v>
       </c>
       <c r="C171" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D171" s="66" t="s">
+      <c r="D171" s="65" t="s">
         <v>503</v>
       </c>
       <c r="E171" s="54" t="s">
@@ -5745,14 +5697,14 @@
         <v>364</v>
       </c>
     </row>
-    <row r="172" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="9" t="s">
         <v>361</v>
       </c>
       <c r="C172" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D172" s="66" t="s">
+      <c r="D172" s="65" t="s">
         <v>504</v>
       </c>
       <c r="E172" s="26" t="s">
@@ -5760,14 +5712,14 @@
       </c>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>363</v>
       </c>
       <c r="C173" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D173" s="66" t="s">
+      <c r="D173" s="65" t="s">
         <v>505</v>
       </c>
       <c r="E173" s="28" t="s">
@@ -5777,7 +5729,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="174" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>365</v>
       </c>
@@ -5794,7 +5746,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="175" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10" t="s">
         <v>367</v>
       </c>
@@ -5811,7 +5763,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="176" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B176" s="10" t="s">
         <v>369</v>
       </c>
@@ -5828,7 +5780,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="177" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B177" s="10" t="s">
         <v>371</v>
       </c>
@@ -5843,7 +5795,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B178" s="10" t="s">
         <v>373</v>
       </c>
@@ -5858,7 +5810,7 @@
       </c>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="21" t="s">
         <v>375</v>
       </c>
@@ -5873,7 +5825,7 @@
       </c>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="21" t="s">
         <v>377</v>
       </c>
@@ -5888,7 +5840,7 @@
       </c>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="21" t="s">
         <v>379</v>
       </c>
@@ -5903,7 +5855,7 @@
       </c>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="21" t="s">
         <v>381</v>
       </c>
@@ -5918,7 +5870,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="21" t="s">
         <v>383</v>
       </c>
@@ -5933,7 +5885,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="21" t="s">
         <v>385</v>
       </c>
@@ -5948,7 +5900,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
         <v>387</v>
       </c>
@@ -5963,7 +5915,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B186" s="3" t="s">
         <v>389</v>
       </c>
@@ -5978,7 +5930,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B187" s="3" t="s">
         <v>391</v>
       </c>
@@ -5993,7 +5945,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="3" t="s">
         <v>393</v>
       </c>
@@ -6008,7 +5960,7 @@
       </c>
       <c r="F188" s="7"/>
     </row>
-    <row r="189" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="21" t="s">
         <v>395</v>
       </c>
@@ -6023,7 +5975,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B190" s="3" t="s">
         <v>397</v>
       </c>
@@ -6038,7 +5990,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="3" t="s">
         <v>399</v>
       </c>
@@ -6053,7 +6005,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="21" t="s">
         <v>401</v>
       </c>
@@ -6066,11 +6018,11 @@
       <c r="E192" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F192" s="68" t="s">
+      <c r="F192" s="67" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
         <v>403</v>
       </c>
@@ -6085,7 +6037,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>405</v>
       </c>
@@ -6098,11 +6050,11 @@
       <c r="E194" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F194" s="68" t="s">
+      <c r="F194" s="67" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>407</v>
       </c>
@@ -6117,7 +6069,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
         <v>409</v>
       </c>
@@ -6132,7 +6084,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>411</v>
       </c>
@@ -6147,7 +6099,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
         <v>413</v>
       </c>
@@ -6162,7 +6114,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="3" t="s">
         <v>415</v>
       </c>
@@ -6177,7 +6129,7 @@
       </c>
       <c r="F199" s="7"/>
     </row>
-    <row r="200" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
         <v>417</v>
       </c>
@@ -6192,7 +6144,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
         <v>419</v>
       </c>
@@ -6207,7 +6159,7 @@
       </c>
       <c r="F201" s="7"/>
     </row>
-    <row r="202" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
         <v>421</v>
       </c>
@@ -6222,7 +6174,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
         <v>423</v>
       </c>
@@ -6237,7 +6189,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
         <v>425</v>
       </c>
@@ -6252,7 +6204,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
         <v>427</v>
       </c>
@@ -6267,7 +6219,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
         <v>429</v>
       </c>
@@ -6282,7 +6234,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
         <v>431</v>
       </c>
@@ -6297,7 +6249,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="21" t="s">
         <v>433</v>
       </c>
@@ -6312,7 +6264,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="21" t="s">
         <v>435</v>
       </c>
@@ -6327,7 +6279,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B210" s="21" t="s">
         <v>437</v>
       </c>
@@ -6342,7 +6294,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="12" t="s">
         <v>439</v>
       </c>
@@ -6357,7 +6309,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="12" t="s">
         <v>441</v>
       </c>
@@ -6372,7 +6324,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="12" t="s">
         <v>443</v>
       </c>
@@ -6387,7 +6339,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="12" t="s">
         <v>445</v>
       </c>
@@ -6402,7 +6354,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="21" t="s">
         <v>447</v>
       </c>
@@ -6415,11 +6367,11 @@
       <c r="E215" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F215" s="68" t="s">
+      <c r="F215" s="67" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="216" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="21" t="s">
         <v>449</v>
       </c>
@@ -6434,7 +6386,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="21" t="s">
         <v>451</v>
       </c>
@@ -6449,7 +6401,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="21" t="s">
         <v>453</v>
       </c>
@@ -6464,7 +6416,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="21" t="s">
         <v>455</v>
       </c>
@@ -6479,7 +6431,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="21" t="s">
         <v>457</v>
       </c>
@@ -6494,7 +6446,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="21" t="s">
         <v>459</v>
       </c>
@@ -6509,7 +6461,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B222" s="21" t="s">
         <v>461</v>
       </c>
@@ -6524,7 +6476,7 @@
       </c>
       <c r="F222" s="7"/>
     </row>
-    <row r="223" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B223" s="21" t="s">
         <v>463</v>
       </c>
@@ -6539,7 +6491,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B224" s="12" t="s">
         <v>465</v>
       </c>
@@ -6554,7 +6506,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B225" s="12" t="s">
         <v>467</v>
       </c>
@@ -6569,7 +6521,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B226" s="12" t="s">
         <v>469</v>
       </c>
@@ -6584,7 +6536,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B227" s="12" t="s">
         <v>471</v>
       </c>
@@ -6599,7 +6551,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B228" s="12" t="s">
         <v>473</v>
       </c>
@@ -6614,7 +6566,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B229" s="12" t="s">
         <v>475</v>
       </c>
@@ -6629,7 +6581,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B230" s="12" t="s">
         <v>477</v>
       </c>
@@ -6644,7 +6596,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B231" s="12" t="s">
         <v>479</v>
       </c>
@@ -6659,7 +6611,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B232" s="12" t="s">
         <v>481</v>
       </c>
@@ -6674,7 +6626,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B233" s="12" t="s">
         <v>483</v>
       </c>
@@ -6689,14 +6641,14 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B234" s="69" t="s">
+    <row r="234" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B234" s="68" t="s">
         <v>602</v>
       </c>
       <c r="C234" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D234" s="69" t="s">
+      <c r="D234" s="68" t="s">
         <v>603</v>
       </c>
       <c r="E234" s="37" t="s">
@@ -6704,14 +6656,14 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B235" s="69" t="s">
+    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B235" s="68" t="s">
         <v>604</v>
       </c>
       <c r="C235" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D235" s="69" t="s">
+      <c r="D235" s="68" t="s">
         <v>605</v>
       </c>
       <c r="E235" s="37" t="s">
@@ -6719,14 +6671,14 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B236" s="69" t="s">
+    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B236" s="68" t="s">
         <v>529</v>
       </c>
       <c r="C236" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D236" s="69" t="s">
+      <c r="D236" s="68" t="s">
         <v>530</v>
       </c>
       <c r="E236" s="37" t="s">
@@ -6734,14 +6686,14 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B237" s="69" t="s">
+    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B237" s="68" t="s">
         <v>531</v>
       </c>
       <c r="C237" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D237" s="69" t="s">
+      <c r="D237" s="68" t="s">
         <v>532</v>
       </c>
       <c r="E237" s="37" t="s">
@@ -6749,14 +6701,14 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B238" s="69" t="s">
+    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B238" s="68" t="s">
         <v>533</v>
       </c>
       <c r="C238" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D238" s="69" t="s">
+      <c r="D238" s="68" t="s">
         <v>534</v>
       </c>
       <c r="E238" s="37" t="s">
@@ -6764,14 +6716,14 @@
       </c>
       <c r="F238" s="7"/>
     </row>
-    <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B239" s="69" t="s">
+    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B239" s="68" t="s">
         <v>606</v>
       </c>
       <c r="C239" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D239" s="69" t="s">
+      <c r="D239" s="68" t="s">
         <v>607</v>
       </c>
       <c r="E239" s="37" t="s">
@@ -6779,14 +6731,14 @@
       </c>
       <c r="F239" s="7"/>
     </row>
-    <row r="240" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B240" s="69" t="s">
+    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B240" s="68" t="s">
         <v>608</v>
       </c>
       <c r="C240" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D240" s="69" t="s">
+      <c r="D240" s="68" t="s">
         <v>609</v>
       </c>
       <c r="E240" s="37" t="s">
@@ -6794,14 +6746,14 @@
       </c>
       <c r="F240" s="7"/>
     </row>
-    <row r="241" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B241" s="69" t="s">
+    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B241" s="68" t="s">
         <v>527</v>
       </c>
       <c r="C241" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D241" s="69" t="s">
+      <c r="D241" s="68" t="s">
         <v>528</v>
       </c>
       <c r="E241" s="37" t="s">
@@ -6809,14 +6761,14 @@
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B242" s="69" t="s">
+    <row r="242" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B242" s="68" t="s">
         <v>535</v>
       </c>
       <c r="C242" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D242" s="69" t="s">
+      <c r="D242" s="68" t="s">
         <v>536</v>
       </c>
       <c r="E242" s="37" t="s">
@@ -6824,14 +6776,14 @@
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B243" s="69" t="s">
+    <row r="243" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B243" s="68" t="s">
         <v>610</v>
       </c>
       <c r="C243" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D243" s="69" t="s">
+      <c r="D243" s="68" t="s">
         <v>611</v>
       </c>
       <c r="E243" s="37" t="s">
@@ -6839,14 +6791,14 @@
       </c>
       <c r="F243" s="7"/>
     </row>
-    <row r="244" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B244" s="69" t="s">
+    <row r="244" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B244" s="68" t="s">
         <v>537</v>
       </c>
       <c r="C244" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D244" s="69" t="s">
+      <c r="D244" s="68" t="s">
         <v>538</v>
       </c>
       <c r="E244" s="37" t="s">
@@ -6854,14 +6806,14 @@
       </c>
       <c r="F244" s="7"/>
     </row>
-    <row r="245" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B245" s="69" t="s">
+    <row r="245" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B245" s="68" t="s">
         <v>539</v>
       </c>
       <c r="C245" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D245" s="69" t="s">
+      <c r="D245" s="68" t="s">
         <v>540</v>
       </c>
       <c r="E245" s="37" t="s">
@@ -6869,14 +6821,14 @@
       </c>
       <c r="F245" s="7"/>
     </row>
-    <row r="246" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B246" s="72" t="s">
+    <row r="246" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="71" t="s">
         <v>543</v>
       </c>
       <c r="C246" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D246" s="72" t="s">
+      <c r="D246" s="71" t="s">
         <v>544</v>
       </c>
       <c r="E246" s="37" t="s">
@@ -6884,14 +6836,14 @@
       </c>
       <c r="F246" s="7"/>
     </row>
-    <row r="247" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B247" s="72" t="s">
+    <row r="247" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B247" s="71" t="s">
         <v>545</v>
       </c>
       <c r="C247" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D247" s="73" t="s">
+      <c r="D247" s="72" t="s">
         <v>546</v>
       </c>
       <c r="E247" s="37" t="s">
@@ -6899,14 +6851,14 @@
       </c>
       <c r="F247" s="7"/>
     </row>
-    <row r="248" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B248" s="72" t="s">
+    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B248" s="71" t="s">
         <v>549</v>
       </c>
       <c r="C248" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D248" s="73" t="s">
+      <c r="D248" s="72" t="s">
         <v>550</v>
       </c>
       <c r="E248" s="37" t="s">
@@ -6914,14 +6866,14 @@
       </c>
       <c r="F248" s="7"/>
     </row>
-    <row r="249" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B249" s="72" t="s">
+    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="71" t="s">
         <v>555</v>
       </c>
       <c r="C249" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D249" s="73" t="s">
+      <c r="D249" s="72" t="s">
         <v>556</v>
       </c>
       <c r="E249" s="37" t="s">
@@ -6929,14 +6881,14 @@
       </c>
       <c r="F249" s="7"/>
     </row>
-    <row r="250" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B250" s="72" t="s">
+    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="71" t="s">
         <v>557</v>
       </c>
       <c r="C250" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D250" s="73" t="s">
+      <c r="D250" s="72" t="s">
         <v>558</v>
       </c>
       <c r="E250" s="37" t="s">
@@ -6944,14 +6896,14 @@
       </c>
       <c r="F250" s="7"/>
     </row>
-    <row r="251" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B251" s="72" t="s">
+    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B251" s="71" t="s">
         <v>547</v>
       </c>
       <c r="C251" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D251" s="73" t="s">
+      <c r="D251" s="72" t="s">
         <v>548</v>
       </c>
       <c r="E251" s="37" t="s">
@@ -6959,14 +6911,14 @@
       </c>
       <c r="F251" s="7"/>
     </row>
-    <row r="252" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B252" s="72" t="s">
+    <row r="252" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B252" s="71" t="s">
         <v>551</v>
       </c>
       <c r="C252" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D252" s="73" t="s">
+      <c r="D252" s="72" t="s">
         <v>552</v>
       </c>
       <c r="E252" s="37" t="s">
@@ -6974,14 +6926,14 @@
       </c>
       <c r="F252" s="7"/>
     </row>
-    <row r="253" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B253" s="72" t="s">
+    <row r="253" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B253" s="71" t="s">
         <v>553</v>
       </c>
       <c r="C253" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D253" s="73" t="s">
+      <c r="D253" s="72" t="s">
         <v>554</v>
       </c>
       <c r="E253" s="37" t="s">
@@ -6989,14 +6941,14 @@
       </c>
       <c r="F253" s="7"/>
     </row>
-    <row r="254" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B254" s="72" t="s">
+    <row r="254" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B254" s="71" t="s">
         <v>559</v>
       </c>
       <c r="C254" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D254" s="73" t="s">
+      <c r="D254" s="72" t="s">
         <v>560</v>
       </c>
       <c r="E254" s="37" t="s">
@@ -7004,14 +6956,14 @@
       </c>
       <c r="F254" s="7"/>
     </row>
-    <row r="255" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B255" s="72" t="s">
+    <row r="255" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B255" s="71" t="s">
         <v>561</v>
       </c>
       <c r="C255" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D255" s="73" t="s">
+      <c r="D255" s="72" t="s">
         <v>562</v>
       </c>
       <c r="E255" s="37" t="s">
@@ -7019,14 +6971,14 @@
       </c>
       <c r="F255" s="7"/>
     </row>
-    <row r="256" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B256" s="72" t="s">
+    <row r="256" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B256" s="71" t="s">
         <v>563</v>
       </c>
       <c r="C256" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D256" s="73" t="s">
+      <c r="D256" s="72" t="s">
         <v>564</v>
       </c>
       <c r="E256" s="37" t="s">
@@ -7034,14 +6986,14 @@
       </c>
       <c r="F256" s="7"/>
     </row>
-    <row r="257" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B257" s="72" t="s">
+    <row r="257" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B257" s="71" t="s">
         <v>618</v>
       </c>
       <c r="C257" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D257" s="73" t="s">
+      <c r="D257" s="72" t="s">
         <v>634</v>
       </c>
       <c r="E257" s="37" t="s">
@@ -7049,14 +7001,14 @@
       </c>
       <c r="F257" s="7"/>
     </row>
-    <row r="258" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B258" s="72" t="s">
+    <row r="258" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B258" s="71" t="s">
         <v>619</v>
       </c>
       <c r="C258" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D258" s="73" t="s">
+      <c r="D258" s="72" t="s">
         <v>641</v>
       </c>
       <c r="E258" s="37" t="s">
@@ -7064,14 +7016,14 @@
       </c>
       <c r="F258" s="7"/>
     </row>
-    <row r="259" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B259" s="72" t="s">
+    <row r="259" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B259" s="71" t="s">
         <v>620</v>
       </c>
       <c r="C259" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D259" s="69" t="s">
+      <c r="D259" s="68" t="s">
         <v>635</v>
       </c>
       <c r="E259" s="37" t="s">
@@ -7079,659 +7031,659 @@
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B260" s="72" t="s">
+    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B260" s="71" t="s">
         <v>621</v>
       </c>
-      <c r="C260" s="75" t="s">
+      <c r="C260" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D260" s="69" t="s">
+      <c r="D260" s="68" t="s">
         <v>649</v>
       </c>
       <c r="E260" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F260" s="69"/>
-    </row>
-    <row r="261" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B261" s="72" t="s">
+      <c r="F260" s="68"/>
+    </row>
+    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B261" s="71" t="s">
         <v>622</v>
       </c>
-      <c r="C261" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D261" s="69" t="s">
+      <c r="C261" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D261" s="68" t="s">
         <v>636</v>
       </c>
       <c r="E261" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F261" s="69"/>
-    </row>
-    <row r="262" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B262" s="72" t="s">
+      <c r="F261" s="68"/>
+    </row>
+    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B262" s="71" t="s">
         <v>623</v>
       </c>
-      <c r="C262" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D262" s="69" t="s">
+      <c r="C262" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D262" s="68" t="s">
         <v>648</v>
       </c>
       <c r="E262" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F262" s="69"/>
-    </row>
-    <row r="263" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B263" s="72" t="s">
+      <c r="F262" s="68"/>
+    </row>
+    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B263" s="71" t="s">
         <v>624</v>
       </c>
-      <c r="C263" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D263" s="69" t="s">
+      <c r="C263" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D263" s="68" t="s">
         <v>637</v>
       </c>
       <c r="E263" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F263" s="69"/>
-    </row>
-    <row r="264" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B264" s="72" t="s">
+      <c r="F263" s="68"/>
+    </row>
+    <row r="264" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B264" s="71" t="s">
         <v>625</v>
       </c>
-      <c r="C264" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D264" s="69" t="s">
+      <c r="C264" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D264" s="68" t="s">
         <v>647</v>
       </c>
       <c r="E264" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F264" s="69"/>
-    </row>
-    <row r="265" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B265" s="72" t="s">
+      <c r="F264" s="68"/>
+    </row>
+    <row r="265" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B265" s="71" t="s">
         <v>626</v>
       </c>
-      <c r="C265" s="75" t="s">
+      <c r="C265" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D265" s="69" t="s">
+      <c r="D265" s="68" t="s">
         <v>638</v>
       </c>
       <c r="E265" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F265" s="69"/>
-    </row>
-    <row r="266" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B266" s="72" t="s">
+      <c r="F265" s="68"/>
+    </row>
+    <row r="266" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B266" s="71" t="s">
         <v>627</v>
       </c>
-      <c r="C266" s="75" t="s">
+      <c r="C266" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D266" s="69" t="s">
+      <c r="D266" s="68" t="s">
         <v>646</v>
       </c>
       <c r="E266" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F266" s="69"/>
-    </row>
-    <row r="267" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B267" s="72" t="s">
+      <c r="F266" s="68"/>
+    </row>
+    <row r="267" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B267" s="71" t="s">
         <v>628</v>
       </c>
-      <c r="C267" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D267" s="69" t="s">
+      <c r="C267" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D267" s="68" t="s">
         <v>639</v>
       </c>
       <c r="E267" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F267" s="69"/>
-    </row>
-    <row r="268" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B268" s="72" t="s">
+      <c r="F267" s="68"/>
+    </row>
+    <row r="268" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B268" s="71" t="s">
         <v>629</v>
       </c>
-      <c r="C268" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D268" s="69" t="s">
+      <c r="C268" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D268" s="68" t="s">
         <v>640</v>
       </c>
       <c r="E268" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F268" s="69"/>
-    </row>
-    <row r="269" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B269" s="72" t="s">
+      <c r="F268" s="68"/>
+    </row>
+    <row r="269" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B269" s="71" t="s">
         <v>630</v>
       </c>
-      <c r="C269" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D269" s="69" t="s">
+      <c r="C269" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D269" s="68" t="s">
         <v>642</v>
       </c>
       <c r="E269" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F269" s="69"/>
-    </row>
-    <row r="270" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B270" s="72" t="s">
+      <c r="F269" s="68"/>
+    </row>
+    <row r="270" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B270" s="71" t="s">
         <v>631</v>
       </c>
-      <c r="C270" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D270" s="69" t="s">
+      <c r="C270" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D270" s="68" t="s">
         <v>643</v>
       </c>
       <c r="E270" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F270" s="69"/>
-    </row>
-    <row r="271" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B271" s="72" t="s">
+      <c r="F270" s="68"/>
+    </row>
+    <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B271" s="71" t="s">
         <v>632</v>
       </c>
-      <c r="C271" s="75" t="s">
+      <c r="C271" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D271" s="69" t="s">
+      <c r="D271" s="68" t="s">
         <v>644</v>
       </c>
       <c r="E271" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F271" s="69"/>
-    </row>
-    <row r="272" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B272" s="72" t="s">
+      <c r="F271" s="68"/>
+    </row>
+    <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B272" s="71" t="s">
         <v>633</v>
       </c>
-      <c r="C272" s="75" t="s">
+      <c r="C272" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D272" s="69" t="s">
+      <c r="D272" s="68" t="s">
         <v>645</v>
       </c>
       <c r="E272" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F272" s="69"/>
-    </row>
-    <row r="273" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B273" s="72" t="s">
+      <c r="F272" s="68"/>
+    </row>
+    <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B273" s="71" t="s">
         <v>650</v>
       </c>
-      <c r="C273" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D273" s="69" t="s">
+      <c r="C273" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D273" s="68" t="s">
         <v>651</v>
       </c>
       <c r="E273" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F273" s="69"/>
-    </row>
-    <row r="274" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B274" s="72" t="s">
+      <c r="F273" s="68"/>
+    </row>
+    <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B274" s="71" t="s">
         <v>652</v>
       </c>
-      <c r="C274" s="75" t="s">
+      <c r="C274" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D274" s="69" t="s">
+      <c r="D274" s="68" t="s">
         <v>653</v>
       </c>
       <c r="E274" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F274" s="69"/>
-    </row>
-    <row r="275" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B275" s="72" t="s">
+      <c r="F274" s="68"/>
+    </row>
+    <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B275" s="71" t="s">
         <v>658</v>
       </c>
-      <c r="C275" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D275" s="69" t="s">
+      <c r="C275" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D275" s="68" t="s">
         <v>656</v>
       </c>
       <c r="E275" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F275" s="69"/>
-    </row>
-    <row r="276" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B276" s="72" t="s">
+      <c r="F275" s="68"/>
+    </row>
+    <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B276" s="71" t="s">
         <v>657</v>
       </c>
-      <c r="C276" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D276" s="69" t="s">
+      <c r="C276" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D276" s="68" t="s">
         <v>659</v>
       </c>
       <c r="E276" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F276" s="69"/>
-    </row>
-    <row r="277" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B277" s="72" t="s">
+      <c r="F276" s="68"/>
+    </row>
+    <row r="277" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B277" s="71" t="s">
         <v>654</v>
       </c>
-      <c r="C277" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D277" s="69" t="s">
+      <c r="C277" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D277" s="68" t="s">
         <v>661</v>
       </c>
       <c r="E277" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F277" s="69"/>
-    </row>
-    <row r="278" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B278" s="72" t="s">
+      <c r="F277" s="68"/>
+    </row>
+    <row r="278" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B278" s="71" t="s">
         <v>655</v>
       </c>
       <c r="C278" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D278" s="69" t="s">
+      <c r="D278" s="68" t="s">
         <v>662</v>
       </c>
       <c r="E278" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F278" s="69"/>
-    </row>
-    <row r="279" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B279" s="72" t="s">
+      <c r="F278" s="68"/>
+    </row>
+    <row r="279" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B279" s="71" t="s">
         <v>660</v>
       </c>
-      <c r="C279" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D279" s="69" t="s">
+      <c r="C279" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D279" s="68" t="s">
         <v>663</v>
       </c>
       <c r="E279" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F279" s="69"/>
-    </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B280" s="69" t="s">
+      <c r="F279" s="68"/>
+    </row>
+    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B280" s="68" t="s">
         <v>664</v>
       </c>
-      <c r="C280" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D280" s="69" t="s">
+      <c r="C280" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D280" s="68" t="s">
         <v>665</v>
       </c>
       <c r="E280" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F280" s="69"/>
-    </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B281" s="69" t="s">
+      <c r="F280" s="68"/>
+    </row>
+    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B281" s="68" t="s">
         <v>666</v>
       </c>
-      <c r="C281" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D281" s="69" t="s">
+      <c r="C281" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D281" s="68" t="s">
         <v>667</v>
       </c>
       <c r="E281" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F281" s="69"/>
-    </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B282" s="69" t="s">
+      <c r="F281" s="68"/>
+    </row>
+    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B282" s="68" t="s">
         <v>668</v>
       </c>
       <c r="C282" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D282" s="69" t="s">
+      <c r="D282" s="68" t="s">
         <v>669</v>
       </c>
       <c r="E282" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F282" s="69"/>
-    </row>
-    <row r="283" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B283" s="69" t="s">
+      <c r="F282" s="68"/>
+    </row>
+    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B283" s="68" t="s">
         <v>670</v>
       </c>
-      <c r="C283" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D283" s="69" t="s">
+      <c r="C283" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D283" s="68" t="s">
         <v>671</v>
       </c>
       <c r="E283" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F283" s="69"/>
-    </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B284" s="69" t="s">
+      <c r="F283" s="68"/>
+    </row>
+    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B284" s="68" t="s">
         <v>672</v>
       </c>
-      <c r="C284" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D284" s="69" t="s">
+      <c r="C284" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D284" s="68" t="s">
         <v>673</v>
       </c>
       <c r="E284" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F284" s="69"/>
-    </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B285" s="69" t="s">
+      <c r="F284" s="68"/>
+    </row>
+    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B285" s="68" t="s">
         <v>674</v>
       </c>
-      <c r="C285" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D285" s="69" t="s">
+      <c r="C285" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D285" s="68" t="s">
         <v>675</v>
       </c>
       <c r="E285" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F285" s="69"/>
-    </row>
-    <row r="286" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B286" s="69" t="s">
+      <c r="F285" s="68"/>
+    </row>
+    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B286" s="68" t="s">
         <v>676</v>
       </c>
-      <c r="C286" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D286" s="69" t="s">
+      <c r="C286" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D286" s="68" t="s">
         <v>677</v>
       </c>
       <c r="E286" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F286" s="69"/>
-    </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B287" s="69" t="s">
+      <c r="F286" s="68"/>
+    </row>
+    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B287" s="68" t="s">
         <v>678</v>
       </c>
-      <c r="C287" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D287" s="69" t="s">
+      <c r="C287" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D287" s="68" t="s">
         <v>679</v>
       </c>
       <c r="E287" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F287" s="69"/>
-    </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B288" s="69" t="s">
+      <c r="F287" s="68"/>
+    </row>
+    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B288" s="68" t="s">
         <v>680</v>
       </c>
-      <c r="C288" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D288" s="69" t="s">
+      <c r="C288" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D288" s="68" t="s">
         <v>681</v>
       </c>
       <c r="E288" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F288" s="69"/>
-    </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B289" s="69" t="s">
+      <c r="F288" s="68"/>
+    </row>
+    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B289" s="68" t="s">
         <v>682</v>
       </c>
-      <c r="C289" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D289" s="69" t="s">
+      <c r="C289" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D289" s="68" t="s">
         <v>683</v>
       </c>
       <c r="E289" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F289" s="69"/>
-    </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B290" s="69" t="s">
+      <c r="F289" s="68"/>
+    </row>
+    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B290" s="68" t="s">
         <v>684</v>
       </c>
-      <c r="C290" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D290" s="69" t="s">
+      <c r="C290" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D290" s="68" t="s">
         <v>685</v>
       </c>
       <c r="E290" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F290" s="69"/>
-    </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B291" s="69" t="s">
+      <c r="F290" s="68"/>
+    </row>
+    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B291" s="68" t="s">
         <v>686</v>
       </c>
       <c r="C291" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D291" s="69" t="s">
+      <c r="D291" s="68" t="s">
         <v>687</v>
       </c>
       <c r="E291" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F291" s="69"/>
-    </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B292" s="69" t="s">
+      <c r="F291" s="68"/>
+    </row>
+    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B292" s="68" t="s">
         <v>688</v>
       </c>
-      <c r="C292" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D292" s="69" t="s">
+      <c r="C292" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D292" s="68" t="s">
         <v>689</v>
       </c>
       <c r="E292" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F292" s="69"/>
-    </row>
-    <row r="293" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B293" s="69" t="s">
+      <c r="F292" s="68"/>
+    </row>
+    <row r="293" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B293" s="68" t="s">
         <v>690</v>
       </c>
-      <c r="C293" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D293" s="69" t="s">
+      <c r="C293" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D293" s="68" t="s">
         <v>691</v>
       </c>
       <c r="E293" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F293" s="69"/>
-    </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B294" s="69" t="s">
+      <c r="F293" s="68"/>
+    </row>
+    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B294" s="68" t="s">
         <v>692</v>
       </c>
-      <c r="C294" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D294" s="69" t="s">
+      <c r="C294" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D294" s="68" t="s">
         <v>693</v>
       </c>
       <c r="E294" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F294" s="69"/>
-    </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B295" s="69" t="s">
+      <c r="F294" s="68"/>
+    </row>
+    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B295" s="68" t="s">
         <v>694</v>
       </c>
-      <c r="C295" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D295" s="69" t="s">
+      <c r="C295" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D295" s="68" t="s">
         <v>695</v>
       </c>
       <c r="E295" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F295" s="69"/>
-    </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B296" s="69" t="s">
+      <c r="F295" s="68"/>
+    </row>
+    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B296" s="68" t="s">
         <v>696</v>
       </c>
-      <c r="C296" s="75" t="s">
+      <c r="C296" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D296" s="69" t="s">
+      <c r="D296" s="68" t="s">
         <v>697</v>
       </c>
       <c r="E296" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F296" s="69"/>
-    </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B297" s="69" t="s">
+      <c r="F296" s="68"/>
+    </row>
+    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B297" s="68" t="s">
         <v>698</v>
       </c>
-      <c r="C297" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D297" s="69" t="s">
+      <c r="C297" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D297" s="68" t="s">
         <v>699</v>
       </c>
       <c r="E297" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F297" s="69"/>
-    </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B298" s="69"/>
-      <c r="C298" s="69"/>
-      <c r="D298" s="69"/>
-      <c r="E298" s="69"/>
-      <c r="F298" s="69"/>
-    </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B299" s="69"/>
-      <c r="C299" s="69"/>
-      <c r="D299" s="69"/>
-      <c r="E299" s="69"/>
-      <c r="F299" s="69"/>
-    </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B300" s="69"/>
-      <c r="C300" s="69"/>
-      <c r="D300" s="69"/>
-      <c r="E300" s="69"/>
-      <c r="F300" s="69"/>
-    </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B301" s="69"/>
-      <c r="C301" s="69"/>
-      <c r="D301" s="69"/>
-      <c r="E301" s="69"/>
-      <c r="F301" s="69"/>
-    </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B302" s="69"/>
-      <c r="C302" s="69"/>
-      <c r="D302" s="69"/>
-      <c r="E302" s="69"/>
-      <c r="F302" s="69"/>
-    </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B303" s="69"/>
-      <c r="C303" s="69"/>
-      <c r="D303" s="69"/>
-      <c r="E303" s="69"/>
-      <c r="F303" s="69"/>
-    </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B304" s="69"/>
-      <c r="C304" s="69"/>
-      <c r="D304" s="69"/>
-      <c r="E304" s="69"/>
-      <c r="F304" s="69"/>
-    </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B305" s="69"/>
-      <c r="C305" s="69"/>
-      <c r="D305" s="69"/>
-      <c r="E305" s="69"/>
-      <c r="F305" s="69"/>
-    </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B306" s="69"/>
-      <c r="C306" s="69"/>
-      <c r="D306" s="69"/>
-      <c r="E306" s="69"/>
-      <c r="F306" s="69"/>
-    </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B307" s="69"/>
-      <c r="C307" s="69"/>
-      <c r="D307" s="69"/>
-      <c r="E307" s="69"/>
-      <c r="F307" s="69"/>
-    </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B308" s="69"/>
-      <c r="C308" s="69"/>
-      <c r="D308" s="69"/>
-      <c r="E308" s="69"/>
-      <c r="F308" s="69"/>
+      <c r="F297" s="68"/>
+    </row>
+    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B298" s="68"/>
+      <c r="C298" s="68"/>
+      <c r="D298" s="68"/>
+      <c r="E298" s="68"/>
+      <c r="F298" s="68"/>
+    </row>
+    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B299" s="68"/>
+      <c r="C299" s="68"/>
+      <c r="D299" s="68"/>
+      <c r="E299" s="68"/>
+      <c r="F299" s="68"/>
+    </row>
+    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B300" s="68"/>
+      <c r="C300" s="68"/>
+      <c r="D300" s="68"/>
+      <c r="E300" s="68"/>
+      <c r="F300" s="68"/>
+    </row>
+    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B301" s="68"/>
+      <c r="C301" s="68"/>
+      <c r="D301" s="68"/>
+      <c r="E301" s="68"/>
+      <c r="F301" s="68"/>
+    </row>
+    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B302" s="68"/>
+      <c r="C302" s="68"/>
+      <c r="D302" s="68"/>
+      <c r="E302" s="68"/>
+      <c r="F302" s="68"/>
+    </row>
+    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B303" s="68"/>
+      <c r="C303" s="68"/>
+      <c r="D303" s="68"/>
+      <c r="E303" s="68"/>
+      <c r="F303" s="68"/>
+    </row>
+    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B304" s="68"/>
+      <c r="C304" s="68"/>
+      <c r="D304" s="68"/>
+      <c r="E304" s="68"/>
+      <c r="F304" s="68"/>
+    </row>
+    <row r="305" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B305" s="68"/>
+      <c r="C305" s="68"/>
+      <c r="D305" s="68"/>
+      <c r="E305" s="68"/>
+      <c r="F305" s="68"/>
+    </row>
+    <row r="306" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B306" s="68"/>
+      <c r="C306" s="68"/>
+      <c r="D306" s="68"/>
+      <c r="E306" s="68"/>
+      <c r="F306" s="68"/>
+    </row>
+    <row r="307" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B307" s="68"/>
+      <c r="C307" s="68"/>
+      <c r="D307" s="68"/>
+      <c r="E307" s="68"/>
+      <c r="F307" s="68"/>
+    </row>
+    <row r="308" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B308" s="68"/>
+      <c r="C308" s="68"/>
+      <c r="D308" s="68"/>
+      <c r="E308" s="68"/>
+      <c r="F308" s="68"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F221">
     <sortCondition ref="B3:B221"/>
-    <sortCondition sortBy="cellColor" ref="C3:C221" dxfId="8"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C221" dxfId="7"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C221" dxfId="6"/>
+    <sortCondition sortBy="cellColor" ref="C3:C221" dxfId="2"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C221" dxfId="1"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C221" dxfId="0"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7747,191 +7699,191 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B2" s="71" t="s">
+    <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="70" t="s">
         <v>541</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="70" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="74" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="73" t="s">
         <v>565</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="74" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="73" t="s">
         <v>567</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="73" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="74" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="73" t="s">
         <v>569</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="73" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="74" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="73" t="s">
         <v>571</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="73" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="74" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="73" t="s">
         <v>573</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="73" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="74" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="73" t="s">
         <v>575</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="73" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="74" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="74" t="s">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="73" t="s">
         <v>580</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="73" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="74" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="73" t="s">
         <v>582</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="73" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="74" t="s">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="73" t="s">
         <v>584</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="73" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="74" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="73" t="s">
         <v>586</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="74" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="73" t="s">
         <v>588</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="74" t="s">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="73" t="s">
         <v>590</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="74" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="73" t="s">
         <v>592</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="74" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="73" t="s">
         <v>594</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="74" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="73" t="s">
         <v>596</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="73" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="74" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="73" t="s">
         <v>598</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="73" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="74" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="73" t="s">
         <v>600</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="74" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="73" t="s">
         <v>612</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="73" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="74" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="73" t="s">
         <v>614</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="70" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="69" t="s">
         <v>616</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="69" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7939,6 +7891,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8159,38 +8128,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8213,9 +8154,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated edges to reroute around preceding nodes in FLC tab
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cody3\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FEA936-4540-624D-AFDB-1B733173F474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0115417C-47D8-416E-BDDA-5566C7B3BC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -2232,7 +2232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2309,6 +2309,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB5E6A2"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -2501,14 +2507,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2636,8 +2643,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="4" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
@@ -3015,20 +3025,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="75" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="75" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="J103" sqref="J103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="255.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="255.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -3060,7 +3070,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -3075,7 +3085,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -3090,7 +3100,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3105,7 +3115,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3120,7 +3130,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3135,7 +3145,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -3150,7 +3160,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3165,7 +3175,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -3180,7 +3190,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -3195,7 +3205,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -3212,7 +3222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3227,7 +3237,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3242,7 +3252,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3257,7 +3267,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3272,7 +3282,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -3287,7 +3297,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -3302,7 +3312,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -3317,7 +3327,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -3332,7 +3342,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -3347,7 +3357,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3372,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3379,7 +3389,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -3396,7 +3406,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -3411,7 +3421,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -3428,7 +3438,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -3443,7 +3453,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3460,7 +3470,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -3475,7 +3485,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -3492,7 +3502,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -3507,7 +3517,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -3524,7 +3534,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -3539,7 +3549,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -3559,7 +3569,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -3574,7 +3584,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -3606,7 +3616,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -3623,7 +3633,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -3638,7 +3648,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -3655,7 +3665,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -3670,7 +3680,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -3687,7 +3697,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -3702,7 +3712,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3719,7 +3729,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3734,7 +3744,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3751,7 +3761,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3766,7 +3776,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3781,7 +3791,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3798,7 +3808,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3813,7 +3823,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3828,7 +3838,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3843,7 +3853,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3853,12 +3863,12 @@
       <c r="D54" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E54" s="28" t="s">
-        <v>15</v>
+      <c r="E54" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3873,7 +3883,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3890,7 +3900,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3905,7 +3915,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3920,7 +3930,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3935,7 +3945,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -3945,12 +3955,12 @@
       <c r="D60" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E60" s="28" t="s">
-        <v>15</v>
+      <c r="E60" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -3965,7 +3975,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -3982,7 +3992,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -3997,7 +4007,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -4012,7 +4022,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -4027,7 +4037,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -4037,12 +4047,12 @@
       <c r="D66" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E66" s="28" t="s">
-        <v>15</v>
+      <c r="E66" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -4057,7 +4067,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -4074,7 +4084,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -4089,7 +4099,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -4104,7 +4114,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -4119,7 +4129,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -4129,12 +4139,12 @@
       <c r="D72" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E72" s="28" t="s">
-        <v>15</v>
+      <c r="E72" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -4149,7 +4159,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -4166,7 +4176,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -4181,7 +4191,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -4196,7 +4206,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -4211,7 +4221,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -4221,12 +4231,12 @@
       <c r="D78" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E78" s="28" t="s">
-        <v>15</v>
+      <c r="E78" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -4241,7 +4251,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -4258,7 +4268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -4273,7 +4283,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -4288,7 +4298,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -4303,7 +4313,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -4313,12 +4323,12 @@
       <c r="D84" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E84" s="28" t="s">
-        <v>15</v>
+      <c r="E84" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -4333,7 +4343,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -4350,7 +4360,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -4365,7 +4375,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -4380,7 +4390,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -4395,7 +4405,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -4405,12 +4415,12 @@
       <c r="D90" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="28" t="s">
-        <v>15</v>
+      <c r="E90" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -4425,7 +4435,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -4442,7 +4452,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
         <v>211</v>
       </c>
@@ -4457,7 +4467,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94" s="3" t="s">
         <v>213</v>
       </c>
@@ -4472,7 +4482,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95" s="3" t="s">
         <v>215</v>
       </c>
@@ -4487,7 +4497,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" s="3" t="s">
         <v>217</v>
       </c>
@@ -4502,7 +4512,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B97" s="3" t="s">
         <v>219</v>
       </c>
@@ -4517,7 +4527,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B98" s="3" t="s">
         <v>221</v>
       </c>
@@ -4532,7 +4542,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B99" s="3" t="s">
         <v>223</v>
       </c>
@@ -4547,7 +4557,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B100" s="3" t="s">
         <v>225</v>
       </c>
@@ -4557,12 +4567,12 @@
       <c r="D100" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E100" s="28" t="s">
-        <v>15</v>
+      <c r="E100" s="79" t="s">
+        <v>489</v>
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B101" s="3" t="s">
         <v>227</v>
       </c>
@@ -4572,12 +4582,12 @@
       <c r="D101" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E101" s="28" t="s">
-        <v>15</v>
+      <c r="E101" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B102" s="3" t="s">
         <v>229</v>
       </c>
@@ -4592,7 +4602,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -4607,7 +4617,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B104" s="60" t="s">
         <v>700</v>
       </c>
@@ -4622,7 +4632,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B105" s="60" t="s">
         <v>702</v>
       </c>
@@ -4637,7 +4647,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B106" s="20" t="s">
         <v>233</v>
       </c>
@@ -4652,7 +4662,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B107" s="20" t="s">
         <v>235</v>
       </c>
@@ -4667,7 +4677,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B108" s="20" t="s">
         <v>237</v>
       </c>
@@ -4682,7 +4692,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B109" s="20" t="s">
         <v>239</v>
       </c>
@@ -4697,7 +4707,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B110" s="20" t="s">
         <v>241</v>
       </c>
@@ -4712,7 +4722,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B111" s="20" t="s">
         <v>243</v>
       </c>
@@ -4729,7 +4739,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B112" s="20" t="s">
         <v>245</v>
       </c>
@@ -4744,7 +4754,7 @@
       </c>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B113" s="20" t="s">
         <v>577</v>
       </c>
@@ -4759,7 +4769,7 @@
       </c>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B114" s="20" t="s">
         <v>247</v>
       </c>
@@ -4774,7 +4784,7 @@
       </c>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B115" s="7" t="s">
         <v>251</v>
       </c>
@@ -4791,7 +4801,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B116" s="7" t="s">
         <v>253</v>
       </c>
@@ -4808,7 +4818,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B117" s="7" t="s">
         <v>255</v>
       </c>
@@ -4825,7 +4835,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B118" s="7" t="s">
         <v>257</v>
       </c>
@@ -4842,7 +4852,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B119" s="7" t="s">
         <v>259</v>
       </c>
@@ -4859,7 +4869,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B120" s="7" t="s">
         <v>262</v>
       </c>
@@ -4876,7 +4886,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B121" s="7" t="s">
         <v>265</v>
       </c>
@@ -4891,7 +4901,7 @@
       </c>
       <c r="F121" s="7"/>
     </row>
-    <row r="122" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B122" s="7" t="s">
         <v>266</v>
       </c>
@@ -4908,7 +4918,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="123" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B123" s="7" t="s">
         <v>269</v>
       </c>
@@ -4925,7 +4935,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B124" s="7" t="s">
         <v>271</v>
       </c>
@@ -4942,7 +4952,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B125" s="7" t="s">
         <v>274</v>
       </c>
@@ -4959,7 +4969,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B126" s="3" t="s">
         <v>277</v>
       </c>
@@ -4976,7 +4986,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B127" s="3" t="s">
         <v>278</v>
       </c>
@@ -4991,7 +5001,7 @@
       </c>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B128" s="3" t="s">
         <v>280</v>
       </c>
@@ -5006,7 +5016,7 @@
       </c>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B129" s="3" t="s">
         <v>282</v>
       </c>
@@ -5021,7 +5031,7 @@
       </c>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B130" s="3" t="s">
         <v>284</v>
       </c>
@@ -5038,7 +5048,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B131" s="3" t="s">
         <v>286</v>
       </c>
@@ -5055,7 +5065,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="132" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B132" s="3" t="s">
         <v>289</v>
       </c>
@@ -5070,7 +5080,7 @@
       </c>
       <c r="F132" s="7"/>
     </row>
-    <row r="133" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B133" s="3" t="s">
         <v>291</v>
       </c>
@@ -5087,7 +5097,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="134" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B134" s="3" t="s">
         <v>293</v>
       </c>
@@ -5104,7 +5114,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B135" s="3" t="s">
         <v>296</v>
       </c>
@@ -5121,7 +5131,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B136" s="3" t="s">
         <v>508</v>
       </c>
@@ -5136,7 +5146,7 @@
       </c>
       <c r="F136" s="7"/>
     </row>
-    <row r="137" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B137" s="3" t="s">
         <v>510</v>
       </c>
@@ -5151,7 +5161,7 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B138" s="60" t="s">
         <v>512</v>
       </c>
@@ -5166,7 +5176,7 @@
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B139" s="60" t="s">
         <v>513</v>
       </c>
@@ -5181,7 +5191,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B140" s="3" t="s">
         <v>299</v>
       </c>
@@ -5198,7 +5208,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B141" s="3" t="s">
         <v>301</v>
       </c>
@@ -5215,7 +5225,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B142" s="3" t="s">
         <v>303</v>
       </c>
@@ -5232,7 +5242,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B143" s="3" t="s">
         <v>305</v>
       </c>
@@ -5249,7 +5259,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B144" s="3" t="s">
         <v>307</v>
       </c>
@@ -5266,7 +5276,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B145" s="3" t="s">
         <v>309</v>
       </c>
@@ -5283,7 +5293,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B146" s="3" t="s">
         <v>311</v>
       </c>
@@ -5298,7 +5308,7 @@
       </c>
       <c r="F146" s="7"/>
     </row>
-    <row r="147" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B147" s="3" t="s">
         <v>313</v>
       </c>
@@ -5315,7 +5325,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="148" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B148" s="3" t="s">
         <v>315</v>
       </c>
@@ -5332,7 +5342,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B149" s="3" t="s">
         <v>317</v>
       </c>
@@ -5349,7 +5359,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B150" s="3" t="s">
         <v>319</v>
       </c>
@@ -5364,7 +5374,7 @@
       </c>
       <c r="F150" s="7"/>
     </row>
-    <row r="151" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B151" s="20" t="s">
         <v>321</v>
       </c>
@@ -5381,7 +5391,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="152" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B152" s="20" t="s">
         <v>323</v>
       </c>
@@ -5396,7 +5406,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B153" s="20" t="s">
         <v>325</v>
       </c>
@@ -5411,7 +5421,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B154" s="20" t="s">
         <v>327</v>
       </c>
@@ -5426,7 +5436,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B155" s="20" t="s">
         <v>329</v>
       </c>
@@ -5441,7 +5451,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B156" s="20" t="s">
         <v>331</v>
       </c>
@@ -5456,7 +5466,7 @@
       </c>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B157" s="20" t="s">
         <v>333</v>
       </c>
@@ -5471,7 +5481,7 @@
       </c>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B158" s="20" t="s">
         <v>335</v>
       </c>
@@ -5486,7 +5496,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B159" s="20" t="s">
         <v>337</v>
       </c>
@@ -5501,7 +5511,7 @@
       </c>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B160" s="20" t="s">
         <v>339</v>
       </c>
@@ -5516,7 +5526,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B161" s="20" t="s">
         <v>341</v>
       </c>
@@ -5533,7 +5543,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="162" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B162" s="20" t="s">
         <v>343</v>
       </c>
@@ -5548,7 +5558,7 @@
       </c>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B163" s="9" t="s">
         <v>345</v>
       </c>
@@ -5565,7 +5575,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="164" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B164" s="9" t="s">
         <v>347</v>
       </c>
@@ -5580,7 +5590,7 @@
       </c>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B165" s="9" t="s">
         <v>348</v>
       </c>
@@ -5597,7 +5607,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="166" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B166" s="9" t="s">
         <v>350</v>
       </c>
@@ -5614,7 +5624,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="167" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B167" s="9" t="s">
         <v>351</v>
       </c>
@@ -5629,7 +5639,7 @@
       </c>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B168" s="9" t="s">
         <v>353</v>
       </c>
@@ -5646,7 +5656,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="169" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B169" s="9" t="s">
         <v>355</v>
       </c>
@@ -5663,7 +5673,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="170" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B170" s="9" t="s">
         <v>357</v>
       </c>
@@ -5680,7 +5690,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="171" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B171" s="9" t="s">
         <v>359</v>
       </c>
@@ -5697,7 +5707,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="172" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B172" s="9" t="s">
         <v>361</v>
       </c>
@@ -5712,7 +5722,7 @@
       </c>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B173" s="9" t="s">
         <v>363</v>
       </c>
@@ -5729,7 +5739,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="174" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B174" s="9" t="s">
         <v>365</v>
       </c>
@@ -5746,7 +5756,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B175" s="10" t="s">
         <v>367</v>
       </c>
@@ -5763,7 +5773,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B176" s="10" t="s">
         <v>369</v>
       </c>
@@ -5780,7 +5790,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B177" s="10" t="s">
         <v>371</v>
       </c>
@@ -5795,7 +5805,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B178" s="10" t="s">
         <v>373</v>
       </c>
@@ -5810,7 +5820,7 @@
       </c>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B179" s="21" t="s">
         <v>375</v>
       </c>
@@ -5825,7 +5835,7 @@
       </c>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B180" s="21" t="s">
         <v>377</v>
       </c>
@@ -5840,7 +5850,7 @@
       </c>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B181" s="21" t="s">
         <v>379</v>
       </c>
@@ -5855,7 +5865,7 @@
       </c>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B182" s="21" t="s">
         <v>381</v>
       </c>
@@ -5870,7 +5880,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B183" s="21" t="s">
         <v>383</v>
       </c>
@@ -5885,7 +5895,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B184" s="21" t="s">
         <v>385</v>
       </c>
@@ -5900,7 +5910,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B185" s="3" t="s">
         <v>387</v>
       </c>
@@ -5915,7 +5925,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B186" s="3" t="s">
         <v>389</v>
       </c>
@@ -5930,7 +5940,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B187" s="3" t="s">
         <v>391</v>
       </c>
@@ -5945,7 +5955,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B188" s="3" t="s">
         <v>393</v>
       </c>
@@ -5960,7 +5970,7 @@
       </c>
       <c r="F188" s="7"/>
     </row>
-    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B189" s="21" t="s">
         <v>395</v>
       </c>
@@ -5975,7 +5985,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B190" s="3" t="s">
         <v>397</v>
       </c>
@@ -5990,7 +6000,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B191" s="3" t="s">
         <v>399</v>
       </c>
@@ -6005,7 +6015,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B192" s="21" t="s">
         <v>401</v>
       </c>
@@ -6022,7 +6032,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B193" s="3" t="s">
         <v>403</v>
       </c>
@@ -6037,7 +6047,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B194" s="3" t="s">
         <v>405</v>
       </c>
@@ -6054,7 +6064,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B195" s="3" t="s">
         <v>407</v>
       </c>
@@ -6069,7 +6079,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B196" s="3" t="s">
         <v>409</v>
       </c>
@@ -6084,7 +6094,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B197" s="3" t="s">
         <v>411</v>
       </c>
@@ -6099,7 +6109,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B198" s="3" t="s">
         <v>413</v>
       </c>
@@ -6114,7 +6124,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B199" s="3" t="s">
         <v>415</v>
       </c>
@@ -6129,7 +6139,7 @@
       </c>
       <c r="F199" s="7"/>
     </row>
-    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B200" s="3" t="s">
         <v>417</v>
       </c>
@@ -6144,7 +6154,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B201" s="3" t="s">
         <v>419</v>
       </c>
@@ -6159,7 +6169,7 @@
       </c>
       <c r="F201" s="7"/>
     </row>
-    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B202" s="3" t="s">
         <v>421</v>
       </c>
@@ -6174,7 +6184,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B203" s="3" t="s">
         <v>423</v>
       </c>
@@ -6189,7 +6199,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B204" s="3" t="s">
         <v>425</v>
       </c>
@@ -6204,7 +6214,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B205" s="3" t="s">
         <v>427</v>
       </c>
@@ -6219,7 +6229,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B206" s="3" t="s">
         <v>429</v>
       </c>
@@ -6234,7 +6244,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B207" s="3" t="s">
         <v>431</v>
       </c>
@@ -6249,7 +6259,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B208" s="21" t="s">
         <v>433</v>
       </c>
@@ -6264,7 +6274,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B209" s="21" t="s">
         <v>435</v>
       </c>
@@ -6279,7 +6289,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B210" s="21" t="s">
         <v>437</v>
       </c>
@@ -6294,7 +6304,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B211" s="12" t="s">
         <v>439</v>
       </c>
@@ -6309,7 +6319,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B212" s="12" t="s">
         <v>441</v>
       </c>
@@ -6324,7 +6334,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B213" s="12" t="s">
         <v>443</v>
       </c>
@@ -6339,7 +6349,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B214" s="12" t="s">
         <v>445</v>
       </c>
@@ -6354,7 +6364,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B215" s="21" t="s">
         <v>447</v>
       </c>
@@ -6371,7 +6381,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="216" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B216" s="21" t="s">
         <v>449</v>
       </c>
@@ -6386,7 +6396,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B217" s="21" t="s">
         <v>451</v>
       </c>
@@ -6401,7 +6411,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B218" s="21" t="s">
         <v>453</v>
       </c>
@@ -6416,7 +6426,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B219" s="21" t="s">
         <v>455</v>
       </c>
@@ -6431,7 +6441,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B220" s="21" t="s">
         <v>457</v>
       </c>
@@ -6446,7 +6456,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B221" s="21" t="s">
         <v>459</v>
       </c>
@@ -6461,7 +6471,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B222" s="21" t="s">
         <v>461</v>
       </c>
@@ -6476,7 +6486,7 @@
       </c>
       <c r="F222" s="7"/>
     </row>
-    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B223" s="21" t="s">
         <v>463</v>
       </c>
@@ -6491,7 +6501,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B224" s="12" t="s">
         <v>465</v>
       </c>
@@ -6506,7 +6516,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B225" s="12" t="s">
         <v>467</v>
       </c>
@@ -6521,7 +6531,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B226" s="12" t="s">
         <v>469</v>
       </c>
@@ -6536,7 +6546,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B227" s="12" t="s">
         <v>471</v>
       </c>
@@ -6551,7 +6561,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B228" s="12" t="s">
         <v>473</v>
       </c>
@@ -6566,7 +6576,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B229" s="12" t="s">
         <v>475</v>
       </c>
@@ -6581,7 +6591,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B230" s="12" t="s">
         <v>477</v>
       </c>
@@ -6596,7 +6606,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B231" s="12" t="s">
         <v>479</v>
       </c>
@@ -6611,7 +6621,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B232" s="12" t="s">
         <v>481</v>
       </c>
@@ -6626,7 +6636,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B233" s="12" t="s">
         <v>483</v>
       </c>
@@ -6641,7 +6651,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B234" s="68" t="s">
         <v>602</v>
       </c>
@@ -6656,7 +6666,7 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B235" s="68" t="s">
         <v>604</v>
       </c>
@@ -6671,7 +6681,7 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B236" s="68" t="s">
         <v>529</v>
       </c>
@@ -6686,7 +6696,7 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B237" s="68" t="s">
         <v>531</v>
       </c>
@@ -6701,7 +6711,7 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B238" s="68" t="s">
         <v>533</v>
       </c>
@@ -6716,7 +6726,7 @@
       </c>
       <c r="F238" s="7"/>
     </row>
-    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B239" s="68" t="s">
         <v>606</v>
       </c>
@@ -6731,7 +6741,7 @@
       </c>
       <c r="F239" s="7"/>
     </row>
-    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B240" s="68" t="s">
         <v>608</v>
       </c>
@@ -6746,7 +6756,7 @@
       </c>
       <c r="F240" s="7"/>
     </row>
-    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B241" s="68" t="s">
         <v>527</v>
       </c>
@@ -6761,7 +6771,7 @@
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B242" s="68" t="s">
         <v>535</v>
       </c>
@@ -6776,7 +6786,7 @@
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B243" s="68" t="s">
         <v>610</v>
       </c>
@@ -6791,7 +6801,7 @@
       </c>
       <c r="F243" s="7"/>
     </row>
-    <row r="244" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B244" s="68" t="s">
         <v>537</v>
       </c>
@@ -6806,7 +6816,7 @@
       </c>
       <c r="F244" s="7"/>
     </row>
-    <row r="245" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B245" s="68" t="s">
         <v>539</v>
       </c>
@@ -6821,7 +6831,7 @@
       </c>
       <c r="F245" s="7"/>
     </row>
-    <row r="246" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B246" s="71" t="s">
         <v>543</v>
       </c>
@@ -6836,7 +6846,7 @@
       </c>
       <c r="F246" s="7"/>
     </row>
-    <row r="247" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B247" s="71" t="s">
         <v>545</v>
       </c>
@@ -6851,7 +6861,7 @@
       </c>
       <c r="F247" s="7"/>
     </row>
-    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B248" s="71" t="s">
         <v>549</v>
       </c>
@@ -6866,7 +6876,7 @@
       </c>
       <c r="F248" s="7"/>
     </row>
-    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B249" s="71" t="s">
         <v>555</v>
       </c>
@@ -6881,7 +6891,7 @@
       </c>
       <c r="F249" s="7"/>
     </row>
-    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B250" s="71" t="s">
         <v>557</v>
       </c>
@@ -6896,7 +6906,7 @@
       </c>
       <c r="F250" s="7"/>
     </row>
-    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B251" s="71" t="s">
         <v>547</v>
       </c>
@@ -6911,7 +6921,7 @@
       </c>
       <c r="F251" s="7"/>
     </row>
-    <row r="252" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B252" s="71" t="s">
         <v>551</v>
       </c>
@@ -6926,7 +6936,7 @@
       </c>
       <c r="F252" s="7"/>
     </row>
-    <row r="253" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B253" s="71" t="s">
         <v>553</v>
       </c>
@@ -6941,7 +6951,7 @@
       </c>
       <c r="F253" s="7"/>
     </row>
-    <row r="254" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B254" s="71" t="s">
         <v>559</v>
       </c>
@@ -6956,7 +6966,7 @@
       </c>
       <c r="F254" s="7"/>
     </row>
-    <row r="255" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B255" s="71" t="s">
         <v>561</v>
       </c>
@@ -6971,7 +6981,7 @@
       </c>
       <c r="F255" s="7"/>
     </row>
-    <row r="256" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B256" s="71" t="s">
         <v>563</v>
       </c>
@@ -6986,7 +6996,7 @@
       </c>
       <c r="F256" s="7"/>
     </row>
-    <row r="257" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B257" s="71" t="s">
         <v>618</v>
       </c>
@@ -7001,7 +7011,7 @@
       </c>
       <c r="F257" s="7"/>
     </row>
-    <row r="258" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B258" s="71" t="s">
         <v>619</v>
       </c>
@@ -7016,7 +7026,7 @@
       </c>
       <c r="F258" s="7"/>
     </row>
-    <row r="259" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B259" s="71" t="s">
         <v>620</v>
       </c>
@@ -7031,7 +7041,7 @@
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B260" s="71" t="s">
         <v>621</v>
       </c>
@@ -7046,7 +7056,7 @@
       </c>
       <c r="F260" s="68"/>
     </row>
-    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B261" s="71" t="s">
         <v>622</v>
       </c>
@@ -7061,7 +7071,7 @@
       </c>
       <c r="F261" s="68"/>
     </row>
-    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B262" s="71" t="s">
         <v>623</v>
       </c>
@@ -7076,7 +7086,7 @@
       </c>
       <c r="F262" s="68"/>
     </row>
-    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B263" s="71" t="s">
         <v>624</v>
       </c>
@@ -7091,7 +7101,7 @@
       </c>
       <c r="F263" s="68"/>
     </row>
-    <row r="264" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B264" s="71" t="s">
         <v>625</v>
       </c>
@@ -7106,7 +7116,7 @@
       </c>
       <c r="F264" s="68"/>
     </row>
-    <row r="265" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B265" s="71" t="s">
         <v>626</v>
       </c>
@@ -7121,7 +7131,7 @@
       </c>
       <c r="F265" s="68"/>
     </row>
-    <row r="266" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B266" s="71" t="s">
         <v>627</v>
       </c>
@@ -7136,7 +7146,7 @@
       </c>
       <c r="F266" s="68"/>
     </row>
-    <row r="267" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B267" s="71" t="s">
         <v>628</v>
       </c>
@@ -7151,7 +7161,7 @@
       </c>
       <c r="F267" s="68"/>
     </row>
-    <row r="268" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B268" s="71" t="s">
         <v>629</v>
       </c>
@@ -7166,7 +7176,7 @@
       </c>
       <c r="F268" s="68"/>
     </row>
-    <row r="269" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B269" s="71" t="s">
         <v>630</v>
       </c>
@@ -7181,7 +7191,7 @@
       </c>
       <c r="F269" s="68"/>
     </row>
-    <row r="270" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B270" s="71" t="s">
         <v>631</v>
       </c>
@@ -7196,7 +7206,7 @@
       </c>
       <c r="F270" s="68"/>
     </row>
-    <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B271" s="71" t="s">
         <v>632</v>
       </c>
@@ -7211,7 +7221,7 @@
       </c>
       <c r="F271" s="68"/>
     </row>
-    <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B272" s="71" t="s">
         <v>633</v>
       </c>
@@ -7226,7 +7236,7 @@
       </c>
       <c r="F272" s="68"/>
     </row>
-    <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B273" s="71" t="s">
         <v>650</v>
       </c>
@@ -7241,7 +7251,7 @@
       </c>
       <c r="F273" s="68"/>
     </row>
-    <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B274" s="71" t="s">
         <v>652</v>
       </c>
@@ -7256,7 +7266,7 @@
       </c>
       <c r="F274" s="68"/>
     </row>
-    <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B275" s="71" t="s">
         <v>658</v>
       </c>
@@ -7271,7 +7281,7 @@
       </c>
       <c r="F275" s="68"/>
     </row>
-    <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B276" s="71" t="s">
         <v>657</v>
       </c>
@@ -7286,7 +7296,7 @@
       </c>
       <c r="F276" s="68"/>
     </row>
-    <row r="277" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B277" s="71" t="s">
         <v>654</v>
       </c>
@@ -7301,7 +7311,7 @@
       </c>
       <c r="F277" s="68"/>
     </row>
-    <row r="278" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B278" s="71" t="s">
         <v>655</v>
       </c>
@@ -7316,7 +7326,7 @@
       </c>
       <c r="F278" s="68"/>
     </row>
-    <row r="279" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B279" s="71" t="s">
         <v>660</v>
       </c>
@@ -7331,7 +7341,7 @@
       </c>
       <c r="F279" s="68"/>
     </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B280" s="68" t="s">
         <v>664</v>
       </c>
@@ -7346,7 +7356,7 @@
       </c>
       <c r="F280" s="68"/>
     </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B281" s="68" t="s">
         <v>666</v>
       </c>
@@ -7361,7 +7371,7 @@
       </c>
       <c r="F281" s="68"/>
     </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B282" s="68" t="s">
         <v>668</v>
       </c>
@@ -7376,7 +7386,7 @@
       </c>
       <c r="F282" s="68"/>
     </row>
-    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B283" s="68" t="s">
         <v>670</v>
       </c>
@@ -7391,7 +7401,7 @@
       </c>
       <c r="F283" s="68"/>
     </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B284" s="68" t="s">
         <v>672</v>
       </c>
@@ -7406,7 +7416,7 @@
       </c>
       <c r="F284" s="68"/>
     </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B285" s="68" t="s">
         <v>674</v>
       </c>
@@ -7421,7 +7431,7 @@
       </c>
       <c r="F285" s="68"/>
     </row>
-    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B286" s="68" t="s">
         <v>676</v>
       </c>
@@ -7436,7 +7446,7 @@
       </c>
       <c r="F286" s="68"/>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B287" s="68" t="s">
         <v>678</v>
       </c>
@@ -7451,7 +7461,7 @@
       </c>
       <c r="F287" s="68"/>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B288" s="68" t="s">
         <v>680</v>
       </c>
@@ -7466,7 +7476,7 @@
       </c>
       <c r="F288" s="68"/>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B289" s="68" t="s">
         <v>682</v>
       </c>
@@ -7481,7 +7491,7 @@
       </c>
       <c r="F289" s="68"/>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B290" s="68" t="s">
         <v>684</v>
       </c>
@@ -7496,7 +7506,7 @@
       </c>
       <c r="F290" s="68"/>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B291" s="68" t="s">
         <v>686</v>
       </c>
@@ -7511,7 +7521,7 @@
       </c>
       <c r="F291" s="68"/>
     </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B292" s="68" t="s">
         <v>688</v>
       </c>
@@ -7526,7 +7536,7 @@
       </c>
       <c r="F292" s="68"/>
     </row>
-    <row r="293" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B293" s="68" t="s">
         <v>690</v>
       </c>
@@ -7541,7 +7551,7 @@
       </c>
       <c r="F293" s="68"/>
     </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B294" s="68" t="s">
         <v>692</v>
       </c>
@@ -7556,7 +7566,7 @@
       </c>
       <c r="F294" s="68"/>
     </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B295" s="68" t="s">
         <v>694</v>
       </c>
@@ -7571,7 +7581,7 @@
       </c>
       <c r="F295" s="68"/>
     </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B296" s="68" t="s">
         <v>696</v>
       </c>
@@ -7586,7 +7596,7 @@
       </c>
       <c r="F296" s="68"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B297" s="68" t="s">
         <v>698</v>
       </c>
@@ -7601,77 +7611,77 @@
       </c>
       <c r="F297" s="68"/>
     </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B298" s="68"/>
       <c r="C298" s="68"/>
       <c r="D298" s="68"/>
       <c r="E298" s="68"/>
       <c r="F298" s="68"/>
     </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B299" s="68"/>
       <c r="C299" s="68"/>
       <c r="D299" s="68"/>
       <c r="E299" s="68"/>
       <c r="F299" s="68"/>
     </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B300" s="68"/>
       <c r="C300" s="68"/>
       <c r="D300" s="68"/>
       <c r="E300" s="68"/>
       <c r="F300" s="68"/>
     </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B301" s="68"/>
       <c r="C301" s="68"/>
       <c r="D301" s="68"/>
       <c r="E301" s="68"/>
       <c r="F301" s="68"/>
     </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B302" s="68"/>
       <c r="C302" s="68"/>
       <c r="D302" s="68"/>
       <c r="E302" s="68"/>
       <c r="F302" s="68"/>
     </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B303" s="68"/>
       <c r="C303" s="68"/>
       <c r="D303" s="68"/>
       <c r="E303" s="68"/>
       <c r="F303" s="68"/>
     </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B304" s="68"/>
       <c r="C304" s="68"/>
       <c r="D304" s="68"/>
       <c r="E304" s="68"/>
       <c r="F304" s="68"/>
     </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B305" s="68"/>
       <c r="C305" s="68"/>
       <c r="D305" s="68"/>
       <c r="E305" s="68"/>
       <c r="F305" s="68"/>
     </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B306" s="68"/>
       <c r="C306" s="68"/>
       <c r="D306" s="68"/>
       <c r="E306" s="68"/>
       <c r="F306" s="68"/>
     </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B307" s="68"/>
       <c r="C307" s="68"/>
       <c r="D307" s="68"/>
       <c r="E307" s="68"/>
       <c r="F307" s="68"/>
     </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B308" s="68"/>
       <c r="C308" s="68"/>
       <c r="D308" s="68"/>
@@ -7699,13 +7709,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="55.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="17" x14ac:dyDescent="0.4">
       <c r="B2" s="70" t="s">
         <v>541</v>
       </c>
@@ -7713,7 +7723,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="73" t="s">
         <v>565</v>
       </c>
@@ -7721,7 +7731,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="73" t="s">
         <v>567</v>
       </c>
@@ -7729,7 +7739,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="73" t="s">
         <v>569</v>
       </c>
@@ -7737,7 +7747,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="73" t="s">
         <v>571</v>
       </c>
@@ -7745,7 +7755,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="73" t="s">
         <v>573</v>
       </c>
@@ -7753,7 +7763,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="73" t="s">
         <v>575</v>
       </c>
@@ -7761,7 +7771,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="73" t="s">
         <v>578</v>
       </c>
@@ -7769,7 +7779,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" s="73" t="s">
         <v>580</v>
       </c>
@@ -7777,7 +7787,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" s="73" t="s">
         <v>582</v>
       </c>
@@ -7785,7 +7795,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="73" t="s">
         <v>584</v>
       </c>
@@ -7793,7 +7803,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" s="73" t="s">
         <v>586</v>
       </c>
@@ -7801,7 +7811,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" s="73" t="s">
         <v>588</v>
       </c>
@@ -7809,7 +7819,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B15" s="73" t="s">
         <v>590</v>
       </c>
@@ -7817,7 +7827,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B16" s="73" t="s">
         <v>592</v>
       </c>
@@ -7825,7 +7835,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="73" t="s">
         <v>594</v>
       </c>
@@ -7833,7 +7843,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="73" t="s">
         <v>596</v>
       </c>
@@ -7841,7 +7851,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="73" t="s">
         <v>598</v>
       </c>
@@ -7849,7 +7859,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="73" t="s">
         <v>600</v>
       </c>
@@ -7857,7 +7867,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="73" t="s">
         <v>612</v>
       </c>
@@ -7865,7 +7875,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="73" t="s">
         <v>614</v>
       </c>
@@ -7873,7 +7883,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="69" t="s">
         <v>616</v>
       </c>
@@ -7881,7 +7891,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="69"/>
       <c r="C24" s="69"/>
     </row>
@@ -7891,23 +7901,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8128,10 +8121,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8154,20 +8175,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reordered Flight Control Requirements
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F9E2C4-FB60-44A2-93C5-C813CCE85537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2285A6AE-F3B1-4431-A241-604DD6065470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -2703,175 +2703,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3242,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="71" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="71" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="F309" sqref="F309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4652,7 +4484,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -4669,153 +4501,153 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E93" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E96" s="79" t="s">
+        <v>489</v>
+      </c>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="C97" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E97" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" s="7"/>
+    </row>
+    <row r="98" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C93" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="2" t="s">
+      <c r="C98" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E93" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F93" s="7"/>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B94" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E94" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F94" s="7"/>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B95" s="3" t="s">
+      <c r="E98" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="99" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C95" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="2" t="s">
+      <c r="C99" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E95" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F95" s="7"/>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C96" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E96" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F96" s="7"/>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B97" s="3" t="s">
+      <c r="E99" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="7"/>
+    </row>
+    <row r="100" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" s="2" t="s">
+      <c r="C100" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E97" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F97" s="7"/>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B98" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C98" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F98" s="7"/>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B99" s="3" t="s">
+      <c r="E100" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="7"/>
+    </row>
+    <row r="101" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C99" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" s="2" t="s">
+      <c r="C101" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E99" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F99" s="7"/>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B100" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="C100" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E100" s="79" t="s">
-        <v>489</v>
-      </c>
-      <c r="F100" s="7"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B101" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C101" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E101" s="80" t="s">
-        <v>489</v>
-      </c>
-      <c r="F101" s="7"/>
+      <c r="E101" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F101" s="68"/>
     </row>
     <row r="102" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B102" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C102" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E102" s="28" t="s">
-        <v>15</v>
+        <v>228</v>
+      </c>
+      <c r="E102" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F102" s="7"/>
     </row>
@@ -8013,9 +7845,9 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F228">
     <sortCondition ref="B3:B228"/>
-    <sortCondition sortBy="cellColor" ref="C3:C228" dxfId="23"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C228" dxfId="22"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C228" dxfId="21"/>
+    <sortCondition sortBy="cellColor" ref="C3:C228" dxfId="2"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C228" dxfId="1"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C228" dxfId="0"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8027,7 +7859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D04BD7-46BC-42FA-8579-8BAD2EA11B93}">
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -8223,14 +8055,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8451,6 +8275,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8461,23 +8293,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8496,6 +8311,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Tested and marked requirements FLC-012,13,14,15,16,17,18,19,20,21,22,23,26,27,32,33,39,45,51,57,63,69,75,83 as complete.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2285A6AE-F3B1-4431-A241-604DD6065470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA9655-2022-C748-B61D-1BF57DE55798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -3074,20 +3074,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="71" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="F309" sqref="F309"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="90" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="255.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -3391,7 +3391,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -3593,12 +3593,12 @@
       <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -3611,14 +3611,14 @@
       <c r="D35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="27" t="s">
-        <v>15</v>
+      <c r="E35" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -3628,12 +3628,12 @@
       <c r="D36" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="28" t="s">
-        <v>15</v>
+      <c r="E36" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -3643,14 +3643,14 @@
       <c r="D37" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="27" t="s">
-        <v>15</v>
+      <c r="E37" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -3660,12 +3660,12 @@
       <c r="D38" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="28" t="s">
-        <v>15</v>
+      <c r="E38" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -3675,14 +3675,14 @@
       <c r="D39" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E39" s="28" t="s">
-        <v>15</v>
+      <c r="E39" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -3692,12 +3692,12 @@
       <c r="D40" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E40" s="28" t="s">
-        <v>15</v>
+      <c r="E40" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -3707,14 +3707,14 @@
       <c r="D41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="28" t="s">
-        <v>15</v>
+      <c r="E41" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -3724,12 +3724,12 @@
       <c r="D42" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="28" t="s">
-        <v>15</v>
+      <c r="E42" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -3739,14 +3739,14 @@
       <c r="D43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>15</v>
+      <c r="E43" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -3756,12 +3756,12 @@
       <c r="D44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="28" t="s">
-        <v>15</v>
+      <c r="E44" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3771,14 +3771,14 @@
       <c r="D45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="28" t="s">
-        <v>15</v>
+      <c r="E45" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3788,12 +3788,12 @@
       <c r="D46" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="28" t="s">
-        <v>15</v>
+      <c r="E46" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3835,12 +3835,12 @@
       <c r="D49" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="28" t="s">
-        <v>15</v>
+      <c r="E49" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3850,14 +3850,14 @@
       <c r="D50" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E50" s="28" t="s">
-        <v>15</v>
+      <c r="E50" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3927,12 +3927,12 @@
       <c r="D55" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="28" t="s">
-        <v>15</v>
+      <c r="E55" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3942,14 +3942,14 @@
       <c r="D56" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E56" s="28" t="s">
-        <v>15</v>
+      <c r="E56" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -4034,14 +4034,14 @@
       <c r="D62" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E62" s="28" t="s">
-        <v>15</v>
+      <c r="E62" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -4051,12 +4051,12 @@
       <c r="D63" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E63" s="28" t="s">
-        <v>15</v>
+      <c r="E63" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -4126,14 +4126,14 @@
       <c r="D68" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E68" s="28" t="s">
-        <v>15</v>
+      <c r="E68" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -4148,7 +4148,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -4218,14 +4218,14 @@
       <c r="D74" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E74" s="28" t="s">
-        <v>15</v>
+      <c r="E74" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F74" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -4310,14 +4310,14 @@
       <c r="D80" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E80" s="28" t="s">
-        <v>15</v>
+      <c r="E80" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F80" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -4402,14 +4402,14 @@
       <c r="D86" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E86" s="28" t="s">
-        <v>15</v>
+      <c r="E86" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F86" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -4494,14 +4494,14 @@
       <c r="D92" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E92" s="28" t="s">
-        <v>15</v>
+      <c r="E92" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F92" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
         <v>213</v>
       </c>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
         <v>217</v>
       </c>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
         <v>221</v>
       </c>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
         <v>225</v>
       </c>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="60" t="s">
         <v>229</v>
       </c>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
         <v>211</v>
       </c>
@@ -4586,12 +4586,12 @@
       <c r="D98" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E98" s="28" t="s">
-        <v>15</v>
+      <c r="E98" s="80" t="s">
+        <v>489</v>
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
         <v>215</v>
       </c>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
         <v>219</v>
       </c>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
         <v>223</v>
       </c>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="F101" s="68"/>
     </row>
-    <row r="102" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
         <v>227</v>
       </c>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="60" t="s">
         <v>700</v>
       </c>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="60" t="s">
         <v>702</v>
       </c>
@@ -4696,7 +4696,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B106" s="60" t="s">
         <v>717</v>
       </c>
@@ -4706,12 +4706,12 @@
       <c r="D106" s="11" t="s">
         <v>718</v>
       </c>
-      <c r="E106" s="36" t="s">
-        <v>15</v>
+      <c r="E106" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="20" t="s">
         <v>233</v>
       </c>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="20" t="s">
         <v>235</v>
       </c>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="20" t="s">
         <v>237</v>
       </c>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="20" t="s">
         <v>239</v>
       </c>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="20" t="s">
         <v>241</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="20" t="s">
         <v>243</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="20" t="s">
         <v>245</v>
       </c>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="20" t="s">
         <v>577</v>
       </c>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B115" s="20" t="s">
         <v>247</v>
       </c>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B116" s="7" t="s">
         <v>251</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B117" s="7" t="s">
         <v>253</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="7" t="s">
         <v>255</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="7" t="s">
         <v>257</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B120" s="7" t="s">
         <v>259</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B121" s="7" t="s">
         <v>262</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B122" s="7" t="s">
         <v>265</v>
       </c>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="7" t="s">
         <v>266</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="7" t="s">
         <v>269</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="125" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B125" s="7" t="s">
         <v>271</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="7" t="s">
         <v>274</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
         <v>277</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
         <v>278</v>
       </c>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
         <v>280</v>
       </c>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
         <v>282</v>
       </c>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
         <v>284</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="132" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
         <v>286</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
         <v>289</v>
       </c>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="F133" s="7"/>
     </row>
-    <row r="134" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
         <v>291</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
         <v>293</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
         <v>296</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="137" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
         <v>508</v>
       </c>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
         <v>510</v>
       </c>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B139" s="60" t="s">
         <v>512</v>
       </c>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B140" s="60" t="s">
         <v>513</v>
       </c>
@@ -5255,7 +5255,7 @@
       </c>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
         <v>299</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
         <v>301</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
         <v>303</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
         <v>305</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
         <v>307</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
         <v>309</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="147" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
         <v>311</v>
       </c>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
         <v>313</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
         <v>315</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
         <v>317</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="151" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
         <v>319</v>
       </c>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B152" s="3" t="s">
         <v>705</v>
       </c>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
         <v>706</v>
       </c>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
         <v>707</v>
       </c>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
         <v>708</v>
       </c>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B156" s="20" t="s">
         <v>321</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B157" s="20" t="s">
         <v>323</v>
       </c>
@@ -5530,7 +5530,7 @@
       </c>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B158" s="20" t="s">
         <v>325</v>
       </c>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B159" s="20" t="s">
         <v>327</v>
       </c>
@@ -5560,7 +5560,7 @@
       </c>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B160" s="20" t="s">
         <v>329</v>
       </c>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B161" s="20" t="s">
         <v>331</v>
       </c>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B162" s="20" t="s">
         <v>333</v>
       </c>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B163" s="20" t="s">
         <v>335</v>
       </c>
@@ -5620,7 +5620,7 @@
       </c>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B164" s="20" t="s">
         <v>337</v>
       </c>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B165" s="20" t="s">
         <v>339</v>
       </c>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="F165" s="7"/>
     </row>
-    <row r="166" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B166" s="20" t="s">
         <v>341</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="167" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="20" t="s">
         <v>343</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="9" t="s">
         <v>345</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="169" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="9" t="s">
         <v>347</v>
       </c>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="F169" s="7"/>
     </row>
-    <row r="170" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="9" t="s">
         <v>348</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="171" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="9" t="s">
         <v>350</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="172" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="9" t="s">
         <v>351</v>
       </c>
@@ -5763,7 +5763,7 @@
       </c>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="9" t="s">
         <v>353</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="174" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="9" t="s">
         <v>355</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="175" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B175" s="9" t="s">
         <v>357</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="176" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B176" s="9" t="s">
         <v>359</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="177" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B177" s="9" t="s">
         <v>361</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B178" s="9" t="s">
         <v>363</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="179" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="9" t="s">
         <v>365</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="180" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10" t="s">
         <v>367</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="181" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10" t="s">
         <v>369</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="182" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10" t="s">
         <v>371</v>
       </c>
@@ -5929,7 +5929,7 @@
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="10" t="s">
         <v>373</v>
       </c>
@@ -5944,7 +5944,7 @@
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="10" t="s">
         <v>713</v>
       </c>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B185" s="10" t="s">
         <v>715</v>
       </c>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B186" s="21" t="s">
         <v>375</v>
       </c>
@@ -5989,7 +5989,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B187" s="21" t="s">
         <v>377</v>
       </c>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B188" s="21" t="s">
         <v>379</v>
       </c>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="F188" s="7"/>
     </row>
-    <row r="189" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B189" s="21" t="s">
         <v>381</v>
       </c>
@@ -6034,7 +6034,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B190" s="21" t="s">
         <v>383</v>
       </c>
@@ -6049,7 +6049,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="21" t="s">
         <v>385</v>
       </c>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
         <v>387</v>
       </c>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="F192" s="7"/>
     </row>
-    <row r="193" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B193" s="3" t="s">
         <v>389</v>
       </c>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>391</v>
       </c>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="F194" s="7"/>
     </row>
-    <row r="195" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B195" s="3" t="s">
         <v>393</v>
       </c>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B196" s="21" t="s">
         <v>395</v>
       </c>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="3" t="s">
         <v>397</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
         <v>399</v>
       </c>
@@ -6169,7 +6169,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B199" s="21" t="s">
         <v>401</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="200" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B200" s="3" t="s">
         <v>403</v>
       </c>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
         <v>405</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B202" s="3" t="s">
         <v>407</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
         <v>409</v>
       </c>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
         <v>411</v>
       </c>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
         <v>413</v>
       </c>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B206" s="3" t="s">
         <v>415</v>
       </c>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
         <v>417</v>
       </c>
@@ -6308,7 +6308,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
         <v>419</v>
       </c>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
         <v>421</v>
       </c>
@@ -6338,7 +6338,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
         <v>423</v>
       </c>
@@ -6353,7 +6353,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
         <v>425</v>
       </c>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
         <v>427</v>
       </c>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
         <v>429</v>
       </c>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
         <v>431</v>
       </c>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="21" t="s">
         <v>433</v>
       </c>
@@ -6428,7 +6428,7 @@
       </c>
       <c r="F215" s="7"/>
     </row>
-    <row r="216" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="21" t="s">
         <v>435</v>
       </c>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="21" t="s">
         <v>437</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="12" t="s">
         <v>439</v>
       </c>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="12" t="s">
         <v>441</v>
       </c>
@@ -6488,7 +6488,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="12" t="s">
         <v>443</v>
       </c>
@@ -6503,7 +6503,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="12" t="s">
         <v>445</v>
       </c>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B222" s="21" t="s">
         <v>447</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="223" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B223" s="21" t="s">
         <v>449</v>
       </c>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B224" s="21" t="s">
         <v>451</v>
       </c>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B225" s="21" t="s">
         <v>453</v>
       </c>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B226" s="21" t="s">
         <v>455</v>
       </c>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B227" s="21" t="s">
         <v>457</v>
       </c>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B228" s="21" t="s">
         <v>459</v>
       </c>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B229" s="21" t="s">
         <v>461</v>
       </c>
@@ -6640,7 +6640,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B230" s="21" t="s">
         <v>463</v>
       </c>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B231" s="12" t="s">
         <v>465</v>
       </c>
@@ -6670,7 +6670,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B232" s="12" t="s">
         <v>467</v>
       </c>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B233" s="12" t="s">
         <v>469</v>
       </c>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B234" s="12" t="s">
         <v>471</v>
       </c>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="12" t="s">
         <v>473</v>
       </c>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B236" s="12" t="s">
         <v>475</v>
       </c>
@@ -6745,7 +6745,7 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B237" s="12" t="s">
         <v>477</v>
       </c>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B238" s="12" t="s">
         <v>479</v>
       </c>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="F238" s="7"/>
     </row>
-    <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B239" s="12" t="s">
         <v>481</v>
       </c>
@@ -6790,7 +6790,7 @@
       </c>
       <c r="F239" s="7"/>
     </row>
-    <row r="240" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B240" s="12" t="s">
         <v>483</v>
       </c>
@@ -6805,7 +6805,7 @@
       </c>
       <c r="F240" s="7"/>
     </row>
-    <row r="241" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B241" s="68" t="s">
         <v>602</v>
       </c>
@@ -6820,7 +6820,7 @@
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B242" s="68" t="s">
         <v>604</v>
       </c>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B243" s="68" t="s">
         <v>529</v>
       </c>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="F243" s="7"/>
     </row>
-    <row r="244" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B244" s="68" t="s">
         <v>531</v>
       </c>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="F244" s="7"/>
     </row>
-    <row r="245" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B245" s="68" t="s">
         <v>533</v>
       </c>
@@ -6880,7 +6880,7 @@
       </c>
       <c r="F245" s="7"/>
     </row>
-    <row r="246" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B246" s="68" t="s">
         <v>606</v>
       </c>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="F246" s="7"/>
     </row>
-    <row r="247" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B247" s="68" t="s">
         <v>608</v>
       </c>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="F247" s="7"/>
     </row>
-    <row r="248" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B248" s="68" t="s">
         <v>527</v>
       </c>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="F248" s="7"/>
     </row>
-    <row r="249" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B249" s="68" t="s">
         <v>535</v>
       </c>
@@ -6940,7 +6940,7 @@
       </c>
       <c r="F249" s="7"/>
     </row>
-    <row r="250" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B250" s="68" t="s">
         <v>610</v>
       </c>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="F250" s="7"/>
     </row>
-    <row r="251" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B251" s="68" t="s">
         <v>537</v>
       </c>
@@ -6970,7 +6970,7 @@
       </c>
       <c r="F251" s="7"/>
     </row>
-    <row r="252" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B252" s="68" t="s">
         <v>539</v>
       </c>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="F252" s="7"/>
     </row>
-    <row r="253" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B253" s="71" t="s">
         <v>543</v>
       </c>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="F253" s="7"/>
     </row>
-    <row r="254" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B254" s="71" t="s">
         <v>545</v>
       </c>
@@ -7015,7 +7015,7 @@
       </c>
       <c r="F254" s="7"/>
     </row>
-    <row r="255" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B255" s="71" t="s">
         <v>549</v>
       </c>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="F255" s="7"/>
     </row>
-    <row r="256" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B256" s="71" t="s">
         <v>555</v>
       </c>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="F256" s="7"/>
     </row>
-    <row r="257" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B257" s="71" t="s">
         <v>557</v>
       </c>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="F257" s="7"/>
     </row>
-    <row r="258" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B258" s="71" t="s">
         <v>547</v>
       </c>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="F258" s="7"/>
     </row>
-    <row r="259" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B259" s="71" t="s">
         <v>551</v>
       </c>
@@ -7090,7 +7090,7 @@
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B260" s="71" t="s">
         <v>553</v>
       </c>
@@ -7105,7 +7105,7 @@
       </c>
       <c r="F260" s="7"/>
     </row>
-    <row r="261" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B261" s="71" t="s">
         <v>559</v>
       </c>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="F261" s="7"/>
     </row>
-    <row r="262" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B262" s="71" t="s">
         <v>561</v>
       </c>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="F262" s="7"/>
     </row>
-    <row r="263" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B263" s="71" t="s">
         <v>563</v>
       </c>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="F263" s="7"/>
     </row>
-    <row r="264" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B264" s="71" t="s">
         <v>618</v>
       </c>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="F264" s="7"/>
     </row>
-    <row r="265" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B265" s="71" t="s">
         <v>619</v>
       </c>
@@ -7180,7 +7180,7 @@
       </c>
       <c r="F265" s="7"/>
     </row>
-    <row r="266" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B266" s="71" t="s">
         <v>620</v>
       </c>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="F266" s="7"/>
     </row>
-    <row r="267" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B267" s="71" t="s">
         <v>621</v>
       </c>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="F267" s="68"/>
     </row>
-    <row r="268" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B268" s="71" t="s">
         <v>622</v>
       </c>
@@ -7225,7 +7225,7 @@
       </c>
       <c r="F268" s="68"/>
     </row>
-    <row r="269" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B269" s="71" t="s">
         <v>623</v>
       </c>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="F269" s="68"/>
     </row>
-    <row r="270" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B270" s="71" t="s">
         <v>624</v>
       </c>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="F270" s="68"/>
     </row>
-    <row r="271" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B271" s="71" t="s">
         <v>625</v>
       </c>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="F271" s="68"/>
     </row>
-    <row r="272" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B272" s="71" t="s">
         <v>626</v>
       </c>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="F272" s="68"/>
     </row>
-    <row r="273" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B273" s="71" t="s">
         <v>627</v>
       </c>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="F273" s="68"/>
     </row>
-    <row r="274" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B274" s="71" t="s">
         <v>628</v>
       </c>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="F274" s="68"/>
     </row>
-    <row r="275" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B275" s="71" t="s">
         <v>629</v>
       </c>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="F275" s="68"/>
     </row>
-    <row r="276" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B276" s="71" t="s">
         <v>630</v>
       </c>
@@ -7345,7 +7345,7 @@
       </c>
       <c r="F276" s="68"/>
     </row>
-    <row r="277" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B277" s="71" t="s">
         <v>631</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="F277" s="68"/>
     </row>
-    <row r="278" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B278" s="71" t="s">
         <v>632</v>
       </c>
@@ -7375,7 +7375,7 @@
       </c>
       <c r="F278" s="68"/>
     </row>
-    <row r="279" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B279" s="71" t="s">
         <v>633</v>
       </c>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="F279" s="68"/>
     </row>
-    <row r="280" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B280" s="71" t="s">
         <v>650</v>
       </c>
@@ -7405,7 +7405,7 @@
       </c>
       <c r="F280" s="68"/>
     </row>
-    <row r="281" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B281" s="71" t="s">
         <v>652</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="F281" s="68"/>
     </row>
-    <row r="282" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B282" s="71" t="s">
         <v>658</v>
       </c>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="F282" s="68"/>
     </row>
-    <row r="283" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B283" s="71" t="s">
         <v>657</v>
       </c>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="F283" s="68"/>
     </row>
-    <row r="284" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B284" s="71" t="s">
         <v>654</v>
       </c>
@@ -7465,7 +7465,7 @@
       </c>
       <c r="F284" s="68"/>
     </row>
-    <row r="285" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B285" s="71" t="s">
         <v>655</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="F285" s="68"/>
     </row>
-    <row r="286" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B286" s="71" t="s">
         <v>660</v>
       </c>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="F286" s="68"/>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B287" s="68" t="s">
         <v>664</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="F287" s="68"/>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B288" s="68" t="s">
         <v>666</v>
       </c>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="F288" s="68"/>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B289" s="68" t="s">
         <v>668</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="F289" s="68"/>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B290" s="68" t="s">
         <v>670</v>
       </c>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="F290" s="68"/>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B291" s="68" t="s">
         <v>672</v>
       </c>
@@ -7570,7 +7570,7 @@
       </c>
       <c r="F291" s="68"/>
     </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B292" s="68" t="s">
         <v>674</v>
       </c>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="F292" s="68"/>
     </row>
-    <row r="293" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B293" s="68" t="s">
         <v>676</v>
       </c>
@@ -7600,7 +7600,7 @@
       </c>
       <c r="F293" s="68"/>
     </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B294" s="68" t="s">
         <v>678</v>
       </c>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="F294" s="68"/>
     </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B295" s="68" t="s">
         <v>680</v>
       </c>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="F295" s="68"/>
     </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B296" s="68" t="s">
         <v>682</v>
       </c>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="F296" s="68"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B297" s="68" t="s">
         <v>684</v>
       </c>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="F297" s="68"/>
     </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B298" s="68" t="s">
         <v>686</v>
       </c>
@@ -7675,7 +7675,7 @@
       </c>
       <c r="F298" s="68"/>
     </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B299" s="68" t="s">
         <v>688</v>
       </c>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="F299" s="68"/>
     </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B300" s="68" t="s">
         <v>690</v>
       </c>
@@ -7705,7 +7705,7 @@
       </c>
       <c r="F300" s="68"/>
     </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B301" s="68" t="s">
         <v>692</v>
       </c>
@@ -7720,7 +7720,7 @@
       </c>
       <c r="F301" s="68"/>
     </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B302" s="68" t="s">
         <v>694</v>
       </c>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="F302" s="68"/>
     </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B303" s="68" t="s">
         <v>696</v>
       </c>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="F303" s="68"/>
     </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B304" s="68" t="s">
         <v>698</v>
       </c>
@@ -7765,77 +7765,77 @@
       </c>
       <c r="F304" s="68"/>
     </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B305" s="68"/>
       <c r="C305" s="68"/>
       <c r="D305" s="68"/>
       <c r="E305" s="68"/>
       <c r="F305" s="68"/>
     </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B306" s="68"/>
       <c r="C306" s="68"/>
       <c r="D306" s="68"/>
       <c r="E306" s="68"/>
       <c r="F306" s="68"/>
     </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B307" s="68"/>
       <c r="C307" s="68"/>
       <c r="D307" s="68"/>
       <c r="E307" s="68"/>
       <c r="F307" s="68"/>
     </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B308" s="68"/>
       <c r="C308" s="68"/>
       <c r="D308" s="68"/>
       <c r="E308" s="68"/>
       <c r="F308" s="68"/>
     </row>
-    <row r="309" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B309" s="68"/>
       <c r="C309" s="68"/>
       <c r="D309" s="68"/>
       <c r="E309" s="68"/>
       <c r="F309" s="68"/>
     </row>
-    <row r="310" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B310" s="68"/>
       <c r="C310" s="68"/>
       <c r="D310" s="68"/>
       <c r="E310" s="68"/>
       <c r="F310" s="68"/>
     </row>
-    <row r="311" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B311" s="68"/>
       <c r="C311" s="68"/>
       <c r="D311" s="68"/>
       <c r="E311" s="68"/>
       <c r="F311" s="68"/>
     </row>
-    <row r="312" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B312" s="68"/>
       <c r="C312" s="68"/>
       <c r="D312" s="68"/>
       <c r="E312" s="68"/>
       <c r="F312" s="68"/>
     </row>
-    <row r="313" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B313" s="68"/>
       <c r="C313" s="68"/>
       <c r="D313" s="68"/>
       <c r="E313" s="68"/>
       <c r="F313" s="68"/>
     </row>
-    <row r="314" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B314" s="68"/>
       <c r="C314" s="68"/>
       <c r="D314" s="68"/>
       <c r="E314" s="68"/>
       <c r="F314" s="68"/>
     </row>
-    <row r="315" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B315" s="68"/>
       <c r="C315" s="68"/>
       <c r="D315" s="68"/>
@@ -7863,13 +7863,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55.21875" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="70" t="s">
         <v>541</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="73" t="s">
         <v>565</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="73" t="s">
         <v>567</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="73" t="s">
         <v>569</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="73" t="s">
         <v>571</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="73" t="s">
         <v>573</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="73" t="s">
         <v>575</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="73" t="s">
         <v>578</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="73" t="s">
         <v>580</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="73" t="s">
         <v>582</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="73" t="s">
         <v>584</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="73" t="s">
         <v>586</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="73" t="s">
         <v>588</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="73" t="s">
         <v>590</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="73" t="s">
         <v>592</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="73" t="s">
         <v>594</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="73" t="s">
         <v>596</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="73" t="s">
         <v>598</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="73" t="s">
         <v>600</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="73" t="s">
         <v>612</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="73" t="s">
         <v>614</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="69" t="s">
         <v>616</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="69"/>
       <c r="C24" s="69"/>
     </row>
@@ -8055,6 +8055,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8275,38 +8292,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8329,9 +8318,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mark Completion of Menu and Propulsion Requirements
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Downloads\jsbsimedit2\requirements_specification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA9655-2022-C748-B61D-1BF57DE55798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81472805-756A-4A99-8843-1B311B1D136E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -3074,20 +3074,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="90" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="52" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
     <col min="4" max="4" width="255.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>9</v>
       </c>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
@@ -3391,7 +3391,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>58</v>
       </c>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>60</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
@@ -3502,7 +3502,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="3" t="s">
         <v>70</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
         <v>73</v>
       </c>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="s">
         <v>75</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
         <v>78</v>
       </c>
@@ -3598,7 +3598,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>84</v>
       </c>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>86</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3" t="s">
         <v>89</v>
       </c>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>91</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>94</v>
       </c>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="F40" s="7"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>96</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>99</v>
       </c>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>101</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
@@ -3761,7 +3761,7 @@
       </c>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>111</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>116</v>
       </c>
@@ -3840,7 +3840,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
         <v>118</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
         <v>121</v>
       </c>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
         <v>123</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
         <v>125</v>
       </c>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
         <v>127</v>
       </c>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="F54" s="7"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
         <v>129</v>
       </c>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="F55" s="7"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
         <v>131</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
         <v>134</v>
       </c>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="F57" s="7"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
         <v>136</v>
       </c>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="F58" s="7"/>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
         <v>138</v>
       </c>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="F59" s="7"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
         <v>140</v>
       </c>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
         <v>142</v>
       </c>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
         <v>144</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
         <v>147</v>
       </c>
@@ -4056,7 +4056,7 @@
       </c>
       <c r="F63" s="7"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
         <v>149</v>
       </c>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
         <v>153</v>
       </c>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="F66" s="7"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
         <v>155</v>
       </c>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="F67" s="7"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
         <v>157</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
         <v>160</v>
       </c>
@@ -4148,7 +4148,7 @@
       </c>
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
         <v>162</v>
       </c>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
         <v>164</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="F71" s="7"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
         <v>166</v>
       </c>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="F72" s="7"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
         <v>168</v>
       </c>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>170</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
         <v>173</v>
       </c>
@@ -4240,7 +4240,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
         <v>175</v>
       </c>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="F76" s="7"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
         <v>177</v>
       </c>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="F77" s="7"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
         <v>179</v>
       </c>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
         <v>181</v>
       </c>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
         <v>183</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
         <v>185</v>
       </c>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="F81" s="7"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
         <v>187</v>
       </c>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="F82" s="7"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
         <v>189</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
         <v>191</v>
       </c>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
         <v>195</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
         <v>198</v>
       </c>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="F87" s="7"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
         <v>200</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
         <v>202</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="F89" s="7"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="3" t="s">
         <v>213</v>
       </c>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="F93" s="7"/>
     </row>
-    <row r="94" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="3" t="s">
         <v>217</v>
       </c>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="F94" s="7"/>
     </row>
-    <row r="95" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="3" t="s">
         <v>221</v>
       </c>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B96" s="3" t="s">
         <v>225</v>
       </c>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="F96" s="7"/>
     </row>
-    <row r="97" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B97" s="60" t="s">
         <v>229</v>
       </c>
@@ -4576,7 +4576,7 @@
       </c>
       <c r="F97" s="7"/>
     </row>
-    <row r="98" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B98" s="3" t="s">
         <v>211</v>
       </c>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="F98" s="7"/>
     </row>
-    <row r="99" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B99" s="3" t="s">
         <v>215</v>
       </c>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="3" t="s">
         <v>219</v>
       </c>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="F100" s="7"/>
     </row>
-    <row r="101" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B101" s="3" t="s">
         <v>223</v>
       </c>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="F101" s="68"/>
     </row>
-    <row r="102" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B102" s="3" t="s">
         <v>227</v>
       </c>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B103" s="3" t="s">
         <v>231</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="60" t="s">
         <v>700</v>
       </c>
@@ -4681,7 +4681,7 @@
       </c>
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="60" t="s">
         <v>702</v>
       </c>
@@ -4696,7 +4696,7 @@
       </c>
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="60" t="s">
         <v>717</v>
       </c>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="20" t="s">
         <v>233</v>
       </c>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="20" t="s">
         <v>235</v>
       </c>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="20" t="s">
         <v>237</v>
       </c>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="20" t="s">
         <v>239</v>
       </c>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="20" t="s">
         <v>241</v>
       </c>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="20" t="s">
         <v>243</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="20" t="s">
         <v>245</v>
       </c>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="F113" s="7"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="20" t="s">
         <v>577</v>
       </c>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="F114" s="7"/>
     </row>
-    <row r="115" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="20" t="s">
         <v>247</v>
       </c>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="7" t="s">
         <v>251</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="7" t="s">
         <v>253</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B118" s="7" t="s">
         <v>255</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="7" t="s">
         <v>257</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B120" s="7" t="s">
         <v>259</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="121" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B121" s="7" t="s">
         <v>262</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="122" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="7" t="s">
         <v>265</v>
       </c>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="7" t="s">
         <v>266</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="124" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B124" s="7" t="s">
         <v>269</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="125" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="7" t="s">
         <v>271</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B126" s="7" t="s">
         <v>274</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
         <v>277</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
         <v>278</v>
       </c>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
         <v>280</v>
       </c>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="F129" s="7"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
         <v>282</v>
       </c>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="F130" s="7"/>
     </row>
-    <row r="131" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B131" s="3" t="s">
         <v>284</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="132" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B132" s="3" t="s">
         <v>286</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="3" t="s">
         <v>289</v>
       </c>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="F133" s="7"/>
     </row>
-    <row r="134" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="3" t="s">
         <v>291</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="3" t="s">
         <v>293</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="3" t="s">
         <v>296</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="137" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="3" t="s">
         <v>508</v>
       </c>
@@ -5205,12 +5205,12 @@
       <c r="D137" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="E137" s="29" t="s">
-        <v>15</v>
+      <c r="E137" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F137" s="7"/>
     </row>
-    <row r="138" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B138" s="3" t="s">
         <v>510</v>
       </c>
@@ -5220,12 +5220,12 @@
       <c r="D138" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="E138" s="29" t="s">
-        <v>15</v>
+      <c r="E138" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B139" s="60" t="s">
         <v>512</v>
       </c>
@@ -5240,7 +5240,7 @@
       </c>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="60" t="s">
         <v>513</v>
       </c>
@@ -5250,12 +5250,12 @@
       <c r="D140" s="11" t="s">
         <v>515</v>
       </c>
-      <c r="E140" s="27" t="s">
-        <v>15</v>
+      <c r="E140" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F140" s="7"/>
     </row>
-    <row r="141" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="3" t="s">
         <v>299</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="3" t="s">
         <v>301</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="3" t="s">
         <v>303</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B144" s="3" t="s">
         <v>305</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B145" s="3" t="s">
         <v>307</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="146" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="3" t="s">
         <v>309</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="147" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B147" s="3" t="s">
         <v>311</v>
       </c>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B148" s="3" t="s">
         <v>313</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="3" t="s">
         <v>315</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="3" t="s">
         <v>317</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="151" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="3" t="s">
         <v>319</v>
       </c>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="F151" s="7"/>
     </row>
-    <row r="152" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="3" t="s">
         <v>705</v>
       </c>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="F152" s="7"/>
     </row>
-    <row r="153" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B153" s="3" t="s">
         <v>706</v>
       </c>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="F153" s="7"/>
     </row>
-    <row r="154" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B154" s="3" t="s">
         <v>707</v>
       </c>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="F154" s="7"/>
     </row>
-    <row r="155" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B155" s="3" t="s">
         <v>708</v>
       </c>
@@ -5498,7 +5498,7 @@
       </c>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="20" t="s">
         <v>321</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="157" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="20" t="s">
         <v>323</v>
       </c>
@@ -5530,7 +5530,7 @@
       </c>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="20" t="s">
         <v>325</v>
       </c>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B159" s="20" t="s">
         <v>327</v>
       </c>
@@ -5560,7 +5560,7 @@
       </c>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="20" t="s">
         <v>329</v>
       </c>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="20" t="s">
         <v>331</v>
       </c>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="20" t="s">
         <v>333</v>
       </c>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="20" t="s">
         <v>335</v>
       </c>
@@ -5620,7 +5620,7 @@
       </c>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="20" t="s">
         <v>337</v>
       </c>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B165" s="20" t="s">
         <v>339</v>
       </c>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="F165" s="7"/>
     </row>
-    <row r="166" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="20" t="s">
         <v>341</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="167" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="20" t="s">
         <v>343</v>
       </c>
@@ -5682,7 +5682,7 @@
       </c>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="9" t="s">
         <v>345</v>
       </c>
@@ -5692,14 +5692,14 @@
       <c r="D168" s="63" t="s">
         <v>496</v>
       </c>
-      <c r="E168" s="54" t="s">
-        <v>15</v>
+      <c r="E168" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F168" s="7" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="169" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B169" s="9" t="s">
         <v>347</v>
       </c>
@@ -5709,12 +5709,12 @@
       <c r="D169" s="64" t="s">
         <v>497</v>
       </c>
-      <c r="E169" s="54" t="s">
-        <v>15</v>
+      <c r="E169" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F169" s="7"/>
     </row>
-    <row r="170" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B170" s="9" t="s">
         <v>348</v>
       </c>
@@ -5724,14 +5724,14 @@
       <c r="D170" s="65" t="s">
         <v>498</v>
       </c>
-      <c r="E170" s="54" t="s">
-        <v>15</v>
+      <c r="E170" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F170" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="171" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B171" s="9" t="s">
         <v>350</v>
       </c>
@@ -5741,14 +5741,14 @@
       <c r="D171" s="64" t="s">
         <v>499</v>
       </c>
-      <c r="E171" s="54" t="s">
-        <v>15</v>
+      <c r="E171" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F171" s="7" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="172" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B172" s="9" t="s">
         <v>351</v>
       </c>
@@ -5758,12 +5758,12 @@
       <c r="D172" s="65" t="s">
         <v>500</v>
       </c>
-      <c r="E172" s="26" t="s">
-        <v>15</v>
+      <c r="E172" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F172" s="7"/>
     </row>
-    <row r="173" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B173" s="9" t="s">
         <v>353</v>
       </c>
@@ -5773,14 +5773,14 @@
       <c r="D173" s="65" t="s">
         <v>501</v>
       </c>
-      <c r="E173" s="54" t="s">
-        <v>15</v>
+      <c r="E173" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F173" s="7" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="174" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B174" s="9" t="s">
         <v>355</v>
       </c>
@@ -5790,14 +5790,14 @@
       <c r="D174" s="51" t="s">
         <v>356</v>
       </c>
-      <c r="E174" s="54" t="s">
-        <v>15</v>
+      <c r="E174" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F174" s="7" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B175" s="9" t="s">
         <v>357</v>
       </c>
@@ -5807,14 +5807,14 @@
       <c r="D175" s="65" t="s">
         <v>502</v>
       </c>
-      <c r="E175" s="54" t="s">
+      <c r="E175" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B176" s="9" t="s">
         <v>359</v>
       </c>
@@ -5824,14 +5824,14 @@
       <c r="D176" s="65" t="s">
         <v>503</v>
       </c>
-      <c r="E176" s="54" t="s">
-        <v>15</v>
+      <c r="E176" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F176" s="7" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B177" s="9" t="s">
         <v>361</v>
       </c>
@@ -5841,12 +5841,12 @@
       <c r="D177" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="E177" s="26" t="s">
-        <v>15</v>
+      <c r="E177" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B178" s="9" t="s">
         <v>363</v>
       </c>
@@ -5856,14 +5856,14 @@
       <c r="D178" s="65" t="s">
         <v>505</v>
       </c>
-      <c r="E178" s="28" t="s">
-        <v>15</v>
+      <c r="E178" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F178" s="7" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="179" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B179" s="9" t="s">
         <v>365</v>
       </c>
@@ -5873,14 +5873,14 @@
       <c r="D179" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="E179" s="28" t="s">
-        <v>15</v>
+      <c r="E179" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F179" s="7" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="180" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B180" s="10" t="s">
         <v>367</v>
       </c>
@@ -5890,14 +5890,14 @@
       <c r="D180" s="59" t="s">
         <v>485</v>
       </c>
-      <c r="E180" s="28" t="s">
-        <v>15</v>
+      <c r="E180" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F180" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="181" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B181" s="10" t="s">
         <v>369</v>
       </c>
@@ -5907,14 +5907,14 @@
       <c r="D181" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="E181" s="28" t="s">
-        <v>15</v>
+      <c r="E181" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F181" s="7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="182" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B182" s="10" t="s">
         <v>371</v>
       </c>
@@ -5924,12 +5924,12 @@
       <c r="D182" s="6" t="s">
         <v>487</v>
       </c>
-      <c r="E182" s="28" t="s">
-        <v>15</v>
+      <c r="E182" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B183" s="10" t="s">
         <v>373</v>
       </c>
@@ -5939,12 +5939,12 @@
       <c r="D183" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="E183" s="28" t="s">
-        <v>15</v>
+      <c r="E183" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B184" s="10" t="s">
         <v>713</v>
       </c>
@@ -5959,7 +5959,7 @@
       </c>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B185" s="10" t="s">
         <v>715</v>
       </c>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="F185" s="7"/>
     </row>
-    <row r="186" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B186" s="21" t="s">
         <v>375</v>
       </c>
@@ -5989,7 +5989,7 @@
       </c>
       <c r="F186" s="7"/>
     </row>
-    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B187" s="21" t="s">
         <v>377</v>
       </c>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="F187" s="7"/>
     </row>
-    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B188" s="21" t="s">
         <v>379</v>
       </c>
@@ -6019,7 +6019,7 @@
       </c>
       <c r="F188" s="7"/>
     </row>
-    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B189" s="21" t="s">
         <v>381</v>
       </c>
@@ -6034,7 +6034,7 @@
       </c>
       <c r="F189" s="7"/>
     </row>
-    <row r="190" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B190" s="21" t="s">
         <v>383</v>
       </c>
@@ -6049,7 +6049,7 @@
       </c>
       <c r="F190" s="7"/>
     </row>
-    <row r="191" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B191" s="21" t="s">
         <v>385</v>
       </c>
@@ -6064,7 +6064,7 @@
       </c>
       <c r="F191" s="7"/>
     </row>
-    <row r="192" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B192" s="3" t="s">
         <v>387</v>
       </c>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="F192" s="7"/>
     </row>
-    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B193" s="3" t="s">
         <v>389</v>
       </c>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="F193" s="7"/>
     </row>
-    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B194" s="3" t="s">
         <v>391</v>
       </c>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="F194" s="7"/>
     </row>
-    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B195" s="3" t="s">
         <v>393</v>
       </c>
@@ -6124,7 +6124,7 @@
       </c>
       <c r="F195" s="7"/>
     </row>
-    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B196" s="21" t="s">
         <v>395</v>
       </c>
@@ -6139,7 +6139,7 @@
       </c>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B197" s="3" t="s">
         <v>397</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="F197" s="7"/>
     </row>
-    <row r="198" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B198" s="3" t="s">
         <v>399</v>
       </c>
@@ -6169,7 +6169,7 @@
       </c>
       <c r="F198" s="7"/>
     </row>
-    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B199" s="21" t="s">
         <v>401</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B200" s="3" t="s">
         <v>403</v>
       </c>
@@ -6201,7 +6201,7 @@
       </c>
       <c r="F200" s="7"/>
     </row>
-    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B201" s="3" t="s">
         <v>405</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B202" s="3" t="s">
         <v>407</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="F202" s="7"/>
     </row>
-    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B203" s="3" t="s">
         <v>409</v>
       </c>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="F203" s="7"/>
     </row>
-    <row r="204" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B204" s="3" t="s">
         <v>411</v>
       </c>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="F204" s="7"/>
     </row>
-    <row r="205" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B205" s="3" t="s">
         <v>413</v>
       </c>
@@ -6278,7 +6278,7 @@
       </c>
       <c r="F205" s="7"/>
     </row>
-    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B206" s="3" t="s">
         <v>415</v>
       </c>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="F206" s="7"/>
     </row>
-    <row r="207" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B207" s="3" t="s">
         <v>417</v>
       </c>
@@ -6308,7 +6308,7 @@
       </c>
       <c r="F207" s="7"/>
     </row>
-    <row r="208" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B208" s="3" t="s">
         <v>419</v>
       </c>
@@ -6323,7 +6323,7 @@
       </c>
       <c r="F208" s="7"/>
     </row>
-    <row r="209" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B209" s="3" t="s">
         <v>421</v>
       </c>
@@ -6338,7 +6338,7 @@
       </c>
       <c r="F209" s="7"/>
     </row>
-    <row r="210" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B210" s="3" t="s">
         <v>423</v>
       </c>
@@ -6353,7 +6353,7 @@
       </c>
       <c r="F210" s="7"/>
     </row>
-    <row r="211" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B211" s="3" t="s">
         <v>425</v>
       </c>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="F211" s="7"/>
     </row>
-    <row r="212" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B212" s="3" t="s">
         <v>427</v>
       </c>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="F212" s="7"/>
     </row>
-    <row r="213" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B213" s="3" t="s">
         <v>429</v>
       </c>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="F213" s="7"/>
     </row>
-    <row r="214" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B214" s="3" t="s">
         <v>431</v>
       </c>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F214" s="7"/>
     </row>
-    <row r="215" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B215" s="21" t="s">
         <v>433</v>
       </c>
@@ -6428,7 +6428,7 @@
       </c>
       <c r="F215" s="7"/>
     </row>
-    <row r="216" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B216" s="21" t="s">
         <v>435</v>
       </c>
@@ -6443,7 +6443,7 @@
       </c>
       <c r="F216" s="7"/>
     </row>
-    <row r="217" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B217" s="21" t="s">
         <v>437</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="F217" s="7"/>
     </row>
-    <row r="218" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B218" s="12" t="s">
         <v>439</v>
       </c>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="F218" s="7"/>
     </row>
-    <row r="219" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B219" s="12" t="s">
         <v>441</v>
       </c>
@@ -6488,7 +6488,7 @@
       </c>
       <c r="F219" s="7"/>
     </row>
-    <row r="220" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B220" s="12" t="s">
         <v>443</v>
       </c>
@@ -6503,7 +6503,7 @@
       </c>
       <c r="F220" s="7"/>
     </row>
-    <row r="221" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B221" s="12" t="s">
         <v>445</v>
       </c>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="F221" s="7"/>
     </row>
-    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B222" s="21" t="s">
         <v>447</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B223" s="21" t="s">
         <v>449</v>
       </c>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="F223" s="7"/>
     </row>
-    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B224" s="21" t="s">
         <v>451</v>
       </c>
@@ -6565,7 +6565,7 @@
       </c>
       <c r="F224" s="7"/>
     </row>
-    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B225" s="21" t="s">
         <v>453</v>
       </c>
@@ -6580,7 +6580,7 @@
       </c>
       <c r="F225" s="7"/>
     </row>
-    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B226" s="21" t="s">
         <v>455</v>
       </c>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="F226" s="7"/>
     </row>
-    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B227" s="21" t="s">
         <v>457</v>
       </c>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="F227" s="7"/>
     </row>
-    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B228" s="21" t="s">
         <v>459</v>
       </c>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="F228" s="7"/>
     </row>
-    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B229" s="21" t="s">
         <v>461</v>
       </c>
@@ -6640,7 +6640,7 @@
       </c>
       <c r="F229" s="7"/>
     </row>
-    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B230" s="21" t="s">
         <v>463</v>
       </c>
@@ -6655,7 +6655,7 @@
       </c>
       <c r="F230" s="7"/>
     </row>
-    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B231" s="12" t="s">
         <v>465</v>
       </c>
@@ -6670,7 +6670,7 @@
       </c>
       <c r="F231" s="7"/>
     </row>
-    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B232" s="12" t="s">
         <v>467</v>
       </c>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="F232" s="7"/>
     </row>
-    <row r="233" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B233" s="12" t="s">
         <v>469</v>
       </c>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="F233" s="7"/>
     </row>
-    <row r="234" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B234" s="12" t="s">
         <v>471</v>
       </c>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="F234" s="7"/>
     </row>
-    <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B235" s="12" t="s">
         <v>473</v>
       </c>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="F235" s="7"/>
     </row>
-    <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B236" s="12" t="s">
         <v>475</v>
       </c>
@@ -6745,7 +6745,7 @@
       </c>
       <c r="F236" s="7"/>
     </row>
-    <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B237" s="12" t="s">
         <v>477</v>
       </c>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="F237" s="7"/>
     </row>
-    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B238" s="12" t="s">
         <v>479</v>
       </c>
@@ -6775,7 +6775,7 @@
       </c>
       <c r="F238" s="7"/>
     </row>
-    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B239" s="12" t="s">
         <v>481</v>
       </c>
@@ -6790,7 +6790,7 @@
       </c>
       <c r="F239" s="7"/>
     </row>
-    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B240" s="12" t="s">
         <v>483</v>
       </c>
@@ -6805,7 +6805,7 @@
       </c>
       <c r="F240" s="7"/>
     </row>
-    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B241" s="68" t="s">
         <v>602</v>
       </c>
@@ -6820,7 +6820,7 @@
       </c>
       <c r="F241" s="7"/>
     </row>
-    <row r="242" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B242" s="68" t="s">
         <v>604</v>
       </c>
@@ -6835,7 +6835,7 @@
       </c>
       <c r="F242" s="7"/>
     </row>
-    <row r="243" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B243" s="68" t="s">
         <v>529</v>
       </c>
@@ -6850,7 +6850,7 @@
       </c>
       <c r="F243" s="7"/>
     </row>
-    <row r="244" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B244" s="68" t="s">
         <v>531</v>
       </c>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="F244" s="7"/>
     </row>
-    <row r="245" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B245" s="68" t="s">
         <v>533</v>
       </c>
@@ -6880,7 +6880,7 @@
       </c>
       <c r="F245" s="7"/>
     </row>
-    <row r="246" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B246" s="68" t="s">
         <v>606</v>
       </c>
@@ -6895,7 +6895,7 @@
       </c>
       <c r="F246" s="7"/>
     </row>
-    <row r="247" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B247" s="68" t="s">
         <v>608</v>
       </c>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="F247" s="7"/>
     </row>
-    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B248" s="68" t="s">
         <v>527</v>
       </c>
@@ -6925,7 +6925,7 @@
       </c>
       <c r="F248" s="7"/>
     </row>
-    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B249" s="68" t="s">
         <v>535</v>
       </c>
@@ -6940,7 +6940,7 @@
       </c>
       <c r="F249" s="7"/>
     </row>
-    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B250" s="68" t="s">
         <v>610</v>
       </c>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="F250" s="7"/>
     </row>
-    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B251" s="68" t="s">
         <v>537</v>
       </c>
@@ -6970,7 +6970,7 @@
       </c>
       <c r="F251" s="7"/>
     </row>
-    <row r="252" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B252" s="68" t="s">
         <v>539</v>
       </c>
@@ -6985,7 +6985,7 @@
       </c>
       <c r="F252" s="7"/>
     </row>
-    <row r="253" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B253" s="71" t="s">
         <v>543</v>
       </c>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="F253" s="7"/>
     </row>
-    <row r="254" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B254" s="71" t="s">
         <v>545</v>
       </c>
@@ -7015,7 +7015,7 @@
       </c>
       <c r="F254" s="7"/>
     </row>
-    <row r="255" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B255" s="71" t="s">
         <v>549</v>
       </c>
@@ -7030,7 +7030,7 @@
       </c>
       <c r="F255" s="7"/>
     </row>
-    <row r="256" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B256" s="71" t="s">
         <v>555</v>
       </c>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="F256" s="7"/>
     </row>
-    <row r="257" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B257" s="71" t="s">
         <v>557</v>
       </c>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="F257" s="7"/>
     </row>
-    <row r="258" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B258" s="71" t="s">
         <v>547</v>
       </c>
@@ -7075,7 +7075,7 @@
       </c>
       <c r="F258" s="7"/>
     </row>
-    <row r="259" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B259" s="71" t="s">
         <v>551</v>
       </c>
@@ -7090,7 +7090,7 @@
       </c>
       <c r="F259" s="7"/>
     </row>
-    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B260" s="71" t="s">
         <v>553</v>
       </c>
@@ -7105,7 +7105,7 @@
       </c>
       <c r="F260" s="7"/>
     </row>
-    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B261" s="71" t="s">
         <v>559</v>
       </c>
@@ -7120,7 +7120,7 @@
       </c>
       <c r="F261" s="7"/>
     </row>
-    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B262" s="71" t="s">
         <v>561</v>
       </c>
@@ -7135,7 +7135,7 @@
       </c>
       <c r="F262" s="7"/>
     </row>
-    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B263" s="71" t="s">
         <v>563</v>
       </c>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="F263" s="7"/>
     </row>
-    <row r="264" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B264" s="71" t="s">
         <v>618</v>
       </c>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="F264" s="7"/>
     </row>
-    <row r="265" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B265" s="71" t="s">
         <v>619</v>
       </c>
@@ -7180,7 +7180,7 @@
       </c>
       <c r="F265" s="7"/>
     </row>
-    <row r="266" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B266" s="71" t="s">
         <v>620</v>
       </c>
@@ -7195,7 +7195,7 @@
       </c>
       <c r="F266" s="7"/>
     </row>
-    <row r="267" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B267" s="71" t="s">
         <v>621</v>
       </c>
@@ -7210,7 +7210,7 @@
       </c>
       <c r="F267" s="68"/>
     </row>
-    <row r="268" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B268" s="71" t="s">
         <v>622</v>
       </c>
@@ -7225,7 +7225,7 @@
       </c>
       <c r="F268" s="68"/>
     </row>
-    <row r="269" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B269" s="71" t="s">
         <v>623</v>
       </c>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="F269" s="68"/>
     </row>
-    <row r="270" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B270" s="71" t="s">
         <v>624</v>
       </c>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="F270" s="68"/>
     </row>
-    <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B271" s="71" t="s">
         <v>625</v>
       </c>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="F271" s="68"/>
     </row>
-    <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B272" s="71" t="s">
         <v>626</v>
       </c>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="F272" s="68"/>
     </row>
-    <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B273" s="71" t="s">
         <v>627</v>
       </c>
@@ -7300,7 +7300,7 @@
       </c>
       <c r="F273" s="68"/>
     </row>
-    <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B274" s="71" t="s">
         <v>628</v>
       </c>
@@ -7315,7 +7315,7 @@
       </c>
       <c r="F274" s="68"/>
     </row>
-    <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B275" s="71" t="s">
         <v>629</v>
       </c>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="F275" s="68"/>
     </row>
-    <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B276" s="71" t="s">
         <v>630</v>
       </c>
@@ -7345,7 +7345,7 @@
       </c>
       <c r="F276" s="68"/>
     </row>
-    <row r="277" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B277" s="71" t="s">
         <v>631</v>
       </c>
@@ -7360,7 +7360,7 @@
       </c>
       <c r="F277" s="68"/>
     </row>
-    <row r="278" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B278" s="71" t="s">
         <v>632</v>
       </c>
@@ -7375,7 +7375,7 @@
       </c>
       <c r="F278" s="68"/>
     </row>
-    <row r="279" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B279" s="71" t="s">
         <v>633</v>
       </c>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="F279" s="68"/>
     </row>
-    <row r="280" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B280" s="71" t="s">
         <v>650</v>
       </c>
@@ -7405,7 +7405,7 @@
       </c>
       <c r="F280" s="68"/>
     </row>
-    <row r="281" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B281" s="71" t="s">
         <v>652</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="F281" s="68"/>
     </row>
-    <row r="282" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B282" s="71" t="s">
         <v>658</v>
       </c>
@@ -7435,7 +7435,7 @@
       </c>
       <c r="F282" s="68"/>
     </row>
-    <row r="283" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B283" s="71" t="s">
         <v>657</v>
       </c>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="F283" s="68"/>
     </row>
-    <row r="284" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B284" s="71" t="s">
         <v>654</v>
       </c>
@@ -7465,7 +7465,7 @@
       </c>
       <c r="F284" s="68"/>
     </row>
-    <row r="285" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B285" s="71" t="s">
         <v>655</v>
       </c>
@@ -7480,7 +7480,7 @@
       </c>
       <c r="F285" s="68"/>
     </row>
-    <row r="286" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B286" s="71" t="s">
         <v>660</v>
       </c>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="F286" s="68"/>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B287" s="68" t="s">
         <v>664</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
       <c r="F287" s="68"/>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B288" s="68" t="s">
         <v>666</v>
       </c>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="F288" s="68"/>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B289" s="68" t="s">
         <v>668</v>
       </c>
@@ -7540,7 +7540,7 @@
       </c>
       <c r="F289" s="68"/>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B290" s="68" t="s">
         <v>670</v>
       </c>
@@ -7555,7 +7555,7 @@
       </c>
       <c r="F290" s="68"/>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B291" s="68" t="s">
         <v>672</v>
       </c>
@@ -7570,7 +7570,7 @@
       </c>
       <c r="F291" s="68"/>
     </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B292" s="68" t="s">
         <v>674</v>
       </c>
@@ -7585,7 +7585,7 @@
       </c>
       <c r="F292" s="68"/>
     </row>
-    <row r="293" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B293" s="68" t="s">
         <v>676</v>
       </c>
@@ -7600,7 +7600,7 @@
       </c>
       <c r="F293" s="68"/>
     </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B294" s="68" t="s">
         <v>678</v>
       </c>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="F294" s="68"/>
     </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B295" s="68" t="s">
         <v>680</v>
       </c>
@@ -7630,7 +7630,7 @@
       </c>
       <c r="F295" s="68"/>
     </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B296" s="68" t="s">
         <v>682</v>
       </c>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="F296" s="68"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B297" s="68" t="s">
         <v>684</v>
       </c>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="F297" s="68"/>
     </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B298" s="68" t="s">
         <v>686</v>
       </c>
@@ -7675,7 +7675,7 @@
       </c>
       <c r="F298" s="68"/>
     </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B299" s="68" t="s">
         <v>688</v>
       </c>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="F299" s="68"/>
     </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B300" s="68" t="s">
         <v>690</v>
       </c>
@@ -7705,7 +7705,7 @@
       </c>
       <c r="F300" s="68"/>
     </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B301" s="68" t="s">
         <v>692</v>
       </c>
@@ -7720,7 +7720,7 @@
       </c>
       <c r="F301" s="68"/>
     </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B302" s="68" t="s">
         <v>694</v>
       </c>
@@ -7735,7 +7735,7 @@
       </c>
       <c r="F302" s="68"/>
     </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B303" s="68" t="s">
         <v>696</v>
       </c>
@@ -7750,7 +7750,7 @@
       </c>
       <c r="F303" s="68"/>
     </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B304" s="68" t="s">
         <v>698</v>
       </c>
@@ -7765,77 +7765,77 @@
       </c>
       <c r="F304" s="68"/>
     </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B305" s="68"/>
       <c r="C305" s="68"/>
       <c r="D305" s="68"/>
       <c r="E305" s="68"/>
       <c r="F305" s="68"/>
     </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B306" s="68"/>
       <c r="C306" s="68"/>
       <c r="D306" s="68"/>
       <c r="E306" s="68"/>
       <c r="F306" s="68"/>
     </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B307" s="68"/>
       <c r="C307" s="68"/>
       <c r="D307" s="68"/>
       <c r="E307" s="68"/>
       <c r="F307" s="68"/>
     </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B308" s="68"/>
       <c r="C308" s="68"/>
       <c r="D308" s="68"/>
       <c r="E308" s="68"/>
       <c r="F308" s="68"/>
     </row>
-    <row r="309" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B309" s="68"/>
       <c r="C309" s="68"/>
       <c r="D309" s="68"/>
       <c r="E309" s="68"/>
       <c r="F309" s="68"/>
     </row>
-    <row r="310" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B310" s="68"/>
       <c r="C310" s="68"/>
       <c r="D310" s="68"/>
       <c r="E310" s="68"/>
       <c r="F310" s="68"/>
     </row>
-    <row r="311" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B311" s="68"/>
       <c r="C311" s="68"/>
       <c r="D311" s="68"/>
       <c r="E311" s="68"/>
       <c r="F311" s="68"/>
     </row>
-    <row r="312" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B312" s="68"/>
       <c r="C312" s="68"/>
       <c r="D312" s="68"/>
       <c r="E312" s="68"/>
       <c r="F312" s="68"/>
     </row>
-    <row r="313" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B313" s="68"/>
       <c r="C313" s="68"/>
       <c r="D313" s="68"/>
       <c r="E313" s="68"/>
       <c r="F313" s="68"/>
     </row>
-    <row r="314" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B314" s="68"/>
       <c r="C314" s="68"/>
       <c r="D314" s="68"/>
       <c r="E314" s="68"/>
       <c r="F314" s="68"/>
     </row>
-    <row r="315" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B315" s="68"/>
       <c r="C315" s="68"/>
       <c r="D315" s="68"/>
@@ -7863,13 +7863,13 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B2" s="70" t="s">
         <v>541</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="73" t="s">
         <v>565</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="73" t="s">
         <v>567</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="73" t="s">
         <v>569</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="73" t="s">
         <v>571</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="73" t="s">
         <v>573</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="73" t="s">
         <v>575</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="73" t="s">
         <v>578</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="73" t="s">
         <v>580</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="73" t="s">
         <v>582</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="73" t="s">
         <v>584</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="73" t="s">
         <v>586</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="73" t="s">
         <v>588</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>590</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="73" t="s">
         <v>592</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="73" t="s">
         <v>594</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="73" t="s">
         <v>596</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="73" t="s">
         <v>598</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="73" t="s">
         <v>600</v>
       </c>
@@ -8021,7 +8021,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="73" t="s">
         <v>612</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="73" t="s">
         <v>614</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="69" t="s">
         <v>616</v>
       </c>
@@ -8045,7 +8045,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="69"/>
       <c r="C24" s="69"/>
     </row>
@@ -8055,20 +8055,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8293,14 +8293,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8313,6 +8305,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added requirements for features that were implemented but not documented, and tested and marked requirements as complete.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C3B39F-4004-0842-90F0-A2D993F384F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FDBA8A-9494-0841-B28E-44E90D42A5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER SPREADSHEET" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>tc={047D126E-D947-419E-ABB9-ADAD162C5DD2}</author>
   </authors>
   <commentList>
-    <comment ref="D209" authorId="0" shapeId="0" xr:uid="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
+    <comment ref="D213" authorId="0" shapeId="0" xr:uid="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="741">
   <si>
     <t>REQUIREMENT ID</t>
   </si>
@@ -2254,6 +2254,30 @@
   </si>
   <si>
     <t>The program shall prompt the user if saving the forces were successful.</t>
+  </si>
+  <si>
+    <t>SYS-METR-016</t>
+  </si>
+  <si>
+    <t>SYS-METR-017</t>
+  </si>
+  <si>
+    <t>SYS-METR-018</t>
+  </si>
+  <si>
+    <t>SYS-METR-019</t>
+  </si>
+  <si>
+    <t>The program shall allow the user to change the unit of measurement for wingarea, wingspan, and chord using a dropdown menu.</t>
+  </si>
+  <si>
+    <t>The program shall allow the user to change the unit of measurement for vtail area, and vtailspan using a dropdown menu.</t>
+  </si>
+  <si>
+    <t>The program shall allow the user to change the unit of measurement for htailarea and htailsapn using a dropdown menu.</t>
+  </si>
+  <si>
+    <t>The program shall allow the user to change the unit of measurement for ADRP, Eye point, and Visual RP using a dropdown menu.</t>
   </si>
 </sst>
 </file>
@@ -2745,79 +2769,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3274,7 +3226,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D209" dT="2025-10-22T19:44:42.55" personId="{0B44E5FE-6282-4086-A5CD-8A4B3BD81016}" id="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
+  <threadedComment ref="D213" dT="2025-10-22T19:44:42.55" personId="{0B44E5FE-6282-4086-A5CD-8A4B3BD81016}" id="{047D126E-D947-419E-ABB9-ADAD162C5DD2}">
     <text>Link to UI Elements(also in github)- https://mavsuta-my.sharepoint.com/:x:/g/personal/eeh6400_mavs_uta_edu/EdM1amBmGwpIlWEx4x01hZsB9_bqH9pYalj-9kd7PPfp2A</text>
   </threadedComment>
 </ThreadedComments>
@@ -3282,10 +3234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
-  <dimension ref="A2:F322"/>
+  <dimension ref="A2:F326"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="89" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5580,8 +5532,8 @@
       <c r="D148" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E148" s="27" t="s">
-        <v>15</v>
+      <c r="E148" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F148" s="67" t="s">
         <v>518</v>
@@ -5597,8 +5549,8 @@
       <c r="D149" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E149" s="27" t="s">
-        <v>15</v>
+      <c r="E149" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F149" s="67" t="s">
         <v>519</v>
@@ -5614,8 +5566,8 @@
       <c r="D150" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E150" s="27" t="s">
-        <v>15</v>
+      <c r="E150" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F150" s="67" t="s">
         <v>520</v>
@@ -5631,8 +5583,8 @@
       <c r="D151" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E151" s="27" t="s">
-        <v>15</v>
+      <c r="E151" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F151" s="67" t="s">
         <v>521</v>
@@ -5648,8 +5600,8 @@
       <c r="D152" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="E152" s="27" t="s">
-        <v>15</v>
+      <c r="E152" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F152" s="67" t="s">
         <v>522</v>
@@ -5665,8 +5617,8 @@
       <c r="D153" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E153" s="27" t="s">
-        <v>15</v>
+      <c r="E153" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F153" s="67" t="s">
         <v>523</v>
@@ -5682,8 +5634,8 @@
       <c r="D154" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E154" s="27" t="s">
-        <v>15</v>
+      <c r="E154" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F154" s="7"/>
     </row>
@@ -5697,8 +5649,8 @@
       <c r="D155" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E155" s="27" t="s">
-        <v>15</v>
+      <c r="E155" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F155" s="67" t="s">
         <v>524</v>
@@ -5714,8 +5666,8 @@
       <c r="D156" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="E156" s="27" t="s">
-        <v>15</v>
+      <c r="E156" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F156" s="67" t="s">
         <v>526</v>
@@ -5731,8 +5683,8 @@
       <c r="D157" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E157" s="29" t="s">
-        <v>15</v>
+      <c r="E157" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F157" s="67" t="s">
         <v>525</v>
@@ -5748,8 +5700,8 @@
       <c r="D158" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E158" s="29" t="s">
-        <v>15</v>
+      <c r="E158" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F158" s="7"/>
     </row>
@@ -5814,136 +5766,136 @@
       <c r="F162" s="7"/>
     </row>
     <row r="163" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="C163" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D163" s="24" t="s">
-        <v>322</v>
-      </c>
-      <c r="E163" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F163" s="67" t="s">
-        <v>120</v>
-      </c>
+      <c r="B163" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="C163" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>737</v>
+      </c>
+      <c r="E163" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F163" s="7"/>
     </row>
     <row r="164" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="20" t="s">
-        <v>323</v>
-      </c>
-      <c r="C164" s="22" t="s">
+      <c r="B164" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="C164" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D164" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="E164" s="29" t="s">
-        <v>15</v>
+        <v>738</v>
+      </c>
+      <c r="E164" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F164" s="7"/>
     </row>
     <row r="165" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="C165" s="22" t="s">
+      <c r="B165" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="C165" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D165" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="E165" s="29" t="s">
-        <v>15</v>
+        <v>739</v>
+      </c>
+      <c r="E165" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F165" s="7"/>
     </row>
     <row r="166" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="C166" s="22" t="s">
+      <c r="B166" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="C166" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D166" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="E166" s="29" t="s">
-        <v>15</v>
+        <v>740</v>
+      </c>
+      <c r="E166" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F166" s="7"/>
     </row>
     <row r="167" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B167" s="20" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C167" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D167" s="11" t="s">
-        <v>330</v>
-      </c>
-      <c r="E167" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F167" s="7"/>
+      <c r="D167" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="E167" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F167" s="67" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="168" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B168" s="20" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C168" s="22" t="s">
         <v>6</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="E168" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="E168" s="29" t="s">
         <v>15</v>
       </c>
       <c r="F168" s="7"/>
     </row>
     <row r="169" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B169" s="20" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C169" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D169" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="E169" s="30" t="s">
+      <c r="D169" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="E169" s="29" t="s">
         <v>15</v>
       </c>
       <c r="F169" s="7"/>
     </row>
     <row r="170" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B170" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="C170" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D170" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="E170" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="C170" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="E170" s="29" t="s">
         <v>15</v>
       </c>
       <c r="F170" s="7"/>
     </row>
     <row r="171" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B171" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="C171" s="18" t="s">
-        <v>23</v>
+        <v>329</v>
+      </c>
+      <c r="C171" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="D171" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E171" s="30" t="s">
         <v>15</v>
@@ -5952,13 +5904,13 @@
     </row>
     <row r="172" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B172" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="C172" s="18" t="s">
-        <v>23</v>
+        <v>331</v>
+      </c>
+      <c r="C172" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="D172" s="11" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E172" s="30" t="s">
         <v>15</v>
@@ -5967,382 +5919,382 @@
     </row>
     <row r="173" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B173" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="C173" s="45" t="s">
-        <v>249</v>
-      </c>
-      <c r="D173" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="E173" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F173" s="7" t="s">
-        <v>346</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="C173" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D173" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="E173" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F173" s="7"/>
     </row>
     <row r="174" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B174" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="C174" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D174" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="E174" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F174" s="7"/>
+    </row>
+    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B175" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C175" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="E175" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F175" s="7"/>
+    </row>
+    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="C176" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D176" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="E176" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F176" s="7"/>
+    </row>
+    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="C177" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="E177" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F177" s="7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B178" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="C174" s="45" t="s">
+      <c r="C178" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="D174" s="11" t="s">
+      <c r="D178" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="E174" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F174" s="7"/>
-    </row>
-    <row r="175" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C175" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D175" s="63" t="s">
-        <v>496</v>
-      </c>
-      <c r="E175" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F175" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="176" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="C176" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D176" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="E176" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F176" s="7"/>
-    </row>
-    <row r="177" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="C177" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D177" s="65" t="s">
-        <v>498</v>
-      </c>
-      <c r="E177" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F177" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="178" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="C178" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D178" s="64" t="s">
-        <v>499</v>
-      </c>
-      <c r="E178" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F178" s="7" t="s">
-        <v>354</v>
-      </c>
+      <c r="E178" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F178" s="7"/>
     </row>
     <row r="179" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B179" s="9" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C179" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D179" s="65" t="s">
-        <v>500</v>
+      <c r="D179" s="63" t="s">
+        <v>496</v>
       </c>
       <c r="E179" s="78" t="s">
         <v>489</v>
       </c>
-      <c r="F179" s="7"/>
+      <c r="F179" s="7" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="180" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B180" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="C180" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D180" s="65" t="s">
-        <v>501</v>
+        <v>347</v>
+      </c>
+      <c r="C180" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" s="64" t="s">
+        <v>497</v>
       </c>
       <c r="E180" s="78" t="s">
         <v>489</v>
       </c>
-      <c r="F180" s="7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="181" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F180" s="7"/>
+    </row>
+    <row r="181" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B181" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="C181" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D181" s="51" t="s">
-        <v>356</v>
+        <v>348</v>
+      </c>
+      <c r="C181" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" s="65" t="s">
+        <v>498</v>
       </c>
       <c r="E181" s="78" t="s">
         <v>489</v>
       </c>
       <c r="F181" s="7" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="182" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B182" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="C182" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D182" s="65" t="s">
-        <v>502</v>
-      </c>
-      <c r="E182" s="28" t="s">
-        <v>15</v>
+        <v>350</v>
+      </c>
+      <c r="C182" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" s="64" t="s">
+        <v>499</v>
+      </c>
+      <c r="E182" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F182" s="7" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="183" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B183" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="C183" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C183" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D183" s="65" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E183" s="78" t="s">
         <v>489</v>
       </c>
-      <c r="F183" s="7" t="s">
-        <v>364</v>
-      </c>
+      <c r="F183" s="7"/>
     </row>
     <row r="184" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B184" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C184" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D184" s="65" t="s">
+        <v>501</v>
+      </c>
+      <c r="E184" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F184" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C185" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D185" s="51" t="s">
+        <v>356</v>
+      </c>
+      <c r="E185" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F185" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="186" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C186" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D186" s="65" t="s">
+        <v>502</v>
+      </c>
+      <c r="E186" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" s="7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="C187" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="65" t="s">
+        <v>503</v>
+      </c>
+      <c r="E187" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F187" s="7" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="C184" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D184" s="65" t="s">
+      <c r="C188" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="E184" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F184" s="7"/>
-    </row>
-    <row r="185" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="9" t="s">
+      <c r="E188" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F188" s="7"/>
+    </row>
+    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B189" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="C185" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D185" s="65" t="s">
+      <c r="C189" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" s="65" t="s">
         <v>505</v>
       </c>
-      <c r="E185" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F185" s="7" t="s">
+      <c r="E189" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F189" s="7" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="186" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="9" t="s">
+    <row r="190" spans="2:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B190" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="C186" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D186" s="51" t="s">
+      <c r="C190" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D190" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="E186" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F186" s="7" t="s">
+      <c r="E190" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F190" s="7" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="187" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="C187" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D187" s="59" t="s">
-        <v>485</v>
-      </c>
-      <c r="E187" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F187" s="7" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="188" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="C188" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D188" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="E188" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="C189" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D189" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="E189" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F189" s="7"/>
-    </row>
-    <row r="190" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="C190" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D190" s="6" t="s">
-        <v>488</v>
-      </c>
-      <c r="E190" s="78" t="s">
-        <v>489</v>
-      </c>
-      <c r="F190" s="7"/>
     </row>
     <row r="191" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
-        <v>713</v>
-      </c>
-      <c r="C191" s="81" t="s">
-        <v>249</v>
-      </c>
-      <c r="D191" s="82" t="s">
-        <v>714</v>
-      </c>
-      <c r="E191" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F191" s="7"/>
+        <v>367</v>
+      </c>
+      <c r="C191" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D191" s="59" t="s">
+        <v>485</v>
+      </c>
+      <c r="E191" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="192" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C192" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="E192" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F192" s="7" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B193" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C193" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D193" s="6" t="s">
+        <v>487</v>
+      </c>
+      <c r="E193" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F193" s="7"/>
+    </row>
+    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B194" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="C194" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="E194" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="F194" s="7"/>
+    </row>
+    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B195" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C195" s="81" t="s">
+        <v>249</v>
+      </c>
+      <c r="D195" s="82" t="s">
+        <v>714</v>
+      </c>
+      <c r="E195" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F195" s="7"/>
+    </row>
+    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B196" s="10" t="s">
         <v>715</v>
       </c>
-      <c r="C192" s="81" t="s">
+      <c r="C196" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="D192" s="82" t="s">
+      <c r="D196" s="82" t="s">
         <v>716</v>
-      </c>
-      <c r="E192" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F192" s="7"/>
-    </row>
-    <row r="193" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="C193" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E193" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F193" s="7"/>
-    </row>
-    <row r="194" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="21" t="s">
-        <v>377</v>
-      </c>
-      <c r="C194" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D194" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="E194" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F194" s="7"/>
-    </row>
-    <row r="195" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="C195" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E195" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F195" s="7"/>
-    </row>
-    <row r="196" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="C196" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="E196" s="28" t="s">
         <v>15</v>
@@ -6351,13 +6303,13 @@
     </row>
     <row r="197" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B197" s="21" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C197" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="E197" s="28" t="s">
         <v>15</v>
@@ -6366,88 +6318,88 @@
     </row>
     <row r="198" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B198" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="C198" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="E198" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F198" s="7"/>
+    </row>
+    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B199" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C199" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E199" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F199" s="7"/>
+    </row>
+    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B200" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="C200" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E200" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F200" s="7"/>
+    </row>
+    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B201" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="C201" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E201" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F201" s="7"/>
+    </row>
+    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="C198" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D198" s="2" t="s">
+      <c r="C202" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D202" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="E198" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F198" s="7"/>
-    </row>
-    <row r="199" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="3" t="s">
+      <c r="E202" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" s="7"/>
+    </row>
+    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B203" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C199" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D199" s="2" t="s">
+      <c r="C203" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="E199" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F199" s="7"/>
-    </row>
-    <row r="200" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C200" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E200" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F200" s="7"/>
-    </row>
-    <row r="201" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C201" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="E201" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F201" s="7"/>
-    </row>
-    <row r="202" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C202" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E202" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F202" s="7"/>
-    </row>
-    <row r="203" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="21" t="s">
-        <v>395</v>
-      </c>
-      <c r="C203" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="E203" s="28" t="s">
         <v>15</v>
@@ -6456,13 +6408,13 @@
     </row>
     <row r="204" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B204" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C204" s="18" t="s">
-        <v>23</v>
+        <v>389</v>
+      </c>
+      <c r="C204" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E204" s="28" t="s">
         <v>15</v>
@@ -6471,45 +6423,43 @@
     </row>
     <row r="205" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C205" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C205" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="E205" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F205" s="7"/>
+    </row>
+    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B206" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C206" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D205" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E205" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F205" s="7"/>
-    </row>
-    <row r="206" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="C206" s="43" t="s">
-        <v>249</v>
-      </c>
       <c r="D206" s="2" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E206" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F206" s="67" t="s">
-        <v>133</v>
-      </c>
+      <c r="F206" s="7"/>
     </row>
     <row r="207" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C207" s="48" t="s">
-        <v>249</v>
+      <c r="B207" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C207" s="49" t="s">
+        <v>23</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="E207" s="28" t="s">
         <v>15</v>
@@ -6518,30 +6468,28 @@
     </row>
     <row r="208" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C208" s="19" t="s">
-        <v>6</v>
+        <v>397</v>
+      </c>
+      <c r="C208" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E208" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F208" s="67" t="s">
-        <v>197</v>
-      </c>
+      <c r="F208" s="7"/>
     </row>
     <row r="209" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C209" s="19" t="s">
-        <v>6</v>
+        <v>399</v>
+      </c>
+      <c r="C209" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="E209" s="28" t="s">
         <v>15</v>
@@ -6549,29 +6497,31 @@
       <c r="F209" s="7"/>
     </row>
     <row r="210" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C210" s="19" t="s">
-        <v>6</v>
+      <c r="B210" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="C210" s="43" t="s">
+        <v>249</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E210" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F210" s="7"/>
+      <c r="F210" s="67" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="211" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C211" s="19" t="s">
-        <v>6</v>
+        <v>403</v>
+      </c>
+      <c r="C211" s="48" t="s">
+        <v>249</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E211" s="28" t="s">
         <v>15</v>
@@ -6580,28 +6530,30 @@
     </row>
     <row r="212" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C212" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="E212" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F212" s="7"/>
+      <c r="F212" s="67" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="213" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C213" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="E213" s="28" t="s">
         <v>15</v>
@@ -6610,13 +6562,13 @@
     </row>
     <row r="214" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C214" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="E214" s="28" t="s">
         <v>15</v>
@@ -6625,13 +6577,13 @@
     </row>
     <row r="215" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C215" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E215" s="28" t="s">
         <v>15</v>
@@ -6640,13 +6592,13 @@
     </row>
     <row r="216" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B216" s="3" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="C216" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="E216" s="28" t="s">
         <v>15</v>
@@ -6655,13 +6607,13 @@
     </row>
     <row r="217" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C217" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="E217" s="28" t="s">
         <v>15</v>
@@ -6670,13 +6622,13 @@
     </row>
     <row r="218" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C218" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="E218" s="28" t="s">
         <v>15</v>
@@ -6685,13 +6637,13 @@
     </row>
     <row r="219" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B219" s="3" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="C219" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="E219" s="28" t="s">
         <v>15</v>
@@ -6700,195 +6652,193 @@
     </row>
     <row r="220" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="C220" s="19" t="s">
         <v>6</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E220" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="E220" s="28" t="s">
         <v>15</v>
       </c>
       <c r="F220" s="7"/>
     </row>
     <row r="221" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C221" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E221" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F221" s="7"/>
+    </row>
+    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B222" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C222" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E222" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F222" s="7"/>
+    </row>
+    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B223" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="C223" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E223" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F223" s="7"/>
+    </row>
+    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B224" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="C224" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E224" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F224" s="7"/>
+    </row>
+    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B225" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C221" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D221" s="2" t="s">
+      <c r="C225" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D225" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E221" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F221" s="7"/>
-    </row>
-    <row r="222" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="21" t="s">
+      <c r="E225" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F225" s="7"/>
+    </row>
+    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B226" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="C222" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D222" s="21" t="s">
+      <c r="C226" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D226" s="21" t="s">
         <v>434</v>
       </c>
-      <c r="E222" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F222" s="7"/>
-    </row>
-    <row r="223" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="21" t="s">
+      <c r="E226" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F226" s="7"/>
+    </row>
+    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B227" s="21" t="s">
         <v>435</v>
       </c>
-      <c r="C223" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D223" s="21" t="s">
+      <c r="C227" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D227" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="E223" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F223" s="7"/>
-    </row>
-    <row r="224" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="21" t="s">
+      <c r="E227" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F227" s="7"/>
+    </row>
+    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B228" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="C224" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D224" s="21" t="s">
+      <c r="C228" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D228" s="21" t="s">
         <v>438</v>
       </c>
-      <c r="E224" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F224" s="7"/>
-    </row>
-    <row r="225" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="12" t="s">
+      <c r="E228" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F228" s="7"/>
+    </row>
+    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B229" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="C225" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D225" s="12" t="s">
+      <c r="C229" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D229" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="E225" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F225" s="7"/>
-    </row>
-    <row r="226" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="12" t="s">
+      <c r="E229" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F229" s="7"/>
+    </row>
+    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B230" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="C226" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D226" s="12" t="s">
+      <c r="C230" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D230" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="E226" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F226" s="7"/>
-    </row>
-    <row r="227" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="12" t="s">
+      <c r="E230" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F230" s="7"/>
+    </row>
+    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B231" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="C227" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D227" s="12" t="s">
+      <c r="C231" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D231" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="E227" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F227" s="7"/>
-    </row>
-    <row r="228" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="12" t="s">
+      <c r="E231" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F231" s="7"/>
+    </row>
+    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B232" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="C228" s="32" t="s">
+      <c r="C232" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D232" s="12" t="s">
         <v>446</v>
-      </c>
-      <c r="E228" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F228" s="7"/>
-    </row>
-    <row r="229" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="21" t="s">
-        <v>447</v>
-      </c>
-      <c r="C229" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D229" s="21" t="s">
-        <v>448</v>
-      </c>
-      <c r="E229" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F229" s="67" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="230" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="21" t="s">
-        <v>449</v>
-      </c>
-      <c r="C230" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D230" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="E230" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F230" s="7"/>
-    </row>
-    <row r="231" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="C231" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D231" s="21" t="s">
-        <v>452</v>
-      </c>
-      <c r="E231" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F231" s="7"/>
-    </row>
-    <row r="232" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="C232" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D232" s="21" t="s">
-        <v>454</v>
       </c>
       <c r="E232" s="37" t="s">
         <v>15</v>
@@ -6897,28 +6847,30 @@
     </row>
     <row r="233" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B233" s="21" t="s">
-        <v>455</v>
-      </c>
-      <c r="C233" s="33" t="s">
-        <v>23</v>
+        <v>447</v>
+      </c>
+      <c r="C233" s="40" t="s">
+        <v>6</v>
       </c>
       <c r="D233" s="21" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="E233" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F233" s="7"/>
+      <c r="F233" s="67" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="234" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B234" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="C234" s="33" t="s">
-        <v>23</v>
+        <v>449</v>
+      </c>
+      <c r="C234" s="40" t="s">
+        <v>6</v>
       </c>
       <c r="D234" s="21" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E234" s="37" t="s">
         <v>15</v>
@@ -6927,13 +6879,13 @@
     </row>
     <row r="235" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B235" s="21" t="s">
-        <v>459</v>
-      </c>
-      <c r="C235" s="33" t="s">
-        <v>23</v>
+        <v>451</v>
+      </c>
+      <c r="C235" s="40" t="s">
+        <v>6</v>
       </c>
       <c r="D235" s="21" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="E235" s="37" t="s">
         <v>15</v>
@@ -6942,13 +6894,13 @@
     </row>
     <row r="236" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B236" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="C236" s="34" t="s">
-        <v>249</v>
+        <v>453</v>
+      </c>
+      <c r="C236" s="40" t="s">
+        <v>6</v>
       </c>
       <c r="D236" s="21" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E236" s="37" t="s">
         <v>15</v>
@@ -6957,73 +6909,73 @@
     </row>
     <row r="237" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B237" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="C237" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D237" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="E237" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F237" s="7"/>
+    </row>
+    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B238" s="21" t="s">
+        <v>457</v>
+      </c>
+      <c r="C238" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D238" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="E238" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F238" s="7"/>
+    </row>
+    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B239" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="C239" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D239" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="E239" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F239" s="7"/>
+    </row>
+    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B240" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="C240" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D240" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="E240" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F240" s="7"/>
+    </row>
+    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B241" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="C237" s="34" t="s">
+      <c r="C241" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="D237" s="21" t="s">
+      <c r="D241" s="21" t="s">
         <v>464</v>
-      </c>
-      <c r="E237" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F237" s="7"/>
-    </row>
-    <row r="238" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="C238" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D238" s="12" t="s">
-        <v>466</v>
-      </c>
-      <c r="E238" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F238" s="7"/>
-    </row>
-    <row r="239" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="C239" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D239" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="E239" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F239" s="7"/>
-    </row>
-    <row r="240" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B240" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="C240" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D240" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="E240" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F240" s="7"/>
-    </row>
-    <row r="241" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="12" t="s">
-        <v>471</v>
-      </c>
-      <c r="C241" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D241" s="12" t="s">
-        <v>472</v>
       </c>
       <c r="E241" s="37" t="s">
         <v>15</v>
@@ -7032,13 +6984,13 @@
     </row>
     <row r="242" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B242" s="12" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="C242" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D242" s="12" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="E242" s="37" t="s">
         <v>15</v>
@@ -7047,13 +6999,13 @@
     </row>
     <row r="243" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B243" s="12" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C243" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D243" s="12" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="E243" s="37" t="s">
         <v>15</v>
@@ -7062,13 +7014,13 @@
     </row>
     <row r="244" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B244" s="12" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="C244" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D244" s="12" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="E244" s="37" t="s">
         <v>15</v>
@@ -7077,13 +7029,13 @@
     </row>
     <row r="245" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B245" s="12" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C245" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="E245" s="37" t="s">
         <v>15</v>
@@ -7092,13 +7044,13 @@
     </row>
     <row r="246" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B246" s="12" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="C246" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="E246" s="37" t="s">
         <v>15</v>
@@ -7107,73 +7059,73 @@
     </row>
     <row r="247" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B247" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="C247" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D247" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="E247" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F247" s="7"/>
+    </row>
+    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B248" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="C248" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D248" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="E248" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F248" s="7"/>
+    </row>
+    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="C249" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D249" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="E249" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F249" s="7"/>
+    </row>
+    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="C250" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D250" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="E250" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F250" s="7"/>
+    </row>
+    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B251" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="C247" s="58" t="s">
+      <c r="C251" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D247" s="12" t="s">
+      <c r="D251" s="12" t="s">
         <v>484</v>
-      </c>
-      <c r="E247" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F247" s="7"/>
-    </row>
-    <row r="248" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="68" t="s">
-        <v>602</v>
-      </c>
-      <c r="C248" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D248" s="68" t="s">
-        <v>603</v>
-      </c>
-      <c r="E248" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F248" s="7"/>
-    </row>
-    <row r="249" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="68" t="s">
-        <v>604</v>
-      </c>
-      <c r="C249" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D249" s="68" t="s">
-        <v>605</v>
-      </c>
-      <c r="E249" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F249" s="7"/>
-    </row>
-    <row r="250" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="68" t="s">
-        <v>529</v>
-      </c>
-      <c r="C250" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D250" s="68" t="s">
-        <v>530</v>
-      </c>
-      <c r="E250" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F250" s="7"/>
-    </row>
-    <row r="251" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="68" t="s">
-        <v>531</v>
-      </c>
-      <c r="C251" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D251" s="68" t="s">
-        <v>532</v>
       </c>
       <c r="E251" s="37" t="s">
         <v>15</v>
@@ -7182,13 +7134,13 @@
     </row>
     <row r="252" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B252" s="68" t="s">
-        <v>533</v>
+        <v>602</v>
       </c>
       <c r="C252" s="50" t="s">
         <v>6</v>
       </c>
       <c r="D252" s="68" t="s">
-        <v>534</v>
+        <v>603</v>
       </c>
       <c r="E252" s="37" t="s">
         <v>15</v>
@@ -7197,13 +7149,13 @@
     </row>
     <row r="253" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B253" s="68" t="s">
-        <v>606</v>
-      </c>
-      <c r="C253" s="58" t="s">
-        <v>23</v>
+        <v>604</v>
+      </c>
+      <c r="C253" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D253" s="68" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E253" s="37" t="s">
         <v>15</v>
@@ -7212,13 +7164,13 @@
     </row>
     <row r="254" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B254" s="68" t="s">
-        <v>608</v>
-      </c>
-      <c r="C254" s="58" t="s">
-        <v>23</v>
+        <v>529</v>
+      </c>
+      <c r="C254" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D254" s="68" t="s">
-        <v>609</v>
+        <v>530</v>
       </c>
       <c r="E254" s="37" t="s">
         <v>15</v>
@@ -7227,13 +7179,13 @@
     </row>
     <row r="255" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B255" s="68" t="s">
-        <v>527</v>
-      </c>
-      <c r="C255" s="58" t="s">
-        <v>23</v>
+        <v>531</v>
+      </c>
+      <c r="C255" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D255" s="68" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="E255" s="37" t="s">
         <v>15</v>
@@ -7242,13 +7194,13 @@
     </row>
     <row r="256" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B256" s="68" t="s">
-        <v>535</v>
-      </c>
-      <c r="C256" s="58" t="s">
-        <v>23</v>
+        <v>533</v>
+      </c>
+      <c r="C256" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D256" s="68" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E256" s="37" t="s">
         <v>15</v>
@@ -7257,13 +7209,13 @@
     </row>
     <row r="257" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B257" s="68" t="s">
-        <v>610</v>
-      </c>
-      <c r="C257" s="32" t="s">
-        <v>249</v>
+        <v>606</v>
+      </c>
+      <c r="C257" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D257" s="68" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E257" s="37" t="s">
         <v>15</v>
@@ -7272,13 +7224,13 @@
     </row>
     <row r="258" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B258" s="68" t="s">
-        <v>537</v>
-      </c>
-      <c r="C258" s="32" t="s">
-        <v>249</v>
+        <v>608</v>
+      </c>
+      <c r="C258" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D258" s="68" t="s">
-        <v>538</v>
+        <v>609</v>
       </c>
       <c r="E258" s="37" t="s">
         <v>15</v>
@@ -7287,73 +7239,73 @@
     </row>
     <row r="259" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B259" s="68" t="s">
+        <v>527</v>
+      </c>
+      <c r="C259" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D259" s="68" t="s">
+        <v>528</v>
+      </c>
+      <c r="E259" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F259" s="7"/>
+    </row>
+    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B260" s="68" t="s">
+        <v>535</v>
+      </c>
+      <c r="C260" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D260" s="68" t="s">
+        <v>536</v>
+      </c>
+      <c r="E260" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F260" s="7"/>
+    </row>
+    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B261" s="68" t="s">
+        <v>610</v>
+      </c>
+      <c r="C261" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D261" s="68" t="s">
+        <v>611</v>
+      </c>
+      <c r="E261" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F261" s="7"/>
+    </row>
+    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B262" s="68" t="s">
+        <v>537</v>
+      </c>
+      <c r="C262" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D262" s="68" t="s">
+        <v>538</v>
+      </c>
+      <c r="E262" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F262" s="7"/>
+    </row>
+    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B263" s="68" t="s">
         <v>539</v>
       </c>
-      <c r="C259" s="32" t="s">
+      <c r="C263" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="D259" s="68" t="s">
+      <c r="D263" s="68" t="s">
         <v>540</v>
-      </c>
-      <c r="E259" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F259" s="7"/>
-    </row>
-    <row r="260" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="71" t="s">
-        <v>543</v>
-      </c>
-      <c r="C260" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D260" s="71" t="s">
-        <v>544</v>
-      </c>
-      <c r="E260" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F260" s="7"/>
-    </row>
-    <row r="261" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="71" t="s">
-        <v>545</v>
-      </c>
-      <c r="C261" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D261" s="72" t="s">
-        <v>546</v>
-      </c>
-      <c r="E261" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F261" s="7"/>
-    </row>
-    <row r="262" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="71" t="s">
-        <v>549</v>
-      </c>
-      <c r="C262" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D262" s="72" t="s">
-        <v>550</v>
-      </c>
-      <c r="E262" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F262" s="7"/>
-    </row>
-    <row r="263" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="71" t="s">
-        <v>555</v>
-      </c>
-      <c r="C263" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="D263" s="72" t="s">
-        <v>556</v>
       </c>
       <c r="E263" s="37" t="s">
         <v>15</v>
@@ -7362,13 +7314,13 @@
     </row>
     <row r="264" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B264" s="71" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="C264" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D264" s="72" t="s">
-        <v>558</v>
+      <c r="D264" s="71" t="s">
+        <v>544</v>
       </c>
       <c r="E264" s="37" t="s">
         <v>15</v>
@@ -7377,13 +7329,13 @@
     </row>
     <row r="265" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B265" s="71" t="s">
-        <v>547</v>
-      </c>
-      <c r="C265" s="58" t="s">
-        <v>23</v>
+        <v>545</v>
+      </c>
+      <c r="C265" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D265" s="72" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E265" s="37" t="s">
         <v>15</v>
@@ -7392,13 +7344,13 @@
     </row>
     <row r="266" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B266" s="71" t="s">
-        <v>551</v>
-      </c>
-      <c r="C266" s="58" t="s">
-        <v>23</v>
+        <v>549</v>
+      </c>
+      <c r="C266" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D266" s="72" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E266" s="37" t="s">
         <v>15</v>
@@ -7407,13 +7359,13 @@
     </row>
     <row r="267" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B267" s="71" t="s">
-        <v>553</v>
-      </c>
-      <c r="C267" s="58" t="s">
-        <v>23</v>
+        <v>555</v>
+      </c>
+      <c r="C267" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D267" s="72" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="E267" s="37" t="s">
         <v>15</v>
@@ -7422,13 +7374,13 @@
     </row>
     <row r="268" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B268" s="71" t="s">
-        <v>559</v>
-      </c>
-      <c r="C268" s="58" t="s">
-        <v>23</v>
+        <v>557</v>
+      </c>
+      <c r="C268" s="50" t="s">
+        <v>6</v>
       </c>
       <c r="D268" s="72" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E268" s="37" t="s">
         <v>15</v>
@@ -7437,13 +7389,13 @@
     </row>
     <row r="269" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B269" s="71" t="s">
-        <v>561</v>
-      </c>
-      <c r="C269" s="32" t="s">
-        <v>249</v>
+        <v>547</v>
+      </c>
+      <c r="C269" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D269" s="72" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="E269" s="37" t="s">
         <v>15</v>
@@ -7452,13 +7404,13 @@
     </row>
     <row r="270" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B270" s="71" t="s">
-        <v>563</v>
-      </c>
-      <c r="C270" s="32" t="s">
-        <v>249</v>
+        <v>551</v>
+      </c>
+      <c r="C270" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D270" s="72" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="E270" s="37" t="s">
         <v>15</v>
@@ -7467,13 +7419,13 @@
     </row>
     <row r="271" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B271" s="71" t="s">
-        <v>618</v>
-      </c>
-      <c r="C271" s="50" t="s">
-        <v>6</v>
+        <v>553</v>
+      </c>
+      <c r="C271" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D271" s="72" t="s">
-        <v>634</v>
+        <v>554</v>
       </c>
       <c r="E271" s="37" t="s">
         <v>15</v>
@@ -7482,13 +7434,13 @@
     </row>
     <row r="272" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B272" s="71" t="s">
-        <v>619</v>
-      </c>
-      <c r="C272" s="50" t="s">
-        <v>6</v>
+        <v>559</v>
+      </c>
+      <c r="C272" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D272" s="72" t="s">
-        <v>641</v>
+        <v>560</v>
       </c>
       <c r="E272" s="37" t="s">
         <v>15</v>
@@ -7497,13 +7449,13 @@
     </row>
     <row r="273" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B273" s="71" t="s">
-        <v>620</v>
-      </c>
-      <c r="C273" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="D273" s="68" t="s">
-        <v>635</v>
+        <v>561</v>
+      </c>
+      <c r="C273" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D273" s="72" t="s">
+        <v>562</v>
       </c>
       <c r="E273" s="37" t="s">
         <v>15</v>
@@ -7512,73 +7464,73 @@
     </row>
     <row r="274" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B274" s="71" t="s">
-        <v>621</v>
-      </c>
-      <c r="C274" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="D274" s="68" t="s">
-        <v>649</v>
+        <v>563</v>
+      </c>
+      <c r="C274" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D274" s="72" t="s">
+        <v>564</v>
       </c>
       <c r="E274" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F274" s="68"/>
+      <c r="F274" s="7"/>
     </row>
     <row r="275" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B275" s="71" t="s">
-        <v>622</v>
-      </c>
-      <c r="C275" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D275" s="68" t="s">
-        <v>636</v>
+        <v>618</v>
+      </c>
+      <c r="C275" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D275" s="72" t="s">
+        <v>634</v>
       </c>
       <c r="E275" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F275" s="68"/>
+      <c r="F275" s="7"/>
     </row>
     <row r="276" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B276" s="71" t="s">
-        <v>623</v>
-      </c>
-      <c r="C276" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D276" s="68" t="s">
-        <v>648</v>
+        <v>619</v>
+      </c>
+      <c r="C276" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D276" s="72" t="s">
+        <v>641</v>
       </c>
       <c r="E276" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F276" s="68"/>
+      <c r="F276" s="7"/>
     </row>
     <row r="277" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B277" s="71" t="s">
-        <v>624</v>
-      </c>
-      <c r="C277" s="75" t="s">
-        <v>6</v>
+        <v>620</v>
+      </c>
+      <c r="C277" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="D277" s="68" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E277" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F277" s="68"/>
+      <c r="F277" s="7"/>
     </row>
     <row r="278" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B278" s="71" t="s">
-        <v>625</v>
-      </c>
-      <c r="C278" s="75" t="s">
-        <v>6</v>
+        <v>621</v>
+      </c>
+      <c r="C278" s="74" t="s">
+        <v>23</v>
       </c>
       <c r="D278" s="68" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="E278" s="37" t="s">
         <v>15</v>
@@ -7587,13 +7539,13 @@
     </row>
     <row r="279" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B279" s="71" t="s">
-        <v>626</v>
-      </c>
-      <c r="C279" s="74" t="s">
-        <v>23</v>
+        <v>622</v>
+      </c>
+      <c r="C279" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D279" s="68" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E279" s="37" t="s">
         <v>15</v>
@@ -7602,13 +7554,13 @@
     </row>
     <row r="280" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B280" s="71" t="s">
-        <v>627</v>
-      </c>
-      <c r="C280" s="74" t="s">
-        <v>23</v>
+        <v>623</v>
+      </c>
+      <c r="C280" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D280" s="68" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="E280" s="37" t="s">
         <v>15</v>
@@ -7617,13 +7569,13 @@
     </row>
     <row r="281" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B281" s="71" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C281" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D281" s="68" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E281" s="37" t="s">
         <v>15</v>
@@ -7632,13 +7584,13 @@
     </row>
     <row r="282" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B282" s="71" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="C282" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D282" s="68" t="s">
-        <v>640</v>
+        <v>647</v>
       </c>
       <c r="E282" s="37" t="s">
         <v>15</v>
@@ -7647,13 +7599,13 @@
     </row>
     <row r="283" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B283" s="71" t="s">
-        <v>630</v>
-      </c>
-      <c r="C283" s="75" t="s">
-        <v>6</v>
+        <v>626</v>
+      </c>
+      <c r="C283" s="74" t="s">
+        <v>23</v>
       </c>
       <c r="D283" s="68" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="E283" s="37" t="s">
         <v>15</v>
@@ -7662,13 +7614,13 @@
     </row>
     <row r="284" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B284" s="71" t="s">
-        <v>631</v>
-      </c>
-      <c r="C284" s="75" t="s">
-        <v>6</v>
+        <v>627</v>
+      </c>
+      <c r="C284" s="74" t="s">
+        <v>23</v>
       </c>
       <c r="D284" s="68" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="E284" s="37" t="s">
         <v>15</v>
@@ -7677,13 +7629,13 @@
     </row>
     <row r="285" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B285" s="71" t="s">
-        <v>632</v>
-      </c>
-      <c r="C285" s="74" t="s">
-        <v>23</v>
+        <v>628</v>
+      </c>
+      <c r="C285" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D285" s="68" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="E285" s="37" t="s">
         <v>15</v>
@@ -7692,13 +7644,13 @@
     </row>
     <row r="286" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B286" s="71" t="s">
-        <v>633</v>
-      </c>
-      <c r="C286" s="74" t="s">
-        <v>23</v>
+        <v>629</v>
+      </c>
+      <c r="C286" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D286" s="68" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E286" s="37" t="s">
         <v>15</v>
@@ -7707,13 +7659,13 @@
     </row>
     <row r="287" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B287" s="71" t="s">
-        <v>650</v>
+        <v>630</v>
       </c>
       <c r="C287" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D287" s="68" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="E287" s="37" t="s">
         <v>15</v>
@@ -7722,13 +7674,13 @@
     </row>
     <row r="288" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B288" s="71" t="s">
-        <v>652</v>
-      </c>
-      <c r="C288" s="74" t="s">
-        <v>23</v>
+        <v>631</v>
+      </c>
+      <c r="C288" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D288" s="68" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="E288" s="37" t="s">
         <v>15</v>
@@ -7737,13 +7689,13 @@
     </row>
     <row r="289" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B289" s="71" t="s">
-        <v>658</v>
-      </c>
-      <c r="C289" s="75" t="s">
-        <v>6</v>
+        <v>632</v>
+      </c>
+      <c r="C289" s="74" t="s">
+        <v>23</v>
       </c>
       <c r="D289" s="68" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
       <c r="E289" s="37" t="s">
         <v>15</v>
@@ -7752,13 +7704,13 @@
     </row>
     <row r="290" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B290" s="71" t="s">
-        <v>657</v>
-      </c>
-      <c r="C290" s="75" t="s">
-        <v>6</v>
+        <v>633</v>
+      </c>
+      <c r="C290" s="74" t="s">
+        <v>23</v>
       </c>
       <c r="D290" s="68" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="E290" s="37" t="s">
         <v>15</v>
@@ -7767,13 +7719,13 @@
     </row>
     <row r="291" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B291" s="71" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C291" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D291" s="68" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="E291" s="37" t="s">
         <v>15</v>
@@ -7782,88 +7734,88 @@
     </row>
     <row r="292" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B292" s="71" t="s">
+        <v>652</v>
+      </c>
+      <c r="C292" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D292" s="68" t="s">
+        <v>653</v>
+      </c>
+      <c r="E292" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F292" s="68"/>
+    </row>
+    <row r="293" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B293" s="71" t="s">
+        <v>658</v>
+      </c>
+      <c r="C293" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D293" s="68" t="s">
+        <v>656</v>
+      </c>
+      <c r="E293" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F293" s="68"/>
+    </row>
+    <row r="294" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B294" s="71" t="s">
+        <v>657</v>
+      </c>
+      <c r="C294" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D294" s="68" t="s">
+        <v>659</v>
+      </c>
+      <c r="E294" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F294" s="68"/>
+    </row>
+    <row r="295" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B295" s="71" t="s">
+        <v>654</v>
+      </c>
+      <c r="C295" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D295" s="68" t="s">
+        <v>661</v>
+      </c>
+      <c r="E295" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F295" s="68"/>
+    </row>
+    <row r="296" spans="2:6" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B296" s="71" t="s">
         <v>655</v>
-      </c>
-      <c r="C292" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="D292" s="68" t="s">
-        <v>662</v>
-      </c>
-      <c r="E292" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F292" s="68"/>
-    </row>
-    <row r="293" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B293" s="71" t="s">
-        <v>660</v>
-      </c>
-      <c r="C293" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D293" s="68" t="s">
-        <v>663</v>
-      </c>
-      <c r="E293" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F293" s="68"/>
-    </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B294" s="68" t="s">
-        <v>664</v>
-      </c>
-      <c r="C294" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D294" s="68" t="s">
-        <v>665</v>
-      </c>
-      <c r="E294" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F294" s="68"/>
-    </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B295" s="68" t="s">
-        <v>666</v>
-      </c>
-      <c r="C295" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D295" s="68" t="s">
-        <v>667</v>
-      </c>
-      <c r="E295" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F295" s="68"/>
-    </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B296" s="68" t="s">
-        <v>668</v>
       </c>
       <c r="C296" s="32" t="s">
         <v>249</v>
       </c>
       <c r="D296" s="68" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="E296" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F296" s="68"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B297" s="68" t="s">
-        <v>670</v>
+    <row r="297" spans="2:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B297" s="71" t="s">
+        <v>660</v>
       </c>
       <c r="C297" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D297" s="68" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="E297" s="37" t="s">
         <v>15</v>
@@ -7872,13 +7824,13 @@
     </row>
     <row r="298" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B298" s="68" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="C298" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D298" s="68" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="E298" s="37" t="s">
         <v>15</v>
@@ -7887,13 +7839,13 @@
     </row>
     <row r="299" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B299" s="68" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="C299" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D299" s="68" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="E299" s="37" t="s">
         <v>15</v>
@@ -7902,13 +7854,13 @@
     </row>
     <row r="300" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B300" s="68" t="s">
-        <v>676</v>
-      </c>
-      <c r="C300" s="75" t="s">
-        <v>6</v>
+        <v>668</v>
+      </c>
+      <c r="C300" s="32" t="s">
+        <v>249</v>
       </c>
       <c r="D300" s="68" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="E300" s="37" t="s">
         <v>15</v>
@@ -7917,13 +7869,13 @@
     </row>
     <row r="301" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B301" s="68" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="C301" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D301" s="68" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E301" s="37" t="s">
         <v>15</v>
@@ -7932,13 +7884,13 @@
     </row>
     <row r="302" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B302" s="68" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="C302" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D302" s="68" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="E302" s="37" t="s">
         <v>15</v>
@@ -7947,13 +7899,13 @@
     </row>
     <row r="303" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B303" s="68" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="C303" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D303" s="68" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="E303" s="37" t="s">
         <v>15</v>
@@ -7962,13 +7914,13 @@
     </row>
     <row r="304" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B304" s="68" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="C304" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D304" s="68" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="E304" s="37" t="s">
         <v>15</v>
@@ -7977,13 +7929,13 @@
     </row>
     <row r="305" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B305" s="68" t="s">
-        <v>686</v>
-      </c>
-      <c r="C305" s="32" t="s">
-        <v>249</v>
+        <v>678</v>
+      </c>
+      <c r="C305" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D305" s="68" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="E305" s="37" t="s">
         <v>15</v>
@@ -7992,13 +7944,13 @@
     </row>
     <row r="306" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B306" s="68" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C306" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D306" s="68" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="E306" s="37" t="s">
         <v>15</v>
@@ -8007,13 +7959,13 @@
     </row>
     <row r="307" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B307" s="68" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="C307" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D307" s="68" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="E307" s="37" t="s">
         <v>15</v>
@@ -8022,13 +7974,13 @@
     </row>
     <row r="308" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B308" s="68" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="C308" s="75" t="s">
         <v>6</v>
       </c>
       <c r="D308" s="68" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="E308" s="37" t="s">
         <v>15</v>
@@ -8037,13 +7989,13 @@
     </row>
     <row r="309" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B309" s="68" t="s">
-        <v>694</v>
-      </c>
-      <c r="C309" s="75" t="s">
-        <v>6</v>
+        <v>686</v>
+      </c>
+      <c r="C309" s="32" t="s">
+        <v>249</v>
       </c>
       <c r="D309" s="68" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="E309" s="37" t="s">
         <v>15</v>
@@ -8052,13 +8004,13 @@
     </row>
     <row r="310" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B310" s="68" t="s">
-        <v>696</v>
-      </c>
-      <c r="C310" s="74" t="s">
-        <v>23</v>
+        <v>688</v>
+      </c>
+      <c r="C310" s="75" t="s">
+        <v>6</v>
       </c>
       <c r="D310" s="68" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="E310" s="37" t="s">
         <v>15</v>
@@ -8067,45 +8019,77 @@
     </row>
     <row r="311" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B311" s="68" t="s">
+        <v>690</v>
+      </c>
+      <c r="C311" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D311" s="68" t="s">
+        <v>691</v>
+      </c>
+      <c r="E311" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F311" s="68"/>
+    </row>
+    <row r="312" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B312" s="68" t="s">
+        <v>692</v>
+      </c>
+      <c r="C312" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D312" s="68" t="s">
+        <v>693</v>
+      </c>
+      <c r="E312" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F312" s="68"/>
+    </row>
+    <row r="313" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B313" s="68" t="s">
+        <v>694</v>
+      </c>
+      <c r="C313" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D313" s="68" t="s">
+        <v>695</v>
+      </c>
+      <c r="E313" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F313" s="68"/>
+    </row>
+    <row r="314" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B314" s="68" t="s">
+        <v>696</v>
+      </c>
+      <c r="C314" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D314" s="68" t="s">
+        <v>697</v>
+      </c>
+      <c r="E314" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F314" s="68"/>
+    </row>
+    <row r="315" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B315" s="68" t="s">
         <v>698</v>
       </c>
-      <c r="C311" s="75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D311" s="68" t="s">
+      <c r="C315" s="75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D315" s="68" t="s">
         <v>699</v>
       </c>
-      <c r="E311" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F311" s="68"/>
-    </row>
-    <row r="312" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B312" s="68"/>
-      <c r="C312" s="68"/>
-      <c r="D312" s="68"/>
-      <c r="E312" s="68"/>
-      <c r="F312" s="68"/>
-    </row>
-    <row r="313" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B313" s="68"/>
-      <c r="C313" s="68"/>
-      <c r="D313" s="68"/>
-      <c r="E313" s="68"/>
-      <c r="F313" s="68"/>
-    </row>
-    <row r="314" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B314" s="68"/>
-      <c r="C314" s="68"/>
-      <c r="D314" s="68"/>
-      <c r="E314" s="68"/>
-      <c r="F314" s="68"/>
-    </row>
-    <row r="315" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B315" s="68"/>
-      <c r="C315" s="68"/>
-      <c r="D315" s="68"/>
-      <c r="E315" s="68"/>
+      <c r="E315" s="37" t="s">
+        <v>15</v>
+      </c>
       <c r="F315" s="68"/>
     </row>
     <row r="316" spans="2:6" x14ac:dyDescent="0.2">
@@ -8157,12 +8141,40 @@
       <c r="E322" s="68"/>
       <c r="F322" s="68"/>
     </row>
+    <row r="323" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B323" s="68"/>
+      <c r="C323" s="68"/>
+      <c r="D323" s="68"/>
+      <c r="E323" s="68"/>
+      <c r="F323" s="68"/>
+    </row>
+    <row r="324" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B324" s="68"/>
+      <c r="C324" s="68"/>
+      <c r="D324" s="68"/>
+      <c r="E324" s="68"/>
+      <c r="F324" s="68"/>
+    </row>
+    <row r="325" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B325" s="68"/>
+      <c r="C325" s="68"/>
+      <c r="D325" s="68"/>
+      <c r="E325" s="68"/>
+      <c r="F325" s="68"/>
+    </row>
+    <row r="326" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B326" s="68"/>
+      <c r="C326" s="68"/>
+      <c r="D326" s="68"/>
+      <c r="E326" s="68"/>
+      <c r="F326" s="68"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F235">
-    <sortCondition ref="B3:B235"/>
-    <sortCondition sortBy="cellColor" ref="C3:C235" dxfId="23"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C235" dxfId="22"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C235" dxfId="21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F239">
+    <sortCondition ref="B3:B239"/>
+    <sortCondition sortBy="cellColor" ref="C3:C239" dxfId="14"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="13"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="12"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8370,6 +8382,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8590,24 +8619,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8624,29 +8661,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tested and marked requirements for DRAG DUE TO: Leading Edge Flap Deflection, Tailing Flap Deflection, Gear, and Speedbrake.
</commit_message>
<xml_diff>
--- a/requirements_specification/REQUIREMENTS.xlsx
+++ b/requirements_specification/REQUIREMENTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erick/Desktop/CSE/CSE-3310/jsbsimedit2/requirements_specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FDBA8A-9494-0841-B28E-44E90D42A5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2CA84D-26BE-DC48-A70C-1ED2E1D98A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{C4EEF77F-D77D-4E6B-9894-738B3E7F657E}"/>
   </bookViews>
@@ -2769,103 +2769,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3236,8 +3140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17077184-61CF-42C1-AD37-F8C4CB1F8259}">
   <dimension ref="A2:F326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="89" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" topLeftCell="D100" zoomScale="89" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5018,8 +4922,8 @@
       <c r="D116" s="24" t="s">
         <v>238</v>
       </c>
-      <c r="E116" s="36" t="s">
-        <v>15</v>
+      <c r="E116" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F116" s="7"/>
     </row>
@@ -5033,8 +4937,8 @@
       <c r="D117" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="E117" s="36" t="s">
-        <v>15</v>
+      <c r="E117" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F117" s="7"/>
     </row>
@@ -5048,8 +4952,8 @@
       <c r="D118" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="E118" s="36" t="s">
-        <v>15</v>
+      <c r="E118" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F118" s="7"/>
     </row>
@@ -5063,8 +4967,8 @@
       <c r="D119" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="E119" s="36" t="s">
-        <v>15</v>
+      <c r="E119" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F119" s="67" t="s">
         <v>159</v>
@@ -5080,8 +4984,8 @@
       <c r="D120" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="E120" s="36" t="s">
-        <v>15</v>
+      <c r="E120" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F120" s="7"/>
     </row>
@@ -5095,8 +4999,8 @@
       <c r="D121" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="E121" s="36" t="s">
-        <v>15</v>
+      <c r="E121" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F121" s="7"/>
     </row>
@@ -5110,8 +5014,8 @@
       <c r="D122" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="E122" s="36" t="s">
-        <v>15</v>
+      <c r="E122" s="77" t="s">
+        <v>489</v>
       </c>
       <c r="F122" s="7"/>
     </row>
@@ -6795,8 +6699,8 @@
       <c r="D229" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="E229" s="31" t="s">
-        <v>15</v>
+      <c r="E229" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F229" s="7"/>
     </row>
@@ -6810,8 +6714,8 @@
       <c r="D230" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="E230" s="31" t="s">
-        <v>15</v>
+      <c r="E230" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F230" s="7"/>
     </row>
@@ -6825,8 +6729,8 @@
       <c r="D231" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="E231" s="37" t="s">
-        <v>15</v>
+      <c r="E231" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F231" s="7"/>
     </row>
@@ -6840,8 +6744,8 @@
       <c r="D232" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="E232" s="37" t="s">
-        <v>15</v>
+      <c r="E232" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F232" s="7"/>
     </row>
@@ -6992,8 +6896,8 @@
       <c r="D242" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="E242" s="37" t="s">
-        <v>15</v>
+      <c r="E242" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F242" s="7"/>
     </row>
@@ -7007,8 +6911,8 @@
       <c r="D243" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="E243" s="37" t="s">
-        <v>15</v>
+      <c r="E243" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F243" s="7"/>
     </row>
@@ -7022,8 +6926,8 @@
       <c r="D244" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="E244" s="37" t="s">
-        <v>15</v>
+      <c r="E244" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F244" s="7"/>
     </row>
@@ -7037,8 +6941,8 @@
       <c r="D245" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="E245" s="37" t="s">
-        <v>15</v>
+      <c r="E245" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F245" s="7"/>
     </row>
@@ -7052,8 +6956,8 @@
       <c r="D246" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="E246" s="37" t="s">
-        <v>15</v>
+      <c r="E246" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F246" s="7"/>
     </row>
@@ -7067,8 +6971,8 @@
       <c r="D247" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="E247" s="37" t="s">
-        <v>15</v>
+      <c r="E247" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F247" s="7"/>
     </row>
@@ -7082,8 +6986,8 @@
       <c r="D248" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="E248" s="37" t="s">
-        <v>15</v>
+      <c r="E248" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F248" s="7"/>
     </row>
@@ -7097,8 +7001,8 @@
       <c r="D249" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="E249" s="37" t="s">
-        <v>15</v>
+      <c r="E249" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F249" s="7"/>
     </row>
@@ -7112,8 +7016,8 @@
       <c r="D250" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="E250" s="37" t="s">
-        <v>15</v>
+      <c r="E250" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F250" s="7"/>
     </row>
@@ -7127,8 +7031,8 @@
       <c r="D251" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E251" s="37" t="s">
-        <v>15</v>
+      <c r="E251" s="78" t="s">
+        <v>489</v>
       </c>
       <c r="F251" s="7"/>
     </row>
@@ -8172,9 +8076,9 @@
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F239">
     <sortCondition ref="B3:B239"/>
-    <sortCondition sortBy="cellColor" ref="C3:C239" dxfId="14"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="13"/>
-    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="12"/>
+    <sortCondition sortBy="cellColor" ref="C3:C239" dxfId="2"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="1"/>
+    <sortCondition descending="1" sortBy="cellColor" ref="C3:C239" dxfId="0"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8382,23 +8286,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B44B9D06410159488B070AC95D68600B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4f40a8ae5d04e781478941758898e75d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xmlns:ns4="b68e5611-82e7-4645-a9b5-4ea828ece9c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d7fa2983aaf7347aa340ea82c2c92eb" ns3:_="" ns4:_="">
     <xsd:import namespace="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
@@ -8619,32 +8506,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f0a658d2-ea9e-4264-95d4-b0ac9b274854" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E6DE447-2651-45BF-9B7B-A5A4748C527F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8661,4 +8540,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46CD9821-123E-468F-9B5B-EC6819DF6DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23527B3-E61F-4045-A715-817FD8CFD8BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f0a658d2-ea9e-4264-95d4-b0ac9b274854"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b68e5611-82e7-4645-a9b5-4ea828ece9c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>